<commit_message>
Refractorisation de la doc, choix technologiques et frameworks front-end
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D24519-3FBE-4944-9E69-8838721776D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FA64EF-04E1-8C4F-8AD2-A9C9B25E3080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
   <si>
     <t>Tâche</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Mise en place du repo Github</t>
+  </si>
+  <si>
+    <t>Environnements d’exécutions</t>
   </si>
 </sst>
 </file>
@@ -445,7 +448,97 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1116,11 +1209,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B34" sqref="B34"/>
+      <selection pane="topRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="8">
-        <f t="shared" ref="F6:F26" si="1">E6/D6</f>
+        <f t="shared" ref="F6:F25" si="1">E6/D6</f>
         <v>0.25</v>
       </c>
     </row>
@@ -1499,14 +1592,14 @@
         <v>2</v>
       </c>
       <c r="D18" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E18" s="9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1577,20 +1670,20 @@
         <v>10</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D22" s="9">
-        <v>16</v>
-      </c>
-      <c r="E22" s="9">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <v>2.5</v>
       </c>
       <c r="F22" s="8">
         <f t="shared" si="1"/>
-        <v>0.375</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1598,20 +1691,20 @@
         <v>10</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D23" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E23">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="F23" s="8">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1619,16 +1712,16 @@
         <v>10</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D24" s="9">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" si="1"/>
@@ -1640,16 +1733,16 @@
         <v>10</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D25" s="9">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E25">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F25" s="8">
         <f t="shared" si="1"/>
@@ -1661,20 +1754,20 @@
         <v>10</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26" s="9">
-        <v>4</v>
-      </c>
-      <c r="E26">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="E26" s="9">
+        <v>7</v>
       </c>
       <c r="F26" s="8">
-        <f t="shared" si="1"/>
-        <v>0.75</v>
+        <f>E26/D26</f>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -1748,13 +1841,16 @@
         <v>45</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D30" s="9">
         <v>4</v>
       </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
       <c r="F30" s="8">
-        <f t="shared" ref="F30:F32" si="7">E30/D30</f>
+        <f t="shared" ref="F30:F33" si="7">E30/D30</f>
         <v>0</v>
       </c>
     </row>
@@ -1781,312 +1877,335 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="9">
+        <v>2</v>
+      </c>
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" ref="F32" si="8">E32/D32</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B33" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C33" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="9">
-        <v>2</v>
-      </c>
-      <c r="E32" s="9"/>
-      <c r="F32" s="8">
+      <c r="D33" s="9">
+        <v>2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>0</v>
+      </c>
+      <c r="F33" s="8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="7"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="F33" s="8"/>
-    </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="9">
-        <v>20</v>
-      </c>
-      <c r="F34" s="8">
-        <f t="shared" ref="F34:F38" si="8">E34/D34</f>
-        <v>0</v>
-      </c>
+      <c r="A34" s="7"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C35" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="2">
-        <v>45</v>
-      </c>
-      <c r="E35" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D35" s="9">
+        <v>12</v>
+      </c>
       <c r="F35" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="F35:F39" si="9">E35/D35</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D36" s="2">
         <v>45</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="2">
-        <v>125</v>
+      <c r="D37" s="9">
+        <v>45</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D38" s="2">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="10"/>
-      <c r="B39" s="17"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="13" t="s">
+      <c r="A39" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2">
+        <v>75</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="10"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="17"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="11"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="14">
-        <f>SUM(D2:D39)</f>
-        <v>452</v>
-      </c>
-      <c r="E40" s="14">
-        <f>SUM(E2:E39)</f>
-        <v>112.5</v>
-      </c>
-      <c r="F40" s="15">
-        <f>E40/D40</f>
-        <v>0.24889380530973451</v>
-      </c>
-      <c r="H40"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H42" s="1"/>
+      <c r="D41" s="14">
+        <f>SUM(D2:D40)</f>
+        <v>450</v>
+      </c>
+      <c r="E41" s="14">
+        <f>SUM(E2:E40)</f>
+        <v>118.5</v>
+      </c>
+      <c r="F41" s="15">
+        <f>E41/D41</f>
+        <v>0.26333333333333331</v>
+      </c>
+      <c r="H41"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H43" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F38" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F39" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
   </mergeCells>
-  <conditionalFormatting sqref="C41:C1048576 C1:C7 C11:C13 C34:C38 C9">
-    <cfRule type="cellIs" dxfId="35" priority="68" operator="equal">
+  <conditionalFormatting sqref="C42:C1048576 C1:C7 C11:C13 C35:C39 C9">
+    <cfRule type="cellIs" dxfId="44" priority="80" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:C1048576 C1:C7 C11:C13 C34:C38 C9">
-    <cfRule type="containsText" dxfId="34" priority="66" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C41:C1048576 C1:C7 C11:C13 C35:C39 C9">
+    <cfRule type="containsText" dxfId="43" priority="78" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C34:C1048576 C9">
-    <cfRule type="containsText" dxfId="33" priority="65" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C35:C1048576 C9">
+    <cfRule type="containsText" dxfId="42" priority="77" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="32" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="31" priority="59" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="40" priority="71" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="30" priority="58" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="39" priority="70" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="29" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="60" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="28" priority="47" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="37" priority="59" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="27" priority="46" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="36" priority="58" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23 C25:C26">
-    <cfRule type="cellIs" dxfId="26" priority="39" operator="equal">
+  <conditionalFormatting sqref="C22:C26">
+    <cfRule type="cellIs" dxfId="35" priority="51" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23 C25:C26">
-    <cfRule type="containsText" dxfId="25" priority="38" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23 C25:C26">
-    <cfRule type="containsText" dxfId="24" priority="37" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C23)))</formula>
+  <conditionalFormatting sqref="C22:C26">
+    <cfRule type="containsText" dxfId="34" priority="50" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C26">
+    <cfRule type="containsText" dxfId="33" priority="49" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="cellIs" dxfId="23" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="48" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="containsText" dxfId="22" priority="35" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="31" priority="47" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="containsText" dxfId="21" priority="34" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="30" priority="46" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="20" priority="33" operator="equal">
+  <conditionalFormatting sqref="C26">
+    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" dxfId="19" priority="32" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="containsText" dxfId="18" priority="31" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C24)))</formula>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="containsText" dxfId="28" priority="35" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C26">
+    <cfRule type="containsText" dxfId="27" priority="34" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C26)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="26" priority="42" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="25" priority="41" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="24" priority="40" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="19" priority="26" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="18" priority="25" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="17" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="24" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" dxfId="16" priority="29" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C33)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="containsText" dxfId="15" priority="28" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C33)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="cellIs" dxfId="14" priority="24" operator="equal">
+  <conditionalFormatting sqref="C31:C32">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
-    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+  <conditionalFormatting sqref="C31:C32">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C32">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30 C32">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30 C32">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C30">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30 C32">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C30">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Mise en place d'Express
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803032D8-D27F-D540-B5DE-427067817200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12833F3D-BC68-F54B-B048-C46B0B206E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="50">
   <si>
     <t>Tâche</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Environnements d’exécutions</t>
+  </si>
+  <si>
+    <t>Test technos API + mise en place d'Express</t>
   </si>
 </sst>
 </file>
@@ -1091,9 +1094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B26" sqref="B26"/>
+      <selection pane="topRight" activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1798,283 +1801,282 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="7"/>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C35" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="9">
+      <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="8">
-        <f t="shared" ref="F35:F39" si="9">E35/D35</f>
-        <v>0</v>
+      <c r="B34" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="9">
+        <v>4</v>
+      </c>
+      <c r="E34" s="9">
+        <v>4</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" ref="F34" si="9">E34/D34</f>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="2"/>
+        <v>10</v>
+      </c>
       <c r="C36" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D36" s="2">
-        <v>45</v>
-      </c>
-      <c r="E36" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D36" s="9">
+        <v>12</v>
+      </c>
       <c r="F36" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="F36:F40" si="10">E36/D36</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="2">
         <v>45</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D38" s="2">
-        <v>125</v>
+      <c r="D38" s="9">
+        <v>40</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D39" s="2">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="13" t="s">
+      <c r="A40" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" s="2">
+        <v>75</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="17"/>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="18"/>
+      <c r="H41"/>
+    </row>
+    <row r="42" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="14">
-        <f>SUM(D2:D40)</f>
-        <v>450</v>
-      </c>
-      <c r="E41" s="14">
-        <f>SUM(E2:E40)</f>
-        <v>120.5</v>
-      </c>
-      <c r="F41" s="15">
-        <f>E41/D41</f>
-        <v>0.26777777777777778</v>
-      </c>
-      <c r="H41"/>
+      <c r="D42" s="14">
+        <f>SUM(D2:D41)</f>
+        <v>449</v>
+      </c>
+      <c r="E42" s="14">
+        <f>SUM(E2:E41)</f>
+        <v>124.5</v>
+      </c>
+      <c r="F42" s="15">
+        <f>E42/D42</f>
+        <v>0.27728285077951004</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H43" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F39" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F40" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
   </mergeCells>
-  <conditionalFormatting sqref="C42:C1048576 C1:C7 C11:C13 C35:C39 C9">
-    <cfRule type="cellIs" dxfId="32" priority="80" operator="equal">
+  <conditionalFormatting sqref="C43:C1048576 C1:C7 C11:C13 C9 C36:C40">
+    <cfRule type="cellIs" dxfId="32" priority="83" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C1048576 C1:C7 C11:C13 C35:C39 C9">
-    <cfRule type="containsText" dxfId="31" priority="78" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C42:C1048576 C1:C7 C11:C13 C9 C36:C40">
+    <cfRule type="containsText" dxfId="31" priority="81" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C35:C1048576 C9">
-    <cfRule type="containsText" dxfId="30" priority="77" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C36:C1048576">
+    <cfRule type="containsText" dxfId="30" priority="80" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="29" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="75" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="28" priority="71" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="28" priority="74" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="27" priority="70" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="27" priority="73" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="26" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="63" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="25" priority="59" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="25" priority="62" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="24" priority="58" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="24" priority="61" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C26">
-    <cfRule type="cellIs" dxfId="23" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="54" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C26">
-    <cfRule type="containsText" dxfId="22" priority="50" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="22" priority="53" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C26">
-    <cfRule type="containsText" dxfId="21" priority="49" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="21" priority="52" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="cellIs" dxfId="20" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="51" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="containsText" dxfId="19" priority="47" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="19" priority="50" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27:C29">
-    <cfRule type="containsText" dxfId="18" priority="46" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="18" priority="49" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="17" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="39" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="16" priority="35" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="16" priority="38" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="containsText" dxfId="15" priority="34" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="15" priority="37" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C26)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="14" priority="42" operator="equal">
+  <conditionalFormatting sqref="C8">
+    <cfRule type="cellIs" dxfId="11" priority="30" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="13" priority="41" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="12" priority="40" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="11" priority="27" operator="equal">
+    <cfRule type="containsText" dxfId="10" priority="29" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="9" priority="28" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C34">
+    <cfRule type="cellIs" dxfId="8" priority="21" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="10" priority="26" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="9" priority="25" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C33">
-    <cfRule type="cellIs" dxfId="5" priority="18" operator="equal">
+  <conditionalFormatting sqref="C31:C34">
+    <cfRule type="containsText" dxfId="7" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31:C34">
+    <cfRule type="containsText" dxfId="6" priority="19" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C31)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C33">
-    <cfRule type="containsText" dxfId="4" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C33">
-    <cfRule type="containsText" dxfId="3" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Terminé"</formula>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36:C1048576 C1:C34" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Mise en place Express
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCE75ED-B459-7D44-8CB1-4632DA28D9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD48F37-4077-FF4C-AAB8-E3425394F5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
   <si>
     <t>Tâche</t>
   </si>
@@ -199,6 +199,12 @@
   </si>
   <si>
     <t>Choix du framework front-end</t>
+  </si>
+  <si>
+    <t>En cours</t>
+  </si>
+  <si>
+    <t>Mise en place de l'environnement de dévellopement</t>
   </si>
 </sst>
 </file>
@@ -463,7 +469,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="105">
+  <dxfs count="108">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1824,11 +1860,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H36" sqref="H36"/>
+      <selection pane="topRight" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2549,7 +2585,7 @@
         <v>5</v>
       </c>
       <c r="F34" s="8">
-        <f t="shared" ref="F34:F39" si="10">E34/D34</f>
+        <f t="shared" ref="F34:F40" si="10">E34/D34</f>
         <v>1.25</v>
       </c>
     </row>
@@ -2618,39 +2654,39 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D38" s="9">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E38" s="9">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F38" s="8">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f t="shared" ref="F38" si="11">E38/D38</f>
+        <v>0.625</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D39" s="9">
-        <v>4</v>
-      </c>
-      <c r="E39">
+        <v>12</v>
+      </c>
+      <c r="E39" s="9">
         <v>0</v>
       </c>
       <c r="F39" s="8">
@@ -2659,215 +2695,251 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F40" s="8"/>
+      <c r="A40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="9">
+        <v>4</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D41" s="2">
-        <v>45</v>
-      </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="8">
-        <f t="shared" ref="F41:F44" si="11">E41/D41</f>
-        <v>0</v>
-      </c>
+      <c r="F41" s="8"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="9">
-        <v>40</v>
+      <c r="D42" s="2">
+        <v>45</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="F42:F45" si="12">E42/D42</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D43" s="2">
-        <v>125</v>
+      <c r="D43" s="9">
+        <v>40</v>
       </c>
       <c r="E43" s="2"/>
       <c r="F43" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="2">
-        <v>75</v>
+        <v>125</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="10"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="18"/>
-      <c r="H45"/>
-    </row>
-    <row r="46" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="11"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="13" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="2"/>
+      <c r="C45" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="2">
+        <v>75</v>
+      </c>
+      <c r="E45" s="2"/>
+      <c r="F45" s="8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="10"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="17"/>
+      <c r="F46" s="18"/>
+      <c r="H46"/>
+    </row>
+    <row r="47" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="14">
-        <f>SUM(D2:D45)</f>
-        <v>455</v>
-      </c>
-      <c r="E46" s="14">
-        <f>SUM(E2:E45)</f>
-        <v>140.5</v>
-      </c>
-      <c r="F46" s="15">
-        <f>E46/D46</f>
-        <v>0.3087912087912088</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H47" s="1"/>
+      <c r="D47" s="14">
+        <f>SUM(D2:D46)</f>
+        <v>459</v>
+      </c>
+      <c r="E47" s="14">
+        <f>SUM(E2:E46)</f>
+        <v>143</v>
+      </c>
+      <c r="F47" s="15">
+        <f>E47/D47</f>
+        <v>0.31154684095860569</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H48" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F44" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F45" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B45:F45"/>
+    <mergeCell ref="B46:F46"/>
   </mergeCells>
-  <conditionalFormatting sqref="C47:C1048576 C1:C7 C11:C13 C9 C41:C44">
-    <cfRule type="cellIs" dxfId="104" priority="179" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46:C1048576 C1:C7 C11:C13 C9 C41:C44">
-    <cfRule type="containsText" dxfId="103" priority="177" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C48:C1048576 C1:C7 C11:C13 C9 C42:C45">
+    <cfRule type="cellIs" dxfId="107" priority="182" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C1048576 C1:C7 C11:C13 C9 C42:C45">
+    <cfRule type="containsText" dxfId="106" priority="180" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C41:C1048576">
-    <cfRule type="containsText" dxfId="102" priority="176" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C42:C1048576">
+    <cfRule type="containsText" dxfId="105" priority="179" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="101" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="174" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="100" priority="170" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="173" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="99" priority="169" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="172" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="98" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="162" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="97" priority="158" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="96" priority="157" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
+    <cfRule type="cellIs" dxfId="98" priority="153" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C28">
+    <cfRule type="containsText" dxfId="97" priority="152" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C28">
+    <cfRule type="containsText" dxfId="96" priority="151" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
     <cfRule type="cellIs" dxfId="95" priority="150" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C28">
+  <conditionalFormatting sqref="C29">
     <cfRule type="containsText" dxfId="94" priority="149" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C28">
+      <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
     <cfRule type="containsText" dxfId="93" priority="148" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="92" priority="147" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="91" priority="146" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="90" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="89" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="129" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="88" priority="125" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="128" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="87" priority="124" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="127" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="86" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="120" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="85" priority="116" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="119" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="84" priority="115" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="118" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="86" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="85" priority="98" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="84" priority="97" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
@@ -2885,34 +2957,34 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="80" priority="93" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="79" priority="92" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="78" priority="91" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
+    <cfRule type="cellIs" dxfId="80" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C37">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C37">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
     <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C37">
+  <conditionalFormatting sqref="C40">
     <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
     <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
@@ -2930,34 +3002,34 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C39)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C34">
     <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
     <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C35">
     <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
     <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
@@ -2975,34 +3047,34 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
@@ -3035,19 +3107,19 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C36">
     <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C36">
     <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
     <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
@@ -3140,19 +3212,19 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
@@ -3275,23 +3347,23 @@
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C38">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C38">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C41:C1048576 C1:C39" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42:C1048576 C1:C40" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add Neo4j in Docker
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FFB1BE-897C-C04A-BFA9-C4AECC5FDAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06588057-7E7A-1B46-9F4F-C28730884FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -484,7 +484,637 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="147">
+  <dxfs count="210">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2267,9 +2897,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H39" sqref="H39"/>
+      <selection pane="topRight" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3113,11 +3743,11 @@
         <v>8</v>
       </c>
       <c r="E40" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F40" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -3128,17 +3758,17 @@
         <v>57</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D41" s="9">
         <v>2</v>
       </c>
       <c r="E41" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F41" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -3300,11 +3930,11 @@
       </c>
       <c r="E51" s="14">
         <f>SUM(E2:E50)</f>
-        <v>145.5</v>
+        <v>149.5</v>
       </c>
       <c r="F51" s="15">
         <f>E51/D51</f>
-        <v>0.32333333333333331</v>
+        <v>0.3322222222222222</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -3316,726 +3946,891 @@
     <mergeCell ref="B50:F50"/>
   </mergeCells>
   <conditionalFormatting sqref="C52:C1048576 C1:C7 C11:C13 C9 C47:C49">
-    <cfRule type="cellIs" dxfId="146" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="287" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C1048576 C1:C7 C11:C13 C9 C47:C49">
-    <cfRule type="containsText" dxfId="145" priority="219" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="285" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C11:C13 C9 C47:C1048576">
-    <cfRule type="containsText" dxfId="144" priority="218" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="284" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="143" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="142" priority="212" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="141" priority="211" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="140" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="139" priority="200" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="138" priority="199" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="137" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="136" priority="191" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="135" priority="190" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="134" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="133" priority="188" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="132" priority="187" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="131" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="234" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="130" priority="167" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="233" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="129" priority="166" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="232" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="128" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="225" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="127" priority="158" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="224" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="126" priority="157" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="223" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="125" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="124" priority="137" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="123" priority="136" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="122" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="121" priority="134" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="120" priority="133" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="119" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="118" priority="119" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="117" priority="118" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42 C45">
-    <cfRule type="cellIs" dxfId="116" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="183" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42 C45">
-    <cfRule type="containsText" dxfId="115" priority="116" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="182" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42 C45">
-    <cfRule type="containsText" dxfId="114" priority="115" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="181" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:C41">
-    <cfRule type="cellIs" dxfId="113" priority="114" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40:C41">
-    <cfRule type="containsText" dxfId="112" priority="113" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="176" priority="180" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="175" priority="179" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40:C41">
-    <cfRule type="containsText" dxfId="111" priority="112" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="174" priority="178" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="110" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="177" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="176" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="108" priority="109" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="175" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="107" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="174" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="173" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="105" priority="106" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="172" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="104" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="171" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="103" priority="104" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="170" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="102" priority="103" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="169" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="101" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="168" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="100" priority="101" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="167" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="99" priority="100" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="166" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="98" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="165" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="97" priority="98" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="164" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="96" priority="97" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="163" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="95" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="162" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="93" priority="94" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="92" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="159" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="91" priority="92" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="158" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="90" priority="91" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="157" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="89" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="156" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="155" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="87" priority="88" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="154" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="86" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="153" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="152" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="151" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="83" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="150" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="149" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="81" priority="82" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="148" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="80" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="147" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="77" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="144" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="142" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="141" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="140" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="139" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="134" priority="138" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="133" priority="137" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="132" priority="136" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="131" priority="135" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="130" priority="134" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="129" priority="133" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="128" priority="132" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="127" priority="131" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="126" priority="130" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="125" priority="129" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="124" priority="128" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="123" priority="127" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="122" priority="126" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="121" priority="125" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="120" priority="124" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="119" priority="123" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="117" priority="121" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="116" priority="120" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="115" priority="119" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="114" priority="118" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="113" priority="117" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="112" priority="116" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="111" priority="115" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="110" priority="114" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="108" priority="112" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="107" priority="111" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="106" priority="110" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="105" priority="109" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="104" priority="75" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="103" priority="74" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="102" priority="73" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="101" priority="105" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="100" priority="104" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="99" priority="103" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="98" priority="102" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="96" priority="100" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="95" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="93" priority="97" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="87" priority="91" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="86" priority="90" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="84" priority="88" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="83" priority="87" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="81" priority="85" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="78" priority="82" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="77" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="75" priority="79" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C44">
     <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="65" priority="66" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="62" priority="63" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="56" priority="57" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="40" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="39" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="32" priority="33" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="29" priority="30" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="26" priority="27" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="23" priority="24" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47:C1048576 C1:C45" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
API register, verify, login
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC75A8D6-3790-024B-84C5-2AD8257E4AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A86E16-B9C9-1A4E-8FAD-3C12A45104FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="19680" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26580" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
@@ -2932,7 +2932,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H43" sqref="H43"/>
+      <selection pane="topRight" activeCell="K48" sqref="K48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3734,11 +3734,11 @@
         <v>4</v>
       </c>
       <c r="E38" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" ref="F38:F39" si="11">E38/D38</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -3878,14 +3878,14 @@
         <v>53</v>
       </c>
       <c r="D45" s="9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E45">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F45" s="8">
         <f t="shared" si="13"/>
-        <v>1.125</v>
+        <v>0.8125</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -3938,7 +3938,7 @@
         <v>22</v>
       </c>
       <c r="D49" s="2">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="8">
@@ -3980,15 +3980,15 @@
       </c>
       <c r="D52" s="14">
         <f>SUM(D2:D51)</f>
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="E52" s="14">
         <f>SUM(E2:E51)</f>
-        <v>158.5</v>
+        <v>164.5</v>
       </c>
       <c r="F52" s="15">
         <f>E52/D52</f>
-        <v>0.34606986899563319</v>
+        <v>0.3647450110864745</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Création des endpoints /profile
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A75AF58D-E340-1746-911A-7B67EDC8B778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AC9B19-E13A-1A41-A807-61A8AE841B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -496,1057 +496,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="420">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="315">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5011,7 +3961,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J50" sqref="J50"/>
+      <selection pane="topRight" activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6044,11 +4994,11 @@
         <v>4</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F49" s="8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -6126,11 +5076,11 @@
       </c>
       <c r="E55" s="14">
         <f>SUM(E2:E54)</f>
-        <v>180.5</v>
+        <v>183.5</v>
       </c>
       <c r="F55" s="15">
         <f>E55/D55</f>
-        <v>0.40022172949002216</v>
+        <v>0.40687361419068735</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -6142,1397 +5092,1397 @@
     <mergeCell ref="B54:F54"/>
   </mergeCells>
   <conditionalFormatting sqref="C56:C1048576 C1:C7 C11:C13 C9 C51:C53">
-    <cfRule type="cellIs" dxfId="419" priority="566" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="566" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C1048576 C1:C7 C11:C13 C9 C51:C53">
-    <cfRule type="containsText" dxfId="418" priority="564" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="564" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C11:C13 C9 C51:C1048576">
-    <cfRule type="containsText" dxfId="417" priority="563" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="563" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="416" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="415" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="414" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="413" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="412" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="411" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="410" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="409" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="408" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="407" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="406" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="405" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="404" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="513" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="403" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="512" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="402" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="511" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="401" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="504" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="400" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="503" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="399" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="502" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="398" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="483" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="397" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="482" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="396" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="481" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="395" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="480" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="394" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="479" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="393" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="478" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="392" priority="465" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="391" priority="464" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="390" priority="463" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="389" priority="462" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="388" priority="461" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="387" priority="460" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="386" priority="459" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="385" priority="458" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="458" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="384" priority="457" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="457" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="383" priority="456" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="382" priority="455" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="455" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="381" priority="454" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="454" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="380" priority="453" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="453" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="379" priority="452" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="452" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="378" priority="451" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="451" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="377" priority="450" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="450" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="376" priority="449" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="449" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="375" priority="448" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="448" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="374" priority="447" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="447" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="373" priority="446" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="446" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="372" priority="445" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="445" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="371" priority="444" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="444" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="370" priority="443" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="443" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="369" priority="442" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="442" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="368" priority="441" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="441" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="367" priority="440" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="440" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="366" priority="439" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="439" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="365" priority="438" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="438" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="364" priority="437" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="437" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="363" priority="436" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="436" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="362" priority="435" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="435" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="361" priority="434" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="434" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="360" priority="433" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="433" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="359" priority="432" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="432" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="358" priority="431" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="431" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="357" priority="430" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="430" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="356" priority="429" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="429" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="355" priority="428" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="428" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="354" priority="427" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="427" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="353" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="426" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="352" priority="425" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="425" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="351" priority="424" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="424" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="350" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="423" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="349" priority="422" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="348" priority="421" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="347" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="346" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="345" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="344" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="417" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="343" priority="416" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="342" priority="415" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="341" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="414" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="340" priority="413" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="339" priority="412" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="338" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="411" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="337" priority="410" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="336" priority="409" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="335" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="408" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="334" priority="407" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="333" priority="406" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="332" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="405" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="331" priority="404" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="330" priority="403" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="329" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="402" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="328" priority="401" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="327" priority="400" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="326" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="399" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="325" priority="398" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="324" priority="397" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="323" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="396" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="322" priority="395" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="395" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="321" priority="394" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="394" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="320" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="393" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="319" priority="392" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="392" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="318" priority="391" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="391" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="317" priority="390" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="390" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="316" priority="389" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="389" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="315" priority="388" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="388" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="314" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="354" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="313" priority="353" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="353" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="312" priority="352" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="352" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="311" priority="384" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="384" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="310" priority="383" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="383" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="309" priority="382" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="382" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="308" priority="381" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="381" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="307" priority="380" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="380" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="306" priority="379" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="379" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="305" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="378" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="304" priority="377" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="377" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="303" priority="376" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="376" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="302" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="375" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="301" priority="374" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="374" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="300" priority="373" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="373" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="299" priority="372" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="372" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="298" priority="371" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="371" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="297" priority="370" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="370" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="296" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="369" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="295" priority="368" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="368" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="294" priority="367" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="367" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="293" priority="366" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="366" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="292" priority="365" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="365" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="291" priority="364" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="364" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="290" priority="363" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="363" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="289" priority="362" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="362" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="288" priority="361" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="361" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="287" priority="360" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="360" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="286" priority="359" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="359" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="285" priority="358" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="358" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="284" priority="357" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="357" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="283" priority="356" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="356" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="282" priority="355" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="355" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="281" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="351" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="280" priority="350" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="350" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="279" priority="349" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="349" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="278" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="348" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="277" priority="347" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="347" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="276" priority="346" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="346" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="275" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="274" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="273" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="272" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="312" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="271" priority="311" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="311" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="270" priority="310" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="310" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="269" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="309" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="268" priority="308" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="308" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="267" priority="307" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="307" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="266" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="306" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="265" priority="305" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="305" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="264" priority="304" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="304" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="263" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="303" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="262" priority="302" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="302" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="261" priority="301" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="301" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="260" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="300" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="259" priority="299" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="299" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="258" priority="298" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="298" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="257" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="297" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="256" priority="296" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="296" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="255" priority="295" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="295" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="254" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="294" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="253" priority="293" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="293" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="252" priority="292" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="292" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="251" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="291" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="250" priority="290" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="290" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="249" priority="289" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="289" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="248" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="288" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="247" priority="287" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="287" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="246" priority="286" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="286" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="245" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="285" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="244" priority="284" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="284" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="243" priority="283" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="283" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="206" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="177" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="205" priority="176" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="176" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="204" priority="175" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="175" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="203" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="207" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="202" priority="206" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="206" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="201" priority="205" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="205" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="200" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="199" priority="203" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="198" priority="202" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="197" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="196" priority="200" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="195" priority="199" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="194" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="198" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="193" priority="197" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="197" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="192" priority="196" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="196" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="191" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="195" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="190" priority="194" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="194" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="189" priority="193" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="193" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="188" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="192" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="187" priority="191" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="191" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="186" priority="190" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="190" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="185" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="189" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="184" priority="188" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="188" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="183" priority="187" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="187" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="182" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="181" priority="185" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="180" priority="184" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="179" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="183" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="178" priority="182" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="182" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="177" priority="181" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="181" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="176" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="180" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="175" priority="179" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="179" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="174" priority="178" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="178" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="173" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="174" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="172" priority="173" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="173" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="171" priority="172" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="172" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="170" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="141" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="169" priority="140" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="140" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="168" priority="139" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="139" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="167" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="171" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="166" priority="170" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="170" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="165" priority="169" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="169" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="164" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="168" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="163" priority="167" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="167" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="162" priority="166" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="166" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="161" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="165" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="160" priority="164" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="164" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="159" priority="163" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="163" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="158" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="162" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="157" priority="161" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="156" priority="160" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="155" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="159" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="154" priority="158" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="158" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="153" priority="157" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="157" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="152" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="156" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="151" priority="155" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="155" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="150" priority="154" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="154" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="149" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="153" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="148" priority="152" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="152" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="147" priority="151" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="151" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="146" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="150" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="145" priority="149" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="149" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="144" priority="148" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="148" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="143" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="147" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="142" priority="146" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="73" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="141" priority="145" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="72" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="140" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="144" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="70" priority="143" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="138" priority="142" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="69" priority="142" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="134" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="133" priority="71" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="132" priority="70" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="66" priority="70" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="131" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="102" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="130" priority="101" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="64" priority="101" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="129" priority="100" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="63" priority="100" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="128" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="99" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="127" priority="98" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="61" priority="98" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="126" priority="97" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="60" priority="97" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="125" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="96" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="124" priority="95" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="58" priority="95" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="123" priority="94" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="57" priority="94" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="122" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="93" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="121" priority="92" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="55" priority="92" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="120" priority="91" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="54" priority="91" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="119" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="90" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="118" priority="89" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="52" priority="89" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="117" priority="88" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="51" priority="88" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="116" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="87" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="115" priority="86" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="49" priority="86" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="114" priority="85" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="48" priority="85" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="113" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="84" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="112" priority="83" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="46" priority="83" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="111" priority="82" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="45" priority="82" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="110" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="81" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="109" priority="80" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="43" priority="80" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="108" priority="79" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="42" priority="79" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="107" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="78" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="106" priority="77" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="40" priority="77" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="105" priority="76" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="39" priority="76" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="104" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="75" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="103" priority="74" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="37" priority="74" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="102" priority="73" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="36" priority="73" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix on /auth & /profile endpoints
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12AC9B19-E13A-1A41-A807-61A8AE841B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F5179A-4D92-FA44-A8A4-5A086E950F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$53</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$56</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
   <si>
     <t>Tâche</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>Express, endpoints /profile</t>
+  </si>
+  <si>
+    <t>Express, endpoints /users</t>
+  </si>
+  <si>
+    <t>Ajout de Neo4j et de Neode</t>
+  </si>
+  <si>
+    <t>Surcharge des endpoints existants avec Neode</t>
   </si>
 </sst>
 </file>
@@ -496,7 +505,727 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="315">
+  <dxfs count="387">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3957,11 +4686,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L49" sqref="L49"/>
+      <selection pane="topRight" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4988,36 +5717,58 @@
         <v>64</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="D49" s="9">
         <v>4</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F49" s="8">
         <f t="shared" si="10"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F50" s="8"/>
+      <c r="A50" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="9">
+        <v>2</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50" s="8">
+        <f t="shared" ref="F50" si="16">E50/D50</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="C51" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D51" s="2">
-        <v>15</v>
-      </c>
-      <c r="E51" s="2"/>
+      <c r="D51" s="9">
+        <v>4</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
       <c r="F51" s="8">
-        <f t="shared" ref="F51:F53" si="16">E51/D51</f>
+        <f t="shared" ref="F51:F52" si="17">E51/D51</f>
         <v>0</v>
       </c>
     </row>
@@ -5025,1649 +5776,1705 @@
       <c r="A52" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="2"/>
+      <c r="B52" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="C52" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D52" s="2">
-        <v>175</v>
-      </c>
-      <c r="E52" s="2"/>
+      <c r="D52" s="9">
+        <v>2</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
       <c r="F52" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="9" t="s">
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D53" s="2">
-        <v>50</v>
-      </c>
-      <c r="E53" s="2"/>
-      <c r="F53" s="8">
-        <f t="shared" si="16"/>
+      <c r="D54" s="2">
+        <v>15</v>
+      </c>
+      <c r="E54" s="2"/>
+      <c r="F54" s="8">
+        <f t="shared" ref="F54:F56" si="18">E54/D54</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="10"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="17"/>
-      <c r="E54" s="17"/>
-      <c r="F54" s="18"/>
-      <c r="H54"/>
-    </row>
-    <row r="55" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="11"/>
-      <c r="B55" s="12"/>
-      <c r="C55" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="14">
-        <f>SUM(D2:D54)</f>
-        <v>451</v>
-      </c>
-      <c r="E55" s="14">
-        <f>SUM(E2:E54)</f>
-        <v>183.5</v>
-      </c>
-      <c r="F55" s="15">
-        <f>E55/D55</f>
-        <v>0.40687361419068735</v>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="2">
+        <v>175</v>
+      </c>
+      <c r="E55" s="2"/>
+      <c r="F55" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H56" s="1"/>
+      <c r="A56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="2"/>
+      <c r="C56" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="2">
+        <v>50</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="10"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="18"/>
+      <c r="H57"/>
+    </row>
+    <row r="58" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="14">
+        <f>SUM(D2:D57)</f>
+        <v>459</v>
+      </c>
+      <c r="E58" s="14">
+        <f>SUM(E2:E57)</f>
+        <v>184.5</v>
+      </c>
+      <c r="F58" s="15">
+        <f>E58/D58</f>
+        <v>0.40196078431372551</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H59" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F53" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F56" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B57:F57"/>
   </mergeCells>
-  <conditionalFormatting sqref="C56:C1048576 C1:C7 C11:C13 C9 C51:C53">
-    <cfRule type="cellIs" dxfId="314" priority="566" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C55:C1048576 C1:C7 C11:C13 C9 C51:C53">
-    <cfRule type="containsText" dxfId="313" priority="564" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C59:C1048576 C1:C7 C11:C13 C9 C54:C56">
+    <cfRule type="cellIs" dxfId="386" priority="638" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58:C1048576 C1:C7 C11:C13 C9 C54:C56">
+    <cfRule type="containsText" dxfId="385" priority="636" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C51:C1048576">
-    <cfRule type="containsText" dxfId="312" priority="563" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C54:C1048576">
+    <cfRule type="containsText" dxfId="384" priority="635" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="311" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="310" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="309" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="308" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="307" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="306" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="305" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="609" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="304" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="608" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="303" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="607" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="302" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="606" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="301" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="605" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="300" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="604" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="299" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="585" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="298" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="584" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="297" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="583" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="296" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="576" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="295" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="575" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="294" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="574" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="293" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="292" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="291" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="290" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="289" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="288" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
+    <cfRule type="cellIs" dxfId="359" priority="537" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C37">
+    <cfRule type="containsText" dxfId="358" priority="536" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C37">
+    <cfRule type="containsText" dxfId="357" priority="535" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="cellIs" dxfId="356" priority="534" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="containsText" dxfId="355" priority="533" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="containsText" dxfId="354" priority="532" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="353" priority="531" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="352" priority="530" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="351" priority="529" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="350" priority="528" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="349" priority="527" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="348" priority="526" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="347" priority="525" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="346" priority="524" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="345" priority="523" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="344" priority="522" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="343" priority="521" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="342" priority="520" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="341" priority="519" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="340" priority="518" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="339" priority="517" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="338" priority="516" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="337" priority="515" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="336" priority="514" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="335" priority="513" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="334" priority="512" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="333" priority="511" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="332" priority="510" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="331" priority="509" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="330" priority="508" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="329" priority="507" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="328" priority="506" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="327" priority="505" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="326" priority="504" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="325" priority="503" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="324" priority="502" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="323" priority="501" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="322" priority="500" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="321" priority="499" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="320" priority="498" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="319" priority="497" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="318" priority="496" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="317" priority="495" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="316" priority="494" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="315" priority="493" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="314" priority="492" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="313" priority="491" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="312" priority="490" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="311" priority="489" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="310" priority="488" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="309" priority="487" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="308" priority="486" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="307" priority="485" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="306" priority="484" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="305" priority="483" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="304" priority="482" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="303" priority="481" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="302" priority="480" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="301" priority="479" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="300" priority="478" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="299" priority="477" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="298" priority="476" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="297" priority="475" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="296" priority="474" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="295" priority="473" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="294" priority="472" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="293" priority="471" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="292" priority="470" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="291" priority="469" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="290" priority="468" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="289" priority="467" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="288" priority="466" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="287" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C37">
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="286" priority="464" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="285" priority="463" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="284" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="283" priority="461" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="282" priority="460" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="281" priority="459" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="280" priority="458" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="279" priority="457" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="281" priority="426" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="280" priority="425" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="279" priority="424" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="278" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="277" priority="455" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="276" priority="454" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="275" priority="453" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="274" priority="452" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="273" priority="451" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="272" priority="450" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="271" priority="449" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="270" priority="448" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="269" priority="447" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="268" priority="446" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="267" priority="445" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="266" priority="444" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="265" priority="443" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="264" priority="442" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="263" priority="441" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="262" priority="440" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="261" priority="439" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="260" priority="438" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="259" priority="437" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="258" priority="436" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="257" priority="435" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="256" priority="434" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="255" priority="433" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="254" priority="432" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="253" priority="431" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="252" priority="430" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="251" priority="429" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="250" priority="428" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="249" priority="427" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="248" priority="426" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="247" priority="425" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="246" priority="424" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="245" priority="423" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="244" priority="422" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="243" priority="421" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="242" priority="420" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="241" priority="419" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="240" priority="418" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="239" priority="417" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="238" priority="416" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="237" priority="415" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="236" priority="414" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="235" priority="413" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="234" priority="412" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="233" priority="411" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="232" priority="410" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="231" priority="409" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="230" priority="408" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="229" priority="407" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="228" priority="406" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="227" priority="405" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="226" priority="404" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="225" priority="403" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="224" priority="402" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="223" priority="401" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="222" priority="400" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="221" priority="399" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="220" priority="398" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="219" priority="397" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="218" priority="396" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="217" priority="395" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="216" priority="394" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="215" priority="393" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="214" priority="392" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="213" priority="391" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="212" priority="390" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="211" priority="389" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="210" priority="388" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="209" priority="354" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="208" priority="353" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="207" priority="352" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="206" priority="384" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="205" priority="383" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="204" priority="382" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="203" priority="381" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="202" priority="380" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="201" priority="379" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="200" priority="378" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="199" priority="377" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="198" priority="376" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="197" priority="375" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="196" priority="374" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="195" priority="373" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="194" priority="372" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="193" priority="371" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="192" priority="370" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="191" priority="369" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="190" priority="368" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="189" priority="367" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="188" priority="366" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="187" priority="365" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="186" priority="364" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="185" priority="363" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="184" priority="362" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="183" priority="361" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="182" priority="360" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="181" priority="359" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="180" priority="358" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="179" priority="357" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="178" priority="356" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="177" priority="355" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="176" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="423" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="175" priority="350" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="174" priority="349" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="173" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="172" priority="347" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="171" priority="346" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="170" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="354" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="169" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="353" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="168" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="352" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="167" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="384" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="166" priority="311" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="383" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="165" priority="310" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="382" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="164" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="381" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="163" priority="308" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="380" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="162" priority="307" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="379" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="161" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="378" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="160" priority="305" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="377" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="159" priority="304" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="376" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="158" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="375" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="157" priority="302" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="374" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="156" priority="301" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="373" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="155" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="372" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="154" priority="299" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="371" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="153" priority="298" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="370" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="152" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="369" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="151" priority="296" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="368" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="150" priority="295" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="367" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="149" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="366" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="148" priority="293" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="365" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="147" priority="292" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="364" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="146" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="363" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="145" priority="290" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="362" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="144" priority="289" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="361" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="143" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="360" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="142" priority="287" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="359" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="141" priority="286" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="358" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="140" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="357" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="139" priority="284" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="356" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="138" priority="283" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="355" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="137" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="249" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="136" priority="176" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="248" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="135" priority="175" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="247" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="134" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="133" priority="206" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="132" priority="205" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="131" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="130" priority="203" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="129" priority="202" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="128" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="127" priority="200" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="126" priority="199" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="125" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="124" priority="197" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="123" priority="196" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="122" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="121" priority="194" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="120" priority="193" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="119" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="118" priority="191" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="117" priority="190" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="116" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="115" priority="188" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="114" priority="187" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="113" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="112" priority="185" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="111" priority="184" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="110" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="109" priority="182" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="108" priority="181" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="107" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="252" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="106" priority="179" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="251" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="105" priority="178" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="250" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="104" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="246" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="103" priority="173" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="245" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="102" priority="172" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="244" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="101" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="213" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="100" priority="140" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="212" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="99" priority="139" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="211" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="98" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="243" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="97" priority="170" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="242" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="96" priority="169" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="241" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="95" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="240" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="94" priority="167" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="239" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="93" priority="166" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="238" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="92" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="237" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="91" priority="164" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="236" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="90" priority="163" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="235" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="89" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="234" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="88" priority="161" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="233" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="87" priority="160" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="232" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="86" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="231" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="85" priority="158" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="230" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="84" priority="157" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="229" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="83" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="228" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="82" priority="155" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="227" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="81" priority="154" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="226" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="80" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="225" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="79" priority="152" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="224" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="78" priority="151" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="223" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="77" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="222" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="76" priority="149" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="221" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="75" priority="148" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="220" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="74" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="219" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="73" priority="146" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="218" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="72" priority="145" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="217" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="71" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="216" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="70" priority="143" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="215" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="69" priority="142" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="214" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="144" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="66" priority="70" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="142" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="65" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="174" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="64" priority="101" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="173" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="63" priority="100" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="172" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="62" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="171" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="61" priority="98" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="170" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="60" priority="97" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="169" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="59" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="168" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="58" priority="95" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="167" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="57" priority="94" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="166" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="56" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="165" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="55" priority="92" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="164" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="54" priority="91" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="163" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="53" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="162" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="52" priority="89" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="51" priority="88" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="50" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="159" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="49" priority="86" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="158" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="48" priority="85" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="157" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="47" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="156" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="46" priority="83" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="155" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="45" priority="82" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="154" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="44" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="153" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="43" priority="80" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="152" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="42" priority="79" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="151" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="41" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="150" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="40" priority="77" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="149" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="39" priority="76" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="148" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="38" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="147" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="37" priority="74" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="36" priority="73" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="42" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="41" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="40" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="71" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="70" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="69" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="68" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="67" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="66" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="65" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="64" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="63" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="62" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="61" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="60" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="59" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="58" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="57" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="56" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="55" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="53" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="52" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="50" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="49" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="48" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="47" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="46" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="45" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="73" priority="44" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="72" priority="43" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="cellIs" dxfId="71" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="containsText" dxfId="69" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:C52">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:C52">
+    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51:C52">
+    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51:C1048576 C1:C49" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54:C1048576 C1:C52" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[S1] Création des endpoints /users
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F5179A-4D92-FA44-A8A4-5A086E950F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8166783-D36E-AE40-AAFF-D691EF4AAD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -505,337 +505,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="387">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="354">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4690,7 +4360,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J51" sqref="J51"/>
+      <selection pane="topRight" activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5738,17 +5408,17 @@
         <v>65</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D50" s="9">
         <v>2</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F50" s="8">
         <f t="shared" ref="F50" si="16">E50/D50</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -5759,7 +5429,7 @@
         <v>66</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="D51" s="9">
         <v>4</v>
@@ -5868,11 +5538,11 @@
       </c>
       <c r="E58" s="14">
         <f>SUM(E2:E57)</f>
-        <v>184.5</v>
+        <v>188.5</v>
       </c>
       <c r="F58" s="15">
         <f>E58/D58</f>
-        <v>0.40196078431372551</v>
+        <v>0.41067538126361658</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -5884,1592 +5554,1757 @@
     <mergeCell ref="B57:F57"/>
   </mergeCells>
   <conditionalFormatting sqref="C59:C1048576 C1:C7 C11:C13 C9 C54:C56">
-    <cfRule type="cellIs" dxfId="386" priority="638" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="674" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C1048576 C1:C7 C11:C13 C9 C54:C56">
-    <cfRule type="containsText" dxfId="385" priority="636" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="672" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C11:C13 C9 C54:C1048576">
-    <cfRule type="containsText" dxfId="384" priority="635" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="671" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="383" priority="630" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="666" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="382" priority="629" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="665" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="381" priority="628" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="664" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="380" priority="618" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="654" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="379" priority="617" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="653" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="378" priority="616" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="652" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="377" priority="609" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="645" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="376" priority="608" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="644" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="375" priority="607" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="643" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="374" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="642" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="373" priority="605" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="641" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="372" priority="604" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="640" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="371" priority="585" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="621" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="370" priority="584" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="620" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="369" priority="583" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="619" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="368" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="612" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="367" priority="575" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="611" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="366" priority="574" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="610" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="365" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="591" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="364" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="590" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="363" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="589" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="362" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="588" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="361" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="587" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="360" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="586" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="359" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="573" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="358" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="572" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="357" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="571" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="356" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="355" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="354" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="353" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="567" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="352" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="566" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="351" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="565" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="350" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="349" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="348" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="347" priority="525" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="346" priority="524" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="345" priority="523" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="344" priority="522" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="343" priority="521" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="342" priority="520" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="341" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="340" priority="518" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="339" priority="517" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="338" priority="516" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="337" priority="515" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="336" priority="514" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="335" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="334" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="333" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="332" priority="510" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="331" priority="509" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="330" priority="508" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="329" priority="507" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="328" priority="506" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="327" priority="505" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="326" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="325" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="324" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="323" priority="501" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="322" priority="500" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="321" priority="499" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="320" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="319" priority="497" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="318" priority="496" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="317" priority="495" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="531" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="316" priority="494" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="530" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="315" priority="493" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="529" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="314" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="528" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="313" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="527" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="312" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="526" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="311" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="525" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="310" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="524" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="309" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="523" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="308" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="522" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="307" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="521" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="306" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="520" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="305" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="519" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="304" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="518" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="303" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="517" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="302" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="516" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="301" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="515" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="300" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="514" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="299" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="513" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="298" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="512" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="297" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="511" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="296" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="510" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="295" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="509" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="294" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="508" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="293" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="507" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="292" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="506" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="291" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="505" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="290" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="504" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="289" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="503" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="288" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="502" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="287" priority="465" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="501" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="286" priority="464" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="500" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="285" priority="463" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="499" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="284" priority="462" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="498" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="283" priority="461" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="497" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="282" priority="460" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="496" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="281" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="280" priority="425" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="279" priority="424" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="278" priority="456" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="492" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="277" priority="455" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="491" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="276" priority="454" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="490" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="275" priority="453" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="489" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="274" priority="452" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="488" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="273" priority="451" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="487" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="272" priority="450" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="486" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="271" priority="449" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="485" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="270" priority="448" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="484" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="269" priority="447" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="483" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="268" priority="446" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="482" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="267" priority="445" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="481" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="266" priority="444" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="480" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="265" priority="443" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="479" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="264" priority="442" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="478" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="263" priority="441" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="477" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="262" priority="440" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="476" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="261" priority="439" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="475" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="260" priority="438" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="474" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="259" priority="437" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="473" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="258" priority="436" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="472" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="257" priority="435" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="471" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="256" priority="434" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="470" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="255" priority="433" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="469" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="254" priority="432" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="468" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="253" priority="431" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="467" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="252" priority="430" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="466" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="251" priority="429" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="250" priority="428" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="249" priority="427" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="248" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="247" priority="422" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="458" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="246" priority="421" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="457" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="245" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="244" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="455" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="243" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="454" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="242" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="390" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="241" priority="353" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="389" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="240" priority="352" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="388" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="239" priority="384" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="238" priority="383" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="237" priority="382" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="236" priority="381" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="417" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="235" priority="380" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="234" priority="379" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="233" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="414" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="232" priority="377" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="231" priority="376" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="230" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="411" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="229" priority="374" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="228" priority="373" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="227" priority="372" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="408" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="226" priority="371" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="225" priority="370" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="224" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="405" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="223" priority="368" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="222" priority="367" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="221" priority="366" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="402" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="220" priority="365" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="219" priority="364" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="218" priority="363" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="399" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="217" priority="362" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="216" priority="361" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="215" priority="360" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="396" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="214" priority="359" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="395" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="213" priority="358" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="394" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="212" priority="357" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="393" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="211" priority="356" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="392" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="210" priority="355" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="391" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="209" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="285" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="208" priority="248" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="284" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="207" priority="247" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="283" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="206" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="315" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="205" priority="278" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="314" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="204" priority="277" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="313" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="203" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="312" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="202" priority="275" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="311" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="201" priority="274" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="310" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="200" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="309" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="199" priority="272" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="308" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="198" priority="271" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="307" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="197" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="306" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="196" priority="269" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="305" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="195" priority="268" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="304" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="194" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="303" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="193" priority="266" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="302" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="192" priority="265" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="301" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="191" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="300" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="190" priority="263" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="299" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="189" priority="262" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="298" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="188" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="297" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="187" priority="260" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="296" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="186" priority="259" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="295" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="185" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="294" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="184" priority="257" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="293" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="183" priority="256" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="292" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="182" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="291" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="181" priority="254" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="290" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="180" priority="253" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="289" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="179" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="288" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="178" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="287" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="177" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="286" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="176" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="175" priority="245" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="174" priority="244" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="173" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="249" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="172" priority="212" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="248" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="171" priority="211" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="247" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="170" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="169" priority="242" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="168" priority="241" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="167" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="166" priority="239" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="165" priority="238" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="164" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="163" priority="236" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="162" priority="235" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="161" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="160" priority="233" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="159" priority="232" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="158" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="157" priority="230" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="156" priority="229" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="155" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="154" priority="227" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="153" priority="226" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="152" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="151" priority="224" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="150" priority="223" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="149" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="148" priority="221" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="147" priority="220" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="146" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="145" priority="218" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="144" priority="217" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="143" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="252" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="142" priority="215" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="251" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="141" priority="214" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="250" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="140" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="180" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="179" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="138" priority="142" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="178" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="137" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="210" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="136" priority="173" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="209" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="135" priority="172" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="208" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="134" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="207" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="133" priority="170" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="206" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="132" priority="169" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="205" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="131" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="130" priority="167" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="129" priority="166" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="128" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="127" priority="164" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="126" priority="163" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="125" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="198" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="124" priority="161" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="197" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="123" priority="160" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="196" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="122" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="195" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="121" priority="158" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="194" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="120" priority="157" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="193" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="119" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="192" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="118" priority="155" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="191" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="117" priority="154" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="190" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="116" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="189" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="115" priority="152" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="188" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="114" priority="151" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="187" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="113" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="112" priority="149" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="111" priority="148" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="110" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="183" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="109" priority="146" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="182" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="108" priority="145" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="181" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="104" priority="42" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="103" priority="41" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="102" priority="40" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="101" priority="72" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="100" priority="71" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="71" priority="108" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="70" priority="107" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="99" priority="70" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="69" priority="106" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="98" priority="69" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="97" priority="68" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="68" priority="105" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="67" priority="104" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="96" priority="67" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="66" priority="103" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="95" priority="66" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="94" priority="65" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="65" priority="102" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="64" priority="101" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="93" priority="64" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="63" priority="100" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="92" priority="63" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="91" priority="62" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="62" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="61" priority="98" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="90" priority="61" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="60" priority="97" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="89" priority="60" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="88" priority="59" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="59" priority="96" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="58" priority="95" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="87" priority="58" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="57" priority="94" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="86" priority="57" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="85" priority="56" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="56" priority="93" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="55" priority="92" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="84" priority="55" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="54" priority="91" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="83" priority="54" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="82" priority="53" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="53" priority="90" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="52" priority="89" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="81" priority="52" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="51" priority="88" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="80" priority="51" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="79" priority="50" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="50" priority="87" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="49" priority="86" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="78" priority="49" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="48" priority="85" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="77" priority="48" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="76" priority="47" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="47" priority="84" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="46" priority="83" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="75" priority="46" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="45" priority="82" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="74" priority="45" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="73" priority="44" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="cellIs" dxfId="44" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="43" priority="80" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="containsText" dxfId="72" priority="43" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C50">
+    <cfRule type="containsText" dxfId="42" priority="79" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="71" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="containsText" dxfId="69" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51:C52">
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="37" priority="2" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C52">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C52)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51:C52">
-    <cfRule type="containsText" dxfId="36" priority="1" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[S1] Surcharge des endpoints existants avec Neode
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8166783-D36E-AE40-AAFF-D691EF4AAD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE86182-1E43-2C47-962A-C00ACBBF34C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
   <si>
     <t>Tâche</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Surcharge des endpoints existants avec Neode</t>
+  </si>
+  <si>
+    <t>Création des endpoints /projects</t>
   </si>
 </sst>
 </file>
@@ -4356,11 +4359,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J53" sqref="J53"/>
+      <selection pane="topRight" activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5429,17 +5432,17 @@
         <v>66</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="D51" s="9">
         <v>4</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" ref="F51:F52" si="17">E51/D51</f>
-        <v>0</v>
+        <f t="shared" ref="F51:F53" si="17">E51/D51</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -5450,66 +5453,70 @@
         <v>67</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D52" s="9">
         <v>2</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F53" s="8"/>
+      <c r="A53" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D53" s="9">
+        <v>4</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" s="8">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="2">
-        <v>15</v>
-      </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="8">
-        <f t="shared" ref="F54:F56" si="18">E54/D54</f>
-        <v>0</v>
-      </c>
+      <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D55" s="2">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="F55:F57" si="18">E55/D55</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D56" s="2">
-        <v>50</v>
+        <v>175</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="8">
@@ -5517,1799 +5524,1636 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="10"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="18"/>
-      <c r="H57"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" s="2"/>
+      <c r="C57" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="2">
+        <v>50</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="8">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="58" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
-      <c r="B58" s="12"/>
-      <c r="C58" s="13" t="s">
+    <row r="58" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="10"/>
+      <c r="B58" s="17"/>
+      <c r="C58" s="17"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="18"/>
+      <c r="H58"/>
+    </row>
+    <row r="59" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="14">
-        <f>SUM(D2:D57)</f>
-        <v>459</v>
-      </c>
-      <c r="E58" s="14">
-        <f>SUM(E2:E57)</f>
-        <v>188.5</v>
-      </c>
-      <c r="F58" s="15">
-        <f>E58/D58</f>
-        <v>0.41067538126361658</v>
+      <c r="D59" s="14">
+        <f>SUM(D2:D58)</f>
+        <v>463</v>
+      </c>
+      <c r="E59" s="14">
+        <f>SUM(E2:E58)</f>
+        <v>192.5</v>
+      </c>
+      <c r="F59" s="15">
+        <f>E59/D59</f>
+        <v>0.41576673866090713</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H59" s="1"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H60" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F56" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F57" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B57:F57"/>
+    <mergeCell ref="B58:F58"/>
   </mergeCells>
-  <conditionalFormatting sqref="C59:C1048576 C1:C7 C11:C13 C9 C54:C56">
-    <cfRule type="cellIs" dxfId="353" priority="674" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58:C1048576 C1:C7 C11:C13 C9 C54:C56">
-    <cfRule type="containsText" dxfId="352" priority="672" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C60:C1048576 C1:C7 C11:C13 C9 C55:C57">
+    <cfRule type="cellIs" dxfId="353" priority="677" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:C1048576 C1:C7 C11:C13 C9 C55:C57">
+    <cfRule type="containsText" dxfId="352" priority="675" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C54:C1048576">
-    <cfRule type="containsText" dxfId="351" priority="671" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C55:C1048576">
+    <cfRule type="containsText" dxfId="351" priority="674" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="350" priority="666" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="669" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="349" priority="665" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="668" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="348" priority="664" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="667" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="347" priority="654" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="657" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="346" priority="653" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="656" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="345" priority="652" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="655" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="344" priority="645" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="648" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="343" priority="644" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="647" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="342" priority="643" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="646" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="341" priority="642" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="645" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="340" priority="641" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="644" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="339" priority="640" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="643" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="338" priority="621" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="624" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="337" priority="620" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="623" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="336" priority="619" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="622" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="335" priority="612" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="615" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="334" priority="611" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="614" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="333" priority="610" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="613" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="332" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="594" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="331" priority="590" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="593" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="330" priority="589" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="592" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="329" priority="588" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="591" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="328" priority="587" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="590" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="327" priority="586" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="589" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="326" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="576" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="325" priority="572" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="575" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="324" priority="571" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="574" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="323" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="573" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="322" priority="569" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="572" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="321" priority="568" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="571" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="320" priority="567" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="319" priority="566" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="318" priority="565" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="317" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="567" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="316" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="566" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="315" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="565" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="314" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="313" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="312" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="311" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="310" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="309" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="308" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="307" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="306" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="305" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="304" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="303" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="302" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="301" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="300" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="299" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="298" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="297" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="296" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="295" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="294" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="293" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="292" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="291" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="290" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="289" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="288" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="287" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="286" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="285" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="284" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="283" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="282" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="281" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="531" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="280" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="530" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="279" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="529" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="278" priority="525" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="528" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="277" priority="524" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="527" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="276" priority="523" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="526" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="275" priority="522" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="525" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="274" priority="521" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="524" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="273" priority="520" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="523" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="272" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="522" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="271" priority="518" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="521" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="270" priority="517" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="520" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="269" priority="516" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="519" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="268" priority="515" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="518" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="267" priority="514" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="517" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="266" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="516" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="265" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="515" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="264" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="514" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="263" priority="510" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="513" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="262" priority="509" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="512" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="261" priority="508" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="511" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="260" priority="507" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="510" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="259" priority="506" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="509" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="258" priority="505" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="508" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="257" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="507" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="256" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="506" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="255" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="505" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="254" priority="501" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="504" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="253" priority="500" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="503" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="252" priority="499" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="502" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="251" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="501" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="250" priority="497" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="500" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="249" priority="496" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="499" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="248" priority="462" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="247" priority="461" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="246" priority="460" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="245" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="495" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="244" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="494" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="243" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="493" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="242" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="492" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="241" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="491" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="240" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="490" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="239" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="489" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="238" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="488" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="237" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="487" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="236" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="486" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="235" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="485" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="234" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="484" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="233" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="483" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="232" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="482" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="231" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="481" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="230" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="480" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="229" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="479" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="228" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="478" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="227" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="477" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="226" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="476" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="225" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="475" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="224" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="474" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="223" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="473" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="222" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="472" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="221" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="471" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="220" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="470" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="219" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="469" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="218" priority="465" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="468" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="217" priority="464" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="467" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="216" priority="463" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="466" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="215" priority="459" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="214" priority="458" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="213" priority="457" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="212" priority="456" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="211" priority="455" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="458" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="210" priority="454" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="457" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="209" priority="390" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="393" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="208" priority="389" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="392" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="207" priority="388" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="391" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="206" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="423" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="205" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="204" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="203" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="202" priority="416" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="201" priority="415" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="200" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="417" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="199" priority="413" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="198" priority="412" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="197" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="414" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="196" priority="410" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="195" priority="409" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="194" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="411" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="193" priority="407" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="192" priority="406" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="191" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="408" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="190" priority="404" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="189" priority="403" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="188" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="405" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="187" priority="401" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="186" priority="400" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="185" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="402" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="184" priority="398" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="183" priority="397" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="182" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="399" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="181" priority="395" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="180" priority="394" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="179" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="396" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="178" priority="392" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="395" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="177" priority="391" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="394" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="176" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="288" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="175" priority="284" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="287" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="174" priority="283" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="286" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="173" priority="315" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="318" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="172" priority="314" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="317" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="171" priority="313" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="316" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="170" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="315" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="169" priority="311" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="314" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="168" priority="310" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="313" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="167" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="312" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="166" priority="308" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="311" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="165" priority="307" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="310" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="164" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="309" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="163" priority="305" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="308" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="162" priority="304" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="307" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="161" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="306" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="160" priority="302" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="305" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="159" priority="301" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="304" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="158" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="303" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="157" priority="299" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="302" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="156" priority="298" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="301" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="155" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="300" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="154" priority="296" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="299" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="153" priority="295" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="298" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="152" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="297" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="151" priority="293" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="296" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="150" priority="292" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="295" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="149" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="294" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="148" priority="290" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="293" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="147" priority="289" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="292" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="146" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="291" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="145" priority="287" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="290" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="144" priority="286" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="289" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="143" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="285" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="142" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="284" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="141" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="283" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="140" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="252" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="139" priority="248" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="251" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="138" priority="247" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="250" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="137" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="136" priority="278" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="135" priority="277" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="134" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="133" priority="275" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="132" priority="274" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="131" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="130" priority="272" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="129" priority="271" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="128" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="127" priority="269" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="126" priority="268" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="125" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="124" priority="266" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="123" priority="265" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="122" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="121" priority="263" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="120" priority="262" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="119" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="118" priority="260" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="117" priority="259" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="116" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="115" priority="257" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="114" priority="256" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="113" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="112" priority="254" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="111" priority="253" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="110" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="109" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="108" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="107" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="183" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="106" priority="179" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="182" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="105" priority="178" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="181" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="104" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="213" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="103" priority="209" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="212" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="102" priority="208" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="211" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="101" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="210" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="100" priority="206" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="209" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="99" priority="205" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="208" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="98" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="207" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="97" priority="203" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="206" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="96" priority="202" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="205" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="95" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="94" priority="200" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="93" priority="199" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="92" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="91" priority="197" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="90" priority="196" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="89" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="198" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="88" priority="194" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="197" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="87" priority="193" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="196" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="86" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="195" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="85" priority="191" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="194" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="84" priority="190" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="193" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="83" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="192" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="82" priority="188" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="191" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="81" priority="187" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="190" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="80" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="189" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="79" priority="185" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="188" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="78" priority="184" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="187" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="77" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="76" priority="182" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="75" priority="181" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="74" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="72" priority="79" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="71" priority="108" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="70" priority="107" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="71" priority="111" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="70" priority="110" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="69" priority="106" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="69" priority="109" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="68" priority="105" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="67" priority="104" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="68" priority="108" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="67" priority="107" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="66" priority="103" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="66" priority="106" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="65" priority="102" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="64" priority="101" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="65" priority="105" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="64" priority="104" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="63" priority="100" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="63" priority="103" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="62" priority="99" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="61" priority="98" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="62" priority="102" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="61" priority="101" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="60" priority="97" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="60" priority="100" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="59" priority="96" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="58" priority="95" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="59" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="58" priority="98" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="57" priority="94" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="57" priority="97" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="56" priority="93" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="55" priority="92" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="56" priority="96" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="55" priority="95" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="54" priority="91" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="54" priority="94" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="53" priority="90" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="52" priority="89" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="53" priority="93" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="52" priority="92" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="51" priority="88" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="51" priority="91" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="50" priority="87" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="49" priority="86" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="50" priority="90" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="49" priority="89" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="48" priority="85" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="48" priority="88" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="47" priority="84" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="46" priority="83" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="47" priority="87" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="46" priority="86" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="45" priority="82" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="45" priority="85" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="cellIs" dxfId="44" priority="81" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="43" priority="80" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="cellIs" dxfId="44" priority="84" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="43" priority="83" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C50">
-    <cfRule type="containsText" dxfId="42" priority="79" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C52">
+    <cfRule type="containsText" dxfId="42" priority="82" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C52)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C51)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C51)))</formula>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54:C1048576 C1:C52" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C55:C1048576 C1:C53" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[S1] Création des endpoints de relations (Neo4j)
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE86182-1E43-2C47-962A-C00ACBBF34C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79431EA6-70F3-FB44-ADDE-9737B198A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$58</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="70">
   <si>
     <t>Tâche</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Création des endpoints /projects</t>
+  </si>
+  <si>
+    <t>Création des endpoints /teams</t>
   </si>
 </sst>
 </file>
@@ -508,337 +511,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="354">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="321">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4359,11 +4032,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N51" sqref="N51"/>
+      <selection pane="topRight" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5480,1680 +5153,1716 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F54" s="8"/>
+      <c r="A54" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="9">
+        <v>4</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" s="8">
+        <f t="shared" ref="F54" si="18">E54/D54</f>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D55" s="2">
-        <v>15</v>
-      </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="8">
-        <f t="shared" ref="F55:F57" si="18">E55/D55</f>
-        <v>0</v>
-      </c>
+      <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D56" s="2">
-        <v>175</v>
+        <v>15</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="F56:F58" si="19">E56/D56</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D57" s="2">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="8">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
-      <c r="D58" s="17"/>
-      <c r="E58" s="17"/>
-      <c r="F58" s="18"/>
-      <c r="H58"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="2">
+        <v>50</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="59" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
-      <c r="B59" s="12"/>
-      <c r="C59" s="13" t="s">
+    <row r="59" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="10"/>
+      <c r="B59" s="17"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="18"/>
+      <c r="H59"/>
+    </row>
+    <row r="60" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="14">
-        <f>SUM(D2:D58)</f>
-        <v>463</v>
-      </c>
-      <c r="E59" s="14">
-        <f>SUM(E2:E58)</f>
-        <v>192.5</v>
-      </c>
-      <c r="F59" s="15">
-        <f>E59/D59</f>
-        <v>0.41576673866090713</v>
+      <c r="D60" s="14">
+        <f>SUM(D2:D59)</f>
+        <v>452</v>
+      </c>
+      <c r="E60" s="14">
+        <f>SUM(E2:E59)</f>
+        <v>194.5</v>
+      </c>
+      <c r="F60" s="15">
+        <f>E60/D60</f>
+        <v>0.43030973451327431</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H60" s="1"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H61" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F57" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F58" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B58:F58"/>
+    <mergeCell ref="B59:F59"/>
   </mergeCells>
-  <conditionalFormatting sqref="C60:C1048576 C1:C7 C11:C13 C9 C55:C57">
-    <cfRule type="cellIs" dxfId="353" priority="677" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59:C1048576 C1:C7 C11:C13 C9 C55:C57">
-    <cfRule type="containsText" dxfId="352" priority="675" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C61:C1048576 C1:C7 C11:C13 C9 C56:C58">
+    <cfRule type="cellIs" dxfId="320" priority="680" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60:C1048576 C1:C7 C11:C13 C9 C56:C58">
+    <cfRule type="containsText" dxfId="319" priority="678" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C55:C1048576">
-    <cfRule type="containsText" dxfId="351" priority="674" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C56:C1048576">
+    <cfRule type="containsText" dxfId="318" priority="677" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="350" priority="669" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="672" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="349" priority="668" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="671" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="348" priority="667" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="670" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="347" priority="657" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="660" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="346" priority="656" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="659" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="345" priority="655" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="658" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="344" priority="648" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="651" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="343" priority="647" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="650" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="342" priority="646" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="649" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="341" priority="645" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="648" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="340" priority="644" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="647" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="339" priority="643" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="646" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="338" priority="624" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="337" priority="623" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="336" priority="622" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="335" priority="615" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="334" priority="614" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="333" priority="613" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="332" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="597" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="331" priority="593" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="596" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="330" priority="592" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="595" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="329" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="594" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="328" priority="590" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="593" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="327" priority="589" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="592" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="326" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="579" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="325" priority="575" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="578" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="324" priority="574" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="577" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="323" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="576" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="322" priority="572" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="575" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="321" priority="571" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="574" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="320" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="573" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="319" priority="569" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="572" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="318" priority="568" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="571" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="317" priority="567" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="316" priority="566" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="315" priority="565" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="314" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="567" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="313" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="566" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="312" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="565" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="311" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="310" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="309" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="308" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="307" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="306" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="305" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="304" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="303" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="302" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="301" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="300" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="299" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="298" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="297" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="296" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="295" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="294" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="293" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="292" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="291" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="290" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="289" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="288" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="287" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="286" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="285" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="284" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="283" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="282" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="281" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="280" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="279" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="278" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="531" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="277" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="530" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="276" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="529" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="275" priority="525" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="528" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="274" priority="524" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="527" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="273" priority="523" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="526" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="272" priority="522" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="525" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="271" priority="521" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="524" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="270" priority="520" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="523" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="269" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="522" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="268" priority="518" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="521" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="267" priority="517" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="520" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="266" priority="516" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="519" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="265" priority="515" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="518" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="264" priority="514" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="517" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="263" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="516" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="262" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="515" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="261" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="514" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="260" priority="510" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="513" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="259" priority="509" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="512" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="258" priority="508" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="511" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="257" priority="507" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="510" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="256" priority="506" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="509" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="255" priority="505" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="508" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="254" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="507" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="253" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="506" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="252" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="505" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="251" priority="501" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="504" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="250" priority="500" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="503" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="249" priority="499" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="502" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="248" priority="465" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="468" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="247" priority="464" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="467" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="246" priority="463" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="466" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="245" priority="495" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="498" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="244" priority="494" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="497" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="243" priority="493" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="496" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="242" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="495" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="241" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="494" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="240" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="493" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="239" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="492" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="238" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="491" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="237" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="490" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="236" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="489" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="235" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="488" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="234" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="487" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="233" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="486" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="232" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="485" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="231" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="484" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="230" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="483" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="229" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="482" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="228" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="481" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="227" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="480" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="226" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="479" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="225" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="478" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="224" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="477" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="223" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="476" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="222" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="475" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="221" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="474" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="220" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="473" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="219" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="472" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="218" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="471" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="217" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="470" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="216" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="469" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="215" priority="462" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="214" priority="461" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="213" priority="460" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="212" priority="459" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="211" priority="458" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="210" priority="457" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="209" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="396" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="208" priority="392" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="395" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="207" priority="391" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="394" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="206" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="426" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="205" priority="422" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="425" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="204" priority="421" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="424" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="203" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="423" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="202" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="201" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="200" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="199" priority="416" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="198" priority="415" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="197" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="417" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="196" priority="413" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="195" priority="412" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="194" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="414" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="193" priority="410" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="192" priority="409" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="191" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="411" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="190" priority="407" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="189" priority="406" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="188" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="408" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="187" priority="404" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="186" priority="403" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="185" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="405" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="184" priority="401" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="183" priority="400" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="182" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="402" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="181" priority="398" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="180" priority="397" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="179" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="399" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="178" priority="395" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="177" priority="394" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="176" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="291" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="175" priority="287" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="290" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="174" priority="286" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="289" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="173" priority="318" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="321" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="172" priority="317" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="320" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="171" priority="316" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="319" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="170" priority="315" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="318" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="169" priority="314" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="317" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="168" priority="313" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="316" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="167" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="315" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="166" priority="311" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="314" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="165" priority="310" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="313" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="164" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="312" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="163" priority="308" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="311" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="162" priority="307" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="310" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="161" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="309" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="160" priority="305" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="308" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="159" priority="304" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="307" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="158" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="306" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="157" priority="302" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="305" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="156" priority="301" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="304" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="155" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="303" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="154" priority="299" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="302" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="153" priority="298" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="301" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="152" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="300" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="151" priority="296" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="299" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="150" priority="295" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="298" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="149" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="297" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="148" priority="293" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="296" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="147" priority="292" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="295" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="146" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="294" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="145" priority="290" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="293" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="144" priority="289" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="292" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="143" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="288" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="142" priority="284" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="287" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="141" priority="283" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="286" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="140" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="139" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="138" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="137" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="285" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="136" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="284" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="135" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="283" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="134" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="133" priority="278" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="132" priority="277" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="131" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="130" priority="275" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="129" priority="274" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="128" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="127" priority="272" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="126" priority="271" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="125" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="124" priority="269" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="123" priority="268" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="122" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="121" priority="266" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="120" priority="265" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="119" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="118" priority="263" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="117" priority="262" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="116" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="115" priority="260" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="114" priority="259" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="113" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="112" priority="257" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="111" priority="256" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="110" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="109" priority="254" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="108" priority="253" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="107" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="106" priority="182" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="73" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="105" priority="181" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="72" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="104" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="216" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="103" priority="212" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="70" priority="215" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="102" priority="211" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="69" priority="214" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="101" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="213" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="100" priority="209" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="67" priority="212" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="99" priority="208" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="66" priority="211" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="98" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="210" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="97" priority="206" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="64" priority="209" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="96" priority="205" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="63" priority="208" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="95" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="207" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="94" priority="203" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="61" priority="206" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="93" priority="202" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="60" priority="205" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="92" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="91" priority="200" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="58" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="90" priority="199" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="57" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="89" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="88" priority="197" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="55" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="87" priority="196" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="54" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="86" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="198" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="85" priority="194" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="52" priority="197" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="84" priority="193" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="51" priority="196" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="83" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="195" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="82" priority="191" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="49" priority="194" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="81" priority="190" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="48" priority="193" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="80" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="192" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="79" priority="188" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="46" priority="191" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="78" priority="187" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="45" priority="190" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="77" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="189" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="76" priority="185" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="43" priority="188" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="75" priority="184" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="42" priority="187" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="74" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="84" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="40" priority="83" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="72" priority="79" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="39" priority="82" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="71" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="114" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="70" priority="110" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="37" priority="113" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="69" priority="109" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="36" priority="112" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="68" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="111" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="67" priority="107" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="34" priority="110" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="66" priority="106" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="33" priority="109" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="65" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="108" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="64" priority="104" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="31" priority="107" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="63" priority="103" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="30" priority="106" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="62" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="105" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="61" priority="101" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="28" priority="104" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="60" priority="100" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="27" priority="103" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="59" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="102" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="58" priority="98" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="25" priority="101" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="57" priority="97" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="24" priority="100" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="56" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="99" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="55" priority="95" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="22" priority="98" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="54" priority="94" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="21" priority="97" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="53" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="96" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="52" priority="92" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="19" priority="95" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="51" priority="91" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="18" priority="94" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="50" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="93" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="49" priority="89" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="16" priority="92" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="48" priority="88" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="15" priority="91" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="47" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="90" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="46" priority="86" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="13" priority="89" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="45" priority="85" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="12" priority="88" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="44" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="87" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="43" priority="83" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="10" priority="86" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="42" priority="82" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="9" priority="85" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C53)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
+  <conditionalFormatting sqref="C54">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C55:C1048576 C1:C53" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C56:C1048576 C1:C54" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[S1] Création des endpoints /teams
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79431EA6-70F3-FB44-ADDE-9737B198A435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF20C535-A5E8-9542-8DAA-68E63C97DEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -511,7 +511,307 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="321">
+  <dxfs count="351">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4036,7 +4336,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H57" sqref="H57"/>
+      <selection pane="topRight" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5108,14 +5408,14 @@
         <v>2</v>
       </c>
       <c r="D51" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F51" s="8">
         <f t="shared" ref="F51:F53" si="17">E51/D51</f>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -5129,10 +5429,10 @@
         <v>2</v>
       </c>
       <c r="D52" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E52">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F52" s="8">
         <f t="shared" si="17"/>
@@ -5153,11 +5453,11 @@
         <v>4</v>
       </c>
       <c r="E53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" si="17"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -5168,17 +5468,17 @@
         <v>69</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D54" s="9">
         <v>4</v>
       </c>
       <c r="E54">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F54" s="8">
         <f t="shared" ref="F54" si="18">E54/D54</f>
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -5256,11 +5556,11 @@
       </c>
       <c r="E60" s="14">
         <f>SUM(E2:E59)</f>
-        <v>194.5</v>
+        <v>200.5</v>
       </c>
       <c r="F60" s="15">
         <f>E60/D60</f>
-        <v>0.43030973451327431</v>
+        <v>0.44358407079646017</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -5272,1592 +5572,1742 @@
     <mergeCell ref="B59:F59"/>
   </mergeCells>
   <conditionalFormatting sqref="C61:C1048576 C1:C7 C11:C13 C9 C56:C58">
-    <cfRule type="cellIs" dxfId="320" priority="680" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="713" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60:C1048576 C1:C7 C11:C13 C9 C56:C58">
-    <cfRule type="containsText" dxfId="319" priority="678" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="711" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C11:C13 C9 C56:C1048576">
-    <cfRule type="containsText" dxfId="318" priority="677" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="710" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="317" priority="672" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="705" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="316" priority="671" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="704" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="315" priority="670" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="703" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="314" priority="660" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="693" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="313" priority="659" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="692" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="312" priority="658" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="691" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="311" priority="651" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="684" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="310" priority="650" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="683" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="309" priority="649" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="682" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="308" priority="648" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="681" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="307" priority="647" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="680" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="306" priority="646" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="679" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="305" priority="627" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="660" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="304" priority="626" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="659" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="303" priority="625" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="658" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="302" priority="618" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="651" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="301" priority="617" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="650" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="300" priority="616" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="649" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="299" priority="597" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="298" priority="596" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="297" priority="595" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="296" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="295" priority="593" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="294" priority="592" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="293" priority="579" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="612" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="292" priority="578" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="611" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="291" priority="577" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="610" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="290" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="609" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="289" priority="575" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="608" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="288" priority="574" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="607" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="287" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="606" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="286" priority="572" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="605" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="285" priority="571" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="604" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="284" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="603" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="283" priority="569" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="602" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="282" priority="568" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="601" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="281" priority="567" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="600" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="280" priority="566" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="599" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="279" priority="565" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="598" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="278" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="597" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="277" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="596" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="276" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="595" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="275" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="594" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="274" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="593" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="273" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="592" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="272" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="591" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="271" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="590" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="270" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="589" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="269" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="588" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="268" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="587" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="267" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="586" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="266" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="585" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="265" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="584" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="264" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="583" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="263" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="582" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="262" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="581" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="261" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="580" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="260" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="579" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="259" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="578" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="258" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="577" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="257" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="576" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="256" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="575" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="255" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="574" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="254" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="573" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="253" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="572" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="252" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="571" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="251" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="250" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="249" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="248" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="567" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="247" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="566" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="246" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="565" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="245" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="244" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="243" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="242" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="241" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="240" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="239" priority="525" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="238" priority="524" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="237" priority="523" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="236" priority="522" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="235" priority="521" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="234" priority="520" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="233" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="232" priority="518" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="231" priority="517" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="230" priority="516" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="229" priority="515" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="228" priority="514" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="227" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="226" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="225" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="224" priority="510" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="223" priority="509" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="222" priority="508" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="221" priority="507" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="220" priority="506" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="219" priority="505" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="218" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="217" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="216" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="215" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="501" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="214" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="500" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="213" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="499" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="242" priority="531" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="241" priority="530" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="240" priority="529" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="239" priority="528" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="238" priority="527" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="237" priority="526" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="236" priority="525" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="235" priority="524" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="234" priority="523" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="233" priority="522" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="232" priority="521" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="231" priority="520" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="230" priority="519" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="229" priority="518" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="228" priority="517" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="227" priority="516" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="226" priority="515" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="225" priority="514" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="224" priority="513" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="223" priority="512" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="222" priority="511" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="221" priority="510" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="220" priority="509" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="219" priority="508" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="218" priority="507" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="217" priority="506" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="216" priority="505" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="215" priority="504" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="214" priority="503" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="213" priority="502" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="212" priority="498" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="211" priority="497" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+      <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="210" priority="496" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+      <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="cellIs" dxfId="209" priority="495" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+  <conditionalFormatting sqref="C44">
     <cfRule type="containsText" dxfId="208" priority="494" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+      <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="containsText" dxfId="207" priority="493" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="206" priority="492" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="205" priority="491" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="204" priority="490" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="203" priority="489" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="202" priority="488" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="201" priority="487" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="200" priority="486" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="199" priority="485" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="198" priority="484" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="197" priority="483" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="196" priority="482" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="195" priority="481" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="194" priority="480" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="193" priority="479" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="192" priority="478" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="191" priority="477" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="190" priority="476" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="189" priority="475" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="188" priority="474" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="187" priority="473" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="186" priority="472" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="185" priority="471" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="184" priority="470" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="183" priority="469" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="182" priority="465" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="181" priority="464" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="180" priority="463" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="179" priority="462" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="178" priority="461" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="177" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="176" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="429" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="175" priority="395" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="428" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="174" priority="394" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="427" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="173" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="172" priority="425" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="458" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="171" priority="424" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="457" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="170" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="169" priority="422" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="455" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="168" priority="421" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="454" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="167" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="453" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="166" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="452" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="165" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="451" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="164" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="450" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="163" priority="416" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="449" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="162" priority="415" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="448" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="161" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="447" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="160" priority="413" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="446" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="159" priority="412" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="445" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="158" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="444" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="157" priority="410" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="443" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="156" priority="409" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="442" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="155" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="441" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="154" priority="407" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="440" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="153" priority="406" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="439" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="152" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="438" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="151" priority="404" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="437" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="150" priority="403" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="436" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="149" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="435" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="148" priority="401" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="434" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="147" priority="400" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="433" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="146" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="432" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="145" priority="398" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="431" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="144" priority="397" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="430" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="143" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="324" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="142" priority="290" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="323" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="141" priority="289" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="322" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="170" priority="354" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="169" priority="353" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="168" priority="352" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="167" priority="351" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="166" priority="350" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="165" priority="349" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="164" priority="348" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="163" priority="347" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="162" priority="346" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="161" priority="345" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="160" priority="344" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="159" priority="343" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="158" priority="342" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="157" priority="341" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="156" priority="340" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="155" priority="339" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="154" priority="338" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="153" priority="337" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="152" priority="336" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="151" priority="335" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="150" priority="334" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="149" priority="333" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="148" priority="332" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="147" priority="331" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="146" priority="330" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="145" priority="329" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="144" priority="328" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="143" priority="327" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="142" priority="326" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="141" priority="325" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="cellIs" dxfId="140" priority="321" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+  <conditionalFormatting sqref="C48">
     <cfRule type="containsText" dxfId="139" priority="320" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="containsText" dxfId="138" priority="319" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="137" priority="318" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="136" priority="317" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="135" priority="316" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="134" priority="315" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="133" priority="314" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="132" priority="313" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="131" priority="312" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="130" priority="311" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="129" priority="310" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="128" priority="309" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="127" priority="308" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="126" priority="307" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="125" priority="306" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="124" priority="305" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="123" priority="304" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="122" priority="303" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="121" priority="302" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="120" priority="301" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="119" priority="300" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="118" priority="299" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="117" priority="298" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="116" priority="297" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="115" priority="296" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="114" priority="295" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="113" priority="294" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="112" priority="293" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="111" priority="292" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="110" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="288" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="109" priority="287" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="287" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="108" priority="286" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="286" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="107" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="318" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="106" priority="254" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="317" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="105" priority="253" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="316" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="104" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="315" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="103" priority="284" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="314" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="102" priority="283" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="313" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="101" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="312" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="100" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="311" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="99" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="310" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="98" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="309" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="97" priority="278" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="308" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="96" priority="277" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="307" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="95" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="306" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="94" priority="275" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="305" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="93" priority="274" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="304" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="92" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="303" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="91" priority="272" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="302" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="90" priority="271" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="301" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="89" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="300" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="88" priority="269" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="299" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="87" priority="268" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="298" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="86" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="297" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="85" priority="266" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="296" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="84" priority="265" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="295" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="83" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="294" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="82" priority="263" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="293" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="81" priority="262" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="292" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="80" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="291" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="79" priority="260" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="290" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="78" priority="259" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="289" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="77" priority="258" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="76" priority="257" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="75" priority="256" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="74" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="219" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="73" priority="185" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="218" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="72" priority="184" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="217" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="71" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="249" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="70" priority="215" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="248" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="69" priority="214" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="247" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="68" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="246" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="67" priority="212" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="245" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="66" priority="211" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="244" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="65" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="243" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="64" priority="209" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="242" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="63" priority="208" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="241" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="62" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="240" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="61" priority="206" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="239" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="60" priority="205" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="238" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="59" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="237" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="58" priority="203" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="236" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="57" priority="202" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="235" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="56" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="234" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="55" priority="200" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="233" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="54" priority="199" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="232" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="53" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="231" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="52" priority="197" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="230" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="51" priority="196" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="229" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="50" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="228" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="49" priority="194" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="227" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="48" priority="193" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="226" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="47" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="225" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="46" priority="191" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="224" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="45" priority="190" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="223" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="44" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="222" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="43" priority="188" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="73" priority="221" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="42" priority="187" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="72" priority="220" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="41" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="117" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="40" priority="83" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="70" priority="116" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="39" priority="82" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="69" priority="115" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="38" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="147" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="37" priority="113" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="67" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="36" priority="112" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="66" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="35" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="144" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="34" priority="110" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="64" priority="143" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="33" priority="109" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="63" priority="142" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="32" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="141" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="31" priority="107" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="61" priority="140" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="30" priority="106" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="60" priority="139" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="29" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="138" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="28" priority="104" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="58" priority="137" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="27" priority="103" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="57" priority="136" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="26" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="135" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="25" priority="101" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="55" priority="134" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="24" priority="100" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="54" priority="133" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="23" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="132" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="22" priority="98" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="52" priority="131" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="21" priority="97" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="51" priority="130" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="20" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="129" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="19" priority="95" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="49" priority="128" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="18" priority="94" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="48" priority="127" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="17" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="126" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="16" priority="92" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="46" priority="125" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="15" priority="91" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="45" priority="124" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="14" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="123" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="13" priority="89" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="43" priority="122" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="12" priority="88" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="42" priority="121" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="11" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="120" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="10" priority="86" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="40" priority="119" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="9" priority="85" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="39" priority="118" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Generation de donnes avec Faker
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF20C535-A5E8-9542-8DAA-68E63C97DEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B445F53D-A54A-E440-A314-6D187B2EB4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$59</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="71">
   <si>
     <t>Tâche</t>
   </si>
@@ -248,12 +248,15 @@
   <si>
     <t>Création des endpoints /teams</t>
   </si>
+  <si>
+    <t>Générations de données a l'aide de Faker</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -293,8 +296,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +321,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -470,7 +486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -506,12 +522,673 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="351">
+  <dxfs count="417">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4334,9 +5011,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
   <dimension ref="A1:H61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G56" sqref="G56"/>
+      <selection pane="topRight" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5414,7 +6091,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" ref="F51:F53" si="17">E51/D51</f>
+        <f t="shared" ref="F51:F55" si="17">E51/D51</f>
         <v>1.5</v>
       </c>
     </row>
@@ -5482,52 +6159,56 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F55" s="8"/>
+      <c r="A55" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D55" s="9">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>3</v>
+      </c>
+      <c r="F55" s="8">
+        <f t="shared" si="17"/>
+        <v>0.75</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D56" s="2">
-        <v>15</v>
-      </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="8">
-        <f t="shared" ref="F56:F58" si="19">E56/D56</f>
-        <v>0</v>
-      </c>
+      <c r="F56" s="8"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D57" s="2">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="F57:F59" si="19">E57/D57</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D58" s="2">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="E58" s="2"/>
       <c r="F58" s="8">
@@ -5536,1783 +6217,1798 @@
       </c>
     </row>
     <row r="59" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="10"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="17"/>
-      <c r="D59" s="17"/>
-      <c r="E59" s="17"/>
-      <c r="F59" s="18"/>
+      <c r="A59" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="2">
+        <v>50</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
       <c r="H59"/>
     </row>
-    <row r="60" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="12"/>
-      <c r="C60" s="13" t="s">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="10"/>
+      <c r="B60" s="17"/>
+      <c r="C60" s="17"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="18"/>
+    </row>
+    <row r="61" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D60" s="14">
-        <f>SUM(D2:D59)</f>
-        <v>452</v>
-      </c>
-      <c r="E60" s="14">
-        <f>SUM(E2:E59)</f>
-        <v>200.5</v>
-      </c>
-      <c r="F60" s="15">
-        <f>E60/D60</f>
-        <v>0.44358407079646017</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D61" s="14">
+        <f>SUM(D2:D60)</f>
+        <v>456</v>
+      </c>
+      <c r="E61" s="14">
+        <f>SUM(E2:E60)</f>
+        <v>203.5</v>
+      </c>
+      <c r="F61" s="15">
+        <f>E61/D61</f>
+        <v>0.44627192982456143</v>
+      </c>
       <c r="H61" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F58" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F59" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B59:F59"/>
+    <mergeCell ref="B60:F60"/>
   </mergeCells>
-  <conditionalFormatting sqref="C61:C1048576 C1:C7 C11:C13 C9 C56:C58">
-    <cfRule type="cellIs" dxfId="350" priority="713" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C1048576 C1:C7 C11:C13 C9 C56:C58">
-    <cfRule type="containsText" dxfId="349" priority="711" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C62:C1048576 C1:C7 C11:C13 C9 C57:C59">
+    <cfRule type="cellIs" dxfId="416" priority="746" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61:C1048576 C1:C7 C11:C13 C9 C57:C59">
+    <cfRule type="containsText" dxfId="415" priority="744" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C56:C1048576">
-    <cfRule type="containsText" dxfId="348" priority="710" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C57:C1048576">
+    <cfRule type="containsText" dxfId="414" priority="743" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="347" priority="705" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="738" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="346" priority="704" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="412" priority="737" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="345" priority="703" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="411" priority="736" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="344" priority="693" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="726" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="343" priority="692" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="409" priority="725" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="342" priority="691" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="408" priority="724" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="341" priority="684" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="717" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="340" priority="683" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="406" priority="716" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="339" priority="682" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="405" priority="715" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="338" priority="681" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="714" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="337" priority="680" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="403" priority="713" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="336" priority="679" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="402" priority="712" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="335" priority="660" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="693" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="334" priority="659" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="400" priority="692" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="333" priority="658" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="399" priority="691" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="332" priority="651" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="684" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="331" priority="650" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="397" priority="683" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="330" priority="649" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="396" priority="682" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="329" priority="630" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="663" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="328" priority="629" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="394" priority="662" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="327" priority="628" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="393" priority="661" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="326" priority="627" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="660" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="325" priority="626" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="391" priority="659" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="324" priority="625" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="390" priority="658" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="323" priority="612" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="645" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="322" priority="611" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="388" priority="644" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="321" priority="610" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="387" priority="643" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="320" priority="609" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="642" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="319" priority="608" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="385" priority="641" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="318" priority="607" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="384" priority="640" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="317" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="639" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="316" priority="605" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="638" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="315" priority="604" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="637" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="314" priority="603" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="636" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="313" priority="602" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="635" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="312" priority="601" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="634" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="311" priority="600" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="633" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="310" priority="599" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="632" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="309" priority="598" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="631" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="308" priority="597" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="307" priority="596" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="306" priority="595" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="305" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="304" priority="593" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="303" priority="592" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="302" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="624" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="301" priority="590" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="623" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="300" priority="589" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="622" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="299" priority="588" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="621" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="298" priority="587" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="620" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="297" priority="586" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="619" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="296" priority="585" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="295" priority="584" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="294" priority="583" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="293" priority="582" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="615" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="292" priority="581" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="358" priority="614" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="291" priority="580" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="357" priority="613" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="290" priority="579" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="612" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="289" priority="578" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="355" priority="611" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="288" priority="577" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="354" priority="610" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="287" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="609" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="286" priority="575" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="608" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="285" priority="574" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="607" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="284" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="606" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="283" priority="572" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="605" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="282" priority="571" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="604" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="281" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="603" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="280" priority="569" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="602" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="279" priority="568" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="601" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="278" priority="567" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="600" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="277" priority="566" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="599" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="276" priority="565" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="598" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="275" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="597" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="274" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="596" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="273" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="595" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="272" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="594" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="271" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="593" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="270" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="592" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="269" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="591" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="268" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="590" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="267" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="589" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="266" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="588" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="265" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="587" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="264" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="586" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="263" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="585" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="262" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="584" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="261" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="583" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="260" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="582" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="259" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="581" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="258" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="580" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="257" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="579" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="256" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="578" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="255" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="577" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="254" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="576" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="253" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="575" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="252" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="574" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="251" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="573" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="250" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="572" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="249" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="571" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="248" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="247" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="246" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="245" priority="501" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="244" priority="500" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="243" priority="499" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="242" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="241" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="240" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="239" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="238" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="237" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="236" priority="525" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="235" priority="524" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="234" priority="523" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="233" priority="522" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="232" priority="521" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="231" priority="520" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="230" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="229" priority="518" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="228" priority="517" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="227" priority="516" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="226" priority="515" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="225" priority="514" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="224" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="223" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="222" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="221" priority="510" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="220" priority="509" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="219" priority="508" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="218" priority="507" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="217" priority="506" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="216" priority="505" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="215" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="214" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="213" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="212" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="531" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="211" priority="497" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="530" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="210" priority="496" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="529" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="209" priority="495" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="528" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="208" priority="494" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="527" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="207" priority="493" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="526" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="206" priority="429" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="205" priority="428" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="204" priority="427" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="203" priority="459" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="492" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="202" priority="458" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="491" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="201" priority="457" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="490" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="200" priority="456" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="489" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="199" priority="455" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="488" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="198" priority="454" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="487" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="197" priority="453" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="486" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="196" priority="452" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="485" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="195" priority="451" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="484" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="194" priority="450" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="483" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="193" priority="449" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="482" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="192" priority="448" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="481" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="191" priority="447" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="480" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="190" priority="446" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="479" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="189" priority="445" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="478" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="188" priority="444" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="477" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="187" priority="443" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="476" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="186" priority="442" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="475" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="185" priority="441" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="474" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="184" priority="440" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="473" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="183" priority="439" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="472" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="182" priority="438" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="471" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="181" priority="437" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="470" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="180" priority="436" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="469" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="179" priority="435" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="468" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="178" priority="434" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="467" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="177" priority="433" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="466" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="176" priority="432" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="175" priority="431" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="174" priority="430" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="239" priority="357" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="238" priority="356" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="237" priority="355" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="236" priority="387" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="235" priority="386" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="234" priority="385" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="233" priority="384" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="232" priority="383" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="231" priority="382" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="230" priority="381" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="229" priority="380" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="228" priority="379" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="227" priority="378" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="226" priority="377" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="225" priority="376" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="224" priority="375" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="223" priority="374" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="222" priority="373" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="221" priority="372" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="220" priority="371" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="219" priority="370" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="218" priority="369" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="217" priority="368" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="216" priority="367" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="215" priority="366" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="214" priority="365" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="213" priority="364" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="212" priority="363" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="211" priority="362" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="210" priority="361" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="209" priority="360" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="208" priority="359" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="207" priority="358" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="206" priority="354" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="205" priority="353" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="204" priority="352" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="203" priority="321" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="202" priority="320" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="201" priority="319" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="200" priority="351" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="199" priority="350" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="198" priority="349" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="197" priority="348" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="196" priority="347" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="195" priority="346" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="194" priority="345" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="193" priority="344" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="192" priority="343" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="191" priority="342" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="190" priority="341" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="189" priority="340" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="188" priority="339" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="187" priority="338" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="186" priority="337" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="185" priority="336" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="184" priority="335" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="183" priority="334" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="182" priority="333" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="181" priority="332" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="180" priority="331" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="179" priority="330" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="178" priority="329" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="177" priority="328" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="176" priority="327" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="175" priority="326" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="174" priority="325" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="cellIs" dxfId="173" priority="324" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+  <conditionalFormatting sqref="C48">
     <cfRule type="containsText" dxfId="172" priority="323" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="containsText" dxfId="171" priority="322" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="170" priority="354" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="169" priority="353" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="168" priority="352" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="167" priority="351" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="166" priority="350" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="165" priority="349" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="164" priority="348" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="163" priority="347" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="162" priority="346" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="161" priority="345" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="160" priority="344" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="159" priority="343" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="158" priority="342" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="157" priority="341" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="156" priority="340" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="155" priority="339" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="154" priority="338" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="153" priority="337" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="152" priority="336" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="151" priority="335" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="150" priority="334" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="149" priority="333" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="148" priority="332" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="147" priority="331" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="146" priority="330" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="145" priority="329" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="144" priority="328" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="143" priority="327" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="142" priority="326" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="141" priority="325" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="140" priority="321" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="139" priority="320" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="138" priority="319" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="137" priority="288" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="136" priority="287" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="135" priority="286" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="134" priority="318" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="133" priority="317" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="132" priority="316" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="131" priority="315" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="130" priority="314" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="129" priority="313" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="128" priority="312" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="127" priority="311" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="126" priority="310" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="125" priority="309" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="124" priority="308" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="123" priority="307" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="122" priority="306" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="121" priority="305" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="120" priority="304" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="119" priority="303" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="118" priority="302" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="117" priority="301" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="116" priority="300" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="115" priority="299" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="114" priority="298" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="113" priority="297" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="112" priority="296" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="111" priority="295" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="110" priority="294" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="109" priority="293" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="108" priority="292" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="107" priority="291" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="106" priority="290" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="105" priority="289" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="104" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="252" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="103" priority="218" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="251" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="102" priority="217" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="250" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="101" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="100" priority="248" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="99" priority="247" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="98" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="97" priority="245" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="96" priority="244" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="95" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="94" priority="242" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="93" priority="241" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="92" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="91" priority="239" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="90" priority="238" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="89" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="88" priority="236" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="87" priority="235" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="86" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="85" priority="233" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="84" priority="232" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="83" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="82" priority="230" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="81" priority="229" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="80" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="79" priority="227" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="78" priority="226" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="77" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="76" priority="224" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="75" priority="223" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="74" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="73" priority="221" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="72" priority="220" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="71" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="150" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="70" priority="116" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="149" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="69" priority="115" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="148" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="68" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="180" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="67" priority="146" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="179" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="66" priority="145" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="178" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="65" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="177" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="64" priority="143" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="176" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="63" priority="142" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="175" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="62" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="174" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="61" priority="140" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="173" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="60" priority="139" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="172" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="59" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="171" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="58" priority="137" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="170" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="57" priority="136" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="169" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="56" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="168" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="55" priority="134" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="167" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="54" priority="133" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="166" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="53" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="165" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="52" priority="131" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="164" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="51" priority="130" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="163" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="50" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="162" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="49" priority="128" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="48" priority="127" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="47" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="159" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="46" priority="125" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="158" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="45" priority="124" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="157" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="44" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="156" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="43" priority="122" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="155" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="42" priority="121" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="154" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="41" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="153" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="40" priority="119" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="152" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="39" priority="118" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="151" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="71" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="36" priority="37" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="70" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C53)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="36" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="35" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="34" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="66" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="65" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="64" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="63" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="62" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="61" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="60" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="59" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="58" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="57" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="56" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="55" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="54" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="53" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="52" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="51" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="50" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="49" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="48" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="47" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="46" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="45" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="44" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="43" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="42" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="73" priority="41" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="72" priority="40" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="70" priority="38" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="69" priority="37" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C56:C1048576 C1:C54" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57:C1048576 C1:C54" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
[S1] Création des endpoints /projects
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B445F53D-A54A-E440-A314-6D187B2EB4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071129D8-2F64-754A-8C79-A8B84F782578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$61</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
   <si>
     <t>Tâche</t>
   </si>
@@ -251,12 +251,18 @@
   <si>
     <t>Générations de données a l'aide de Faker</t>
   </si>
+  <si>
+    <t>Création des endpoints restants</t>
+  </si>
+  <si>
+    <t>Rédaction de tests unitaires</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,15 +302,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,12 +320,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -486,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -522,13 +515,42 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="417">
+  <dxfs count="420">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5009,11 +5031,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H61"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D51" sqref="D51"/>
+      <selection pane="topRight" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6091,7 +6113,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" ref="F51:F55" si="17">E51/D51</f>
+        <f t="shared" ref="F51:F57" si="17">E51/D51</f>
         <v>1.5</v>
       </c>
     </row>
@@ -6124,17 +6146,17 @@
         <v>68</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D53" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -6165,8 +6187,8 @@
       <c r="B55" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="19" t="s">
-        <v>53</v>
+      <c r="C55" s="9" t="s">
+        <v>2</v>
       </c>
       <c r="D55" s="9">
         <v>4</v>
@@ -6180,1835 +6202,2220 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F56" s="8"/>
+      <c r="A56" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D56" s="9">
+        <v>4</v>
+      </c>
+      <c r="F56" s="8">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="C57" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="2">
-        <v>15</v>
-      </c>
-      <c r="E57" s="2"/>
+        <v>53</v>
+      </c>
+      <c r="D57" s="9">
+        <v>4</v>
+      </c>
       <c r="F57" s="8">
-        <f t="shared" ref="F57:F59" si="19">E57/D57</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="2">
-        <v>160</v>
-      </c>
-      <c r="E58" s="2"/>
-      <c r="F58" s="8">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
+      <c r="A58" s="7"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="F58" s="8"/>
     </row>
-    <row r="59" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D59" s="2">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="8">
+        <f t="shared" ref="F59:F61" si="19">E59/D59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D60" s="2">
+        <v>160</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="8">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H59"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="10"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="18"/>
+    <row r="61" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="2">
+        <v>50</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H61"/>
     </row>
-    <row r="61" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="12"/>
-      <c r="C61" s="13" t="s">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="10"/>
+      <c r="B62" s="17"/>
+      <c r="C62" s="17"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
+      <c r="F62" s="18"/>
+    </row>
+    <row r="63" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D61" s="14">
-        <f>SUM(D2:D60)</f>
-        <v>456</v>
-      </c>
-      <c r="E61" s="14">
-        <f>SUM(E2:E60)</f>
-        <v>203.5</v>
-      </c>
-      <c r="F61" s="15">
-        <f>E61/D61</f>
-        <v>0.44627192982456143</v>
-      </c>
-      <c r="H61" s="1"/>
+      <c r="D63" s="14">
+        <f>SUM(D2:D62)</f>
+        <v>468</v>
+      </c>
+      <c r="E63" s="14">
+        <f>SUM(E2:E62)</f>
+        <v>215.5</v>
+      </c>
+      <c r="F63" s="15">
+        <f>E63/D63</f>
+        <v>0.46047008547008544</v>
+      </c>
+      <c r="H63" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F59" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F61" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B60:F60"/>
+    <mergeCell ref="B62:F62"/>
   </mergeCells>
-  <conditionalFormatting sqref="C62:C1048576 C1:C7 C11:C13 C9 C57:C59">
-    <cfRule type="cellIs" dxfId="416" priority="746" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61:C1048576 C1:C7 C11:C13 C9 C57:C59">
-    <cfRule type="containsText" dxfId="415" priority="744" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C64:C1048576 C1:C7 C11:C13 C9 C59:C61">
+    <cfRule type="cellIs" dxfId="419" priority="818" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C1048576 C1:C7 C11:C13 C9 C59:C61">
+    <cfRule type="containsText" dxfId="418" priority="816" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C57:C1048576">
-    <cfRule type="containsText" dxfId="414" priority="743" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C59:C1048576">
+    <cfRule type="containsText" dxfId="417" priority="815" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="413" priority="738" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="810" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="412" priority="737" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="415" priority="809" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="411" priority="736" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="414" priority="808" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="410" priority="726" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="798" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="409" priority="725" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="412" priority="797" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="408" priority="724" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="411" priority="796" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="407" priority="717" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="789" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="406" priority="716" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="409" priority="788" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="405" priority="715" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="408" priority="787" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="404" priority="714" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="786" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="403" priority="713" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="406" priority="785" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="402" priority="712" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="405" priority="784" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="401" priority="693" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="765" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="400" priority="692" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="403" priority="764" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="399" priority="691" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="402" priority="763" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="398" priority="684" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="756" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="397" priority="683" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="400" priority="755" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="396" priority="682" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="399" priority="754" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="395" priority="663" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="735" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="394" priority="662" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="397" priority="734" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="393" priority="661" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="396" priority="733" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="392" priority="660" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="732" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="391" priority="659" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="394" priority="731" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="390" priority="658" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="393" priority="730" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="389" priority="645" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="717" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="388" priority="644" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="391" priority="716" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="387" priority="643" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="390" priority="715" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="386" priority="642" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="714" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="385" priority="641" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="388" priority="713" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="384" priority="640" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="387" priority="712" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="383" priority="639" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="711" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="382" priority="638" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="385" priority="710" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="381" priority="637" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="384" priority="709" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="380" priority="636" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="708" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="379" priority="635" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="707" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="378" priority="634" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="706" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="377" priority="633" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="705" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="376" priority="632" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="704" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="375" priority="631" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="703" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="374" priority="630" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="702" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="373" priority="629" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="701" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="372" priority="628" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="700" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="371" priority="627" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="699" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="370" priority="626" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="698" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="369" priority="625" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="697" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="368" priority="624" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="696" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="367" priority="623" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="695" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="366" priority="622" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="694" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="365" priority="621" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="693" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="364" priority="620" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="692" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="363" priority="619" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="691" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="362" priority="618" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="690" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="361" priority="617" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="689" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="360" priority="616" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="688" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="359" priority="615" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="687" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="358" priority="614" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="686" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="357" priority="613" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="685" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="356" priority="612" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="684" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="355" priority="611" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="358" priority="683" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="354" priority="610" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="357" priority="682" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="353" priority="609" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="681" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="352" priority="608" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="355" priority="680" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="351" priority="607" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="354" priority="679" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="350" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="678" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="349" priority="605" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="677" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="348" priority="604" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="676" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="347" priority="603" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="675" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="346" priority="602" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="674" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="345" priority="601" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="673" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="344" priority="600" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="672" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="343" priority="599" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="671" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="342" priority="598" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="670" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="341" priority="597" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="669" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="340" priority="596" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="668" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="339" priority="595" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="667" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="338" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="666" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="337" priority="593" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="665" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="336" priority="592" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="664" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="335" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="663" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="334" priority="590" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="662" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="333" priority="589" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="661" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="332" priority="588" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="660" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="331" priority="587" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="659" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="330" priority="586" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="658" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="329" priority="585" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="657" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="328" priority="584" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="656" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="327" priority="583" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="655" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="326" priority="582" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="654" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="325" priority="581" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="653" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="324" priority="580" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="652" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="323" priority="579" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="651" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="322" priority="578" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="650" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="321" priority="577" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="649" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="320" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="648" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="319" priority="575" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="647" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="318" priority="574" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="646" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="317" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="645" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="316" priority="572" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="644" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="315" priority="571" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="643" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="314" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="642" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="313" priority="569" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="641" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="312" priority="568" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="640" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="311" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="606" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="310" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="605" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="309" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="604" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="308" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="636" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="307" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="635" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="306" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="634" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="305" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="633" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="304" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="632" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="303" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="631" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="302" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="301" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="300" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="299" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="298" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="297" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="296" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="624" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="295" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="623" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="294" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="622" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="293" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="621" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="292" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="620" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="291" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="619" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="290" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="289" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="288" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="287" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="615" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="286" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="614" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="285" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="613" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="284" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="612" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="283" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="611" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="282" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="610" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="281" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="609" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="280" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="608" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="279" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="607" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="278" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="603" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="277" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="602" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="276" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="601" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="275" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="600" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="274" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="599" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="273" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="598" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="272" priority="462" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="271" priority="461" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="270" priority="460" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="269" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="268" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="267" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="266" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="265" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="264" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="263" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="262" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="261" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="260" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="259" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="258" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="257" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="256" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="255" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="254" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="253" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="252" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="251" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="250" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="249" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="248" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="247" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="246" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="245" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="244" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="243" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="242" priority="465" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="537" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="241" priority="464" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="536" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="240" priority="463" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="535" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="239" priority="357" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="429" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="238" priority="356" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="428" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="237" priority="355" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="427" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="236" priority="387" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="235" priority="386" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="458" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="234" priority="385" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="457" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="233" priority="384" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="232" priority="383" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="455" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="231" priority="382" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="454" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="230" priority="381" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="453" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="229" priority="380" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="452" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="228" priority="379" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="451" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="227" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="450" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="226" priority="377" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="449" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="225" priority="376" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="448" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="224" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="447" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="223" priority="374" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="446" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="222" priority="373" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="445" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="221" priority="372" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="444" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="220" priority="371" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="443" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="219" priority="370" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="442" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="218" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="441" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="217" priority="368" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="440" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="216" priority="367" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="439" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="215" priority="366" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="438" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="214" priority="365" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="437" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="213" priority="364" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="436" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="212" priority="363" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="435" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="211" priority="362" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="434" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="210" priority="361" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="433" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="209" priority="360" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="432" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="208" priority="359" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="431" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="207" priority="358" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="430" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="206" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="426" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="205" priority="353" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="425" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="204" priority="352" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="424" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="203" priority="321" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="393" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="202" priority="320" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="392" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="201" priority="319" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="391" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="200" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="423" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="199" priority="350" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="198" priority="349" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="197" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="196" priority="347" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="195" priority="346" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="194" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="417" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="193" priority="344" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="192" priority="343" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="191" priority="342" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="414" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="190" priority="341" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="189" priority="340" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="188" priority="339" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="411" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="187" priority="338" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="186" priority="337" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="185" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="408" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="184" priority="335" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="183" priority="334" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="182" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="405" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="181" priority="332" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="180" priority="331" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="179" priority="330" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="402" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="178" priority="329" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="177" priority="328" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="176" priority="327" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="399" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="175" priority="326" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="174" priority="325" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="176" priority="396" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="175" priority="395" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="containsText" dxfId="174" priority="394" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:C46">
     <cfRule type="cellIs" dxfId="173" priority="324" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
+  <conditionalFormatting sqref="C45:C46">
     <cfRule type="containsText" dxfId="172" priority="323" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
+      <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C45:C46">
     <cfRule type="containsText" dxfId="171" priority="322" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="170" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="354" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="169" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="353" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="168" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="352" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="167" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="351" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="166" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="350" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="165" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="349" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="164" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="348" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="163" priority="278" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="347" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="162" priority="277" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="346" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="161" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="345" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="160" priority="275" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="344" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="159" priority="274" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="343" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="158" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="342" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="157" priority="272" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="341" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="156" priority="271" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="340" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="155" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="339" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="154" priority="269" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="338" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="153" priority="268" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="337" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="152" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="336" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="151" priority="266" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="335" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="150" priority="265" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="334" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="149" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="333" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="148" priority="263" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="332" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="147" priority="262" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="331" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="146" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="330" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="145" priority="260" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="329" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="144" priority="259" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="328" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="143" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="327" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="142" priority="257" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="326" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="141" priority="256" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="325" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="140" priority="255" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="139" priority="254" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="138" priority="253" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="137" priority="150" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="136" priority="149" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="140" priority="222" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="139" priority="221" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="135" priority="148" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="138" priority="220" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="134" priority="180" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="133" priority="179" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="137" priority="252" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="136" priority="251" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="132" priority="178" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="135" priority="250" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="131" priority="177" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="130" priority="176" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="134" priority="249" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="133" priority="248" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="129" priority="175" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="132" priority="247" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="128" priority="174" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="127" priority="173" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="131" priority="246" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="130" priority="245" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="126" priority="172" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="129" priority="244" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="125" priority="171" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="124" priority="170" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="128" priority="243" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="127" priority="242" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="123" priority="169" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="126" priority="241" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="122" priority="168" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="121" priority="167" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="125" priority="240" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="124" priority="239" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="120" priority="166" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="123" priority="238" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="119" priority="165" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="118" priority="164" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="122" priority="237" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="121" priority="236" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="117" priority="163" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="120" priority="235" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="116" priority="162" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="115" priority="161" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="119" priority="234" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="118" priority="233" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="114" priority="160" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="117" priority="232" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="113" priority="159" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="112" priority="158" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="116" priority="231" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="115" priority="230" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="111" priority="157" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="114" priority="229" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="110" priority="156" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="109" priority="155" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="113" priority="228" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="112" priority="227" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="108" priority="154" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="111" priority="226" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="cellIs" dxfId="107" priority="153" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="106" priority="152" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="cellIs" dxfId="110" priority="225" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="109" priority="224" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C52">
-    <cfRule type="containsText" dxfId="105" priority="151" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C53">
+    <cfRule type="containsText" dxfId="108" priority="223" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="104" priority="72" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="103" priority="71" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="containsText" dxfId="102" priority="70" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C53)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="101" priority="36" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="100" priority="35" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="107" priority="72" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="106" priority="71" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="105" priority="70" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="104" priority="108" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="103" priority="107" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="99" priority="34" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="102" priority="106" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="98" priority="66" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="97" priority="65" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="101" priority="138" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="100" priority="137" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="96" priority="64" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="99" priority="136" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="95" priority="63" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="94" priority="62" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="98" priority="135" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="97" priority="134" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="93" priority="61" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="96" priority="133" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="92" priority="60" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="91" priority="59" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="95" priority="132" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="94" priority="131" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="90" priority="58" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="93" priority="130" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="89" priority="57" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="88" priority="56" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="92" priority="129" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="91" priority="128" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="87" priority="55" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="90" priority="127" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="86" priority="54" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="85" priority="53" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="89" priority="126" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="88" priority="125" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="84" priority="52" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="87" priority="124" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="83" priority="51" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="82" priority="50" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="86" priority="123" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="85" priority="122" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="81" priority="49" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="84" priority="121" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="80" priority="48" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="79" priority="47" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="83" priority="120" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="82" priority="119" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="78" priority="46" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="81" priority="118" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="77" priority="45" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="76" priority="44" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="80" priority="117" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="79" priority="116" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="75" priority="43" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="78" priority="115" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="74" priority="42" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="73" priority="41" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="77" priority="114" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="76" priority="113" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="72" priority="40" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="75" priority="112" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="70" priority="38" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="cellIs" dxfId="74" priority="111" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="73" priority="110" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
-    <cfRule type="containsText" dxfId="69" priority="37" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C54:C55">
+    <cfRule type="containsText" dxfId="72" priority="109" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="67" priority="38" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="66" priority="37" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="60" priority="64" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="57" priority="61" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="48" priority="52" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="45" priority="49" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57:C58">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57:C1048576 C1:C54" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{A09BE552-C151-A942-89A4-EF775C8F0777}">
       <formula1>"Terminé,En cours,À faire"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update a Neo4j relation
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{071129D8-2F64-754A-8C79-A8B84F782578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F853CBC-F2F0-4F46-9F7B-C049D2482100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="74">
   <si>
     <t>Tâche</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>Rédaction de tests unitaires</t>
+  </si>
+  <si>
+    <t>Mise à jour des relations Neo4j (Cypher)</t>
   </si>
 </sst>
 </file>
@@ -520,7 +523,307 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="420">
+  <dxfs count="450">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5031,11 +5334,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H63"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I54" sqref="I54"/>
+      <selection pane="topRight" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6113,7 +6416,7 @@
         <v>3</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" ref="F51:F57" si="17">E51/D51</f>
+        <f t="shared" ref="F51:F58" si="17">E51/D51</f>
         <v>1.5</v>
       </c>
     </row>
@@ -6238,2180 +6541,2366 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="7"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
-      <c r="F58" s="8"/>
+      <c r="A58" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D58" s="9">
+        <v>2</v>
+      </c>
+      <c r="E58">
+        <v>2</v>
+      </c>
+      <c r="F58" s="8">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D59" s="2">
-        <v>15</v>
-      </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="8">
-        <f t="shared" ref="F59:F61" si="19">E59/D59</f>
-        <v>0</v>
-      </c>
+      <c r="A59" s="7"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="F59" s="8"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D60" s="2">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="E60" s="2"/>
       <c r="F60" s="8">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="F60:F62" si="19">E60/D60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D61" s="2">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" s="8">
         <f t="shared" si="19"/>
         <v>0</v>
       </c>
-      <c r="H61"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="10"/>
-      <c r="B62" s="17"/>
-      <c r="C62" s="17"/>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
-      <c r="F62" s="18"/>
+    <row r="62" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="2">
+        <v>50</v>
+      </c>
+      <c r="E62" s="2"/>
+      <c r="F62" s="8">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="H62"/>
     </row>
-    <row r="63" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="12"/>
-      <c r="C63" s="13" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="10"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="17"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
+      <c r="F63" s="18"/>
+    </row>
+    <row r="64" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D63" s="14">
-        <f>SUM(D2:D62)</f>
-        <v>468</v>
-      </c>
-      <c r="E63" s="14">
-        <f>SUM(E2:E62)</f>
-        <v>215.5</v>
-      </c>
-      <c r="F63" s="15">
-        <f>E63/D63</f>
-        <v>0.46047008547008544</v>
-      </c>
-      <c r="H63" s="1"/>
+      <c r="D64" s="14">
+        <f>SUM(D2:D63)</f>
+        <v>470</v>
+      </c>
+      <c r="E64" s="14">
+        <f>SUM(E2:E63)</f>
+        <v>217.5</v>
+      </c>
+      <c r="F64" s="15">
+        <f>E64/D64</f>
+        <v>0.46276595744680848</v>
+      </c>
+      <c r="H64" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F61" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F62" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B62:F62"/>
+    <mergeCell ref="B63:F63"/>
   </mergeCells>
-  <conditionalFormatting sqref="C64:C1048576 C1:C7 C11:C13 C9 C59:C61">
-    <cfRule type="cellIs" dxfId="419" priority="818" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63:C1048576 C1:C7 C11:C13 C9 C59:C61">
-    <cfRule type="containsText" dxfId="418" priority="816" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C65:C1048576 C1:C7 C11:C13 C9 C60:C62">
+    <cfRule type="cellIs" dxfId="449" priority="851" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64:C1048576 C1:C7 C11:C13 C9 C60:C62">
+    <cfRule type="containsText" dxfId="448" priority="849" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C59:C1048576">
-    <cfRule type="containsText" dxfId="417" priority="815" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C60:C1048576">
+    <cfRule type="containsText" dxfId="447" priority="848" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="416" priority="810" operator="equal">
+    <cfRule type="cellIs" dxfId="446" priority="843" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="415" priority="809" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="445" priority="842" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="414" priority="808" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="444" priority="841" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="413" priority="798" operator="equal">
+    <cfRule type="cellIs" dxfId="443" priority="831" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="412" priority="797" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="442" priority="830" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="411" priority="796" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="441" priority="829" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="410" priority="789" operator="equal">
+    <cfRule type="cellIs" dxfId="440" priority="822" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="409" priority="788" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="439" priority="821" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="408" priority="787" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="438" priority="820" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="407" priority="786" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="819" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="406" priority="785" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="436" priority="818" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="405" priority="784" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="435" priority="817" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="404" priority="765" operator="equal">
+    <cfRule type="cellIs" dxfId="434" priority="798" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="403" priority="764" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="433" priority="797" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="402" priority="763" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="432" priority="796" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="401" priority="756" operator="equal">
+    <cfRule type="cellIs" dxfId="431" priority="789" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="400" priority="755" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="430" priority="788" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="399" priority="754" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="429" priority="787" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="398" priority="735" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="768" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="397" priority="734" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="427" priority="767" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="396" priority="733" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="426" priority="766" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="395" priority="732" operator="equal">
+    <cfRule type="cellIs" dxfId="425" priority="765" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="394" priority="731" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="424" priority="764" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="393" priority="730" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="423" priority="763" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="392" priority="717" operator="equal">
+    <cfRule type="cellIs" dxfId="422" priority="750" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="391" priority="716" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="421" priority="749" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="390" priority="715" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="420" priority="748" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="389" priority="714" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="747" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="388" priority="713" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="418" priority="746" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="387" priority="712" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="417" priority="745" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="386" priority="711" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="744" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="385" priority="710" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="415" priority="743" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="384" priority="709" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="414" priority="742" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="383" priority="708" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="741" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="382" priority="707" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="412" priority="740" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="381" priority="706" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="411" priority="739" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="380" priority="705" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="738" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="379" priority="704" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="409" priority="737" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="378" priority="703" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="408" priority="736" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="377" priority="702" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="735" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="376" priority="701" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="406" priority="734" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="375" priority="700" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="405" priority="733" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="374" priority="699" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="732" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="373" priority="698" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="403" priority="731" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="372" priority="697" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="402" priority="730" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="371" priority="696" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="729" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="370" priority="695" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="400" priority="728" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="369" priority="694" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="399" priority="727" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="368" priority="693" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="726" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="367" priority="692" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="397" priority="725" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="366" priority="691" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="396" priority="724" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="365" priority="690" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="723" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="364" priority="689" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="394" priority="722" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="363" priority="688" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="393" priority="721" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="362" priority="687" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="720" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="361" priority="686" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="391" priority="719" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="360" priority="685" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="390" priority="718" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="359" priority="684" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="717" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="358" priority="683" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="388" priority="716" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="357" priority="682" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="387" priority="715" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="356" priority="681" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="714" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="355" priority="680" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="385" priority="713" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="354" priority="679" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="384" priority="712" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="353" priority="678" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="711" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="352" priority="677" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="710" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="351" priority="676" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="709" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="350" priority="675" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="708" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="349" priority="674" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="707" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="348" priority="673" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="706" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="347" priority="672" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="705" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="346" priority="671" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="704" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="345" priority="670" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="703" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="344" priority="669" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="702" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="343" priority="668" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="701" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="342" priority="667" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="700" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="341" priority="666" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="699" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="340" priority="665" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="698" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="339" priority="664" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="697" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="338" priority="663" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="696" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="337" priority="662" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="695" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="336" priority="661" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="694" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="335" priority="660" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="693" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="334" priority="659" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="692" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="333" priority="658" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="691" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="332" priority="657" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="690" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="331" priority="656" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="689" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="330" priority="655" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="688" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="329" priority="654" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="687" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="328" priority="653" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="358" priority="686" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="327" priority="652" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="357" priority="685" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="326" priority="651" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="684" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="325" priority="650" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="355" priority="683" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="324" priority="649" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="354" priority="682" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="323" priority="648" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="681" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="322" priority="647" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="680" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="321" priority="646" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="679" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="320" priority="645" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="678" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="319" priority="644" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="677" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="318" priority="643" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="676" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="317" priority="642" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="675" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="316" priority="641" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="674" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="315" priority="640" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="673" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="314" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="639" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="313" priority="605" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="638" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="312" priority="604" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="637" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="341" priority="669" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="340" priority="668" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="339" priority="667" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="338" priority="666" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="337" priority="665" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="336" priority="664" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="335" priority="663" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="334" priority="662" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="333" priority="661" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="332" priority="660" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="331" priority="659" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="330" priority="658" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="329" priority="657" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="328" priority="656" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="327" priority="655" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="326" priority="654" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="325" priority="653" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="324" priority="652" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="323" priority="651" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="322" priority="650" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="321" priority="649" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="320" priority="648" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="319" priority="647" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="318" priority="646" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="317" priority="645" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="316" priority="644" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="315" priority="643" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="314" priority="642" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="313" priority="641" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="312" priority="640" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="311" priority="636" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="310" priority="635" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+      <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="containsText" dxfId="309" priority="634" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+      <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="cellIs" dxfId="308" priority="633" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+  <conditionalFormatting sqref="C44">
     <cfRule type="containsText" dxfId="307" priority="632" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
+      <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44">
     <cfRule type="containsText" dxfId="306" priority="631" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="305" priority="630" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="304" priority="629" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="303" priority="628" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="302" priority="627" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="301" priority="626" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="300" priority="625" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="299" priority="624" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="298" priority="623" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="297" priority="622" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="296" priority="621" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="295" priority="620" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="294" priority="619" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="293" priority="618" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="292" priority="617" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="291" priority="616" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="290" priority="615" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="289" priority="614" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="288" priority="613" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="287" priority="612" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="286" priority="611" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="285" priority="610" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="284" priority="609" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="283" priority="608" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="282" priority="607" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="281" priority="603" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="280" priority="602" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="279" priority="601" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="278" priority="600" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="277" priority="599" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="276" priority="598" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="275" priority="534" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="567" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="274" priority="533" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="566" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="273" priority="532" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="565" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="272" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="597" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="271" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="596" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="270" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="595" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="269" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="594" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="268" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="593" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="267" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="592" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="266" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="591" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="265" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="590" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="264" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="589" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="263" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="588" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="262" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="587" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="261" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="586" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="260" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="585" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="259" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="584" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="258" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="583" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="257" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="582" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="256" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="581" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="255" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="580" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="254" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="579" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="253" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="578" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="252" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="577" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="251" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="576" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="250" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="575" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="249" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="574" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="248" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="573" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="247" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="572" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="246" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="571" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="245" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="244" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="243" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="242" priority="429" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="241" priority="428" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="240" priority="427" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="269" priority="492" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="268" priority="491" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="267" priority="490" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="266" priority="489" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="265" priority="488" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="264" priority="487" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="263" priority="486" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="262" priority="485" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="261" priority="484" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="260" priority="483" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="259" priority="482" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="258" priority="481" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="257" priority="480" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="256" priority="479" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="255" priority="478" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="254" priority="477" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="253" priority="476" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="252" priority="475" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="251" priority="474" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="250" priority="473" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="249" priority="472" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="248" priority="471" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="247" priority="470" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="246" priority="469" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="245" priority="468" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="244" priority="467" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="243" priority="466" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="cellIs" dxfId="242" priority="465" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="241" priority="464" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47">
+    <cfRule type="containsText" dxfId="240" priority="463" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="cellIs" dxfId="239" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+  <conditionalFormatting sqref="C48">
     <cfRule type="containsText" dxfId="238" priority="458" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
     <cfRule type="containsText" dxfId="237" priority="457" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="236" priority="456" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="235" priority="455" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="234" priority="454" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="233" priority="453" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="232" priority="452" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="231" priority="451" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="230" priority="450" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="229" priority="449" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="228" priority="448" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="227" priority="447" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="226" priority="446" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="225" priority="445" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="224" priority="444" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="223" priority="443" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="222" priority="442" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="221" priority="441" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="220" priority="440" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="219" priority="439" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="218" priority="438" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="217" priority="437" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="216" priority="436" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="215" priority="435" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="214" priority="434" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="213" priority="433" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="212" priority="432" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="211" priority="431" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="210" priority="430" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="209" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="426" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="208" priority="425" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="425" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="207" priority="424" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="424" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="206" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="205" priority="392" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="455" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="204" priority="391" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="454" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="203" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="453" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="202" priority="422" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="452" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="201" priority="421" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="451" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="200" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="450" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="199" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="449" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="198" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="448" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="197" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="447" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="196" priority="416" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="446" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="195" priority="415" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="445" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="194" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="444" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="193" priority="413" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="443" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="192" priority="412" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="442" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="191" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="441" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="190" priority="410" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="440" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="189" priority="409" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="439" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="188" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="438" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="187" priority="407" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="437" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="186" priority="406" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="436" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="185" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="435" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="184" priority="404" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="434" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="183" priority="403" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="433" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="182" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="432" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="181" priority="401" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="431" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="180" priority="400" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="430" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="179" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="429" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="178" priority="398" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="428" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="177" priority="397" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="427" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="176" priority="396" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="175" priority="395" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="174" priority="394" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="173" priority="324" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="357" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="172" priority="323" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="356" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="171" priority="322" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="355" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="170" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="387" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="169" priority="353" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="386" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="168" priority="352" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="385" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="167" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="384" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="166" priority="350" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="383" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="165" priority="349" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="382" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="164" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="381" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="163" priority="347" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="380" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="162" priority="346" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="379" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="161" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="378" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="160" priority="344" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="377" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="159" priority="343" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="376" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="158" priority="342" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="375" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="157" priority="341" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="374" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="156" priority="340" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="373" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="155" priority="339" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="372" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="154" priority="338" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="371" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="153" priority="337" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="370" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="152" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="369" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="151" priority="335" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="368" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="150" priority="334" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="367" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="149" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="366" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="148" priority="332" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="365" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="147" priority="331" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="364" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="146" priority="330" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="363" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="145" priority="329" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="362" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="144" priority="328" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="361" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="143" priority="327" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="360" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="142" priority="326" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="359" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="141" priority="325" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="358" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="140" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="139" priority="221" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="138" priority="220" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="137" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="285" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="136" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="284" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="135" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="283" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="134" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="133" priority="248" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="132" priority="247" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="131" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="130" priority="245" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="129" priority="244" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="128" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="127" priority="242" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="126" priority="241" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="125" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="124" priority="239" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="123" priority="238" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="122" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="121" priority="236" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="120" priority="235" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="119" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="118" priority="233" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="117" priority="232" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="116" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="115" priority="230" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="114" priority="229" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="113" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="112" priority="227" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="111" priority="226" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="110" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="109" priority="224" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="108" priority="223" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="107" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="105" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="106" priority="71" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="136" priority="104" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="105" priority="70" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="135" priority="103" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="104" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="141" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="103" priority="107" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="133" priority="140" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="102" priority="106" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="132" priority="139" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="101" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="171" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="100" priority="137" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="130" priority="170" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="99" priority="136" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="129" priority="169" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="98" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="168" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="97" priority="134" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="127" priority="167" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="96" priority="133" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="126" priority="166" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="95" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="165" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="94" priority="131" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="124" priority="164" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="93" priority="130" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="123" priority="163" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="92" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="162" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="91" priority="128" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="121" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="90" priority="127" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="120" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="89" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="159" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="88" priority="125" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="118" priority="158" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="87" priority="124" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="117" priority="157" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="86" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="156" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="85" priority="122" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="115" priority="155" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="84" priority="121" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="114" priority="154" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="83" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="153" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="82" priority="119" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="112" priority="152" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="81" priority="118" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="111" priority="151" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="80" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="150" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="79" priority="116" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="109" priority="149" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="78" priority="115" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="108" priority="148" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="77" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="147" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="76" priority="113" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="75" priority="112" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="cellIs" dxfId="74" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="144" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="73" priority="110" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="143" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C54:C55">
-    <cfRule type="containsText" dxfId="72" priority="109" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="142" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="72" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="67" priority="38" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="71" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="66" priority="37" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="70" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="102" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="100" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="95" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="93" priority="97" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="87" priority="91" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="86" priority="90" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="84" priority="88" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="83" priority="87" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="81" priority="85" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="78" priority="82" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="77" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="75" priority="79" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="70" priority="74" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="containsText" dxfId="69" priority="73" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="cellIs" dxfId="68" priority="69" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="cellIs" dxfId="65" priority="36" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="containsText" dxfId="64" priority="35" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="containsText" dxfId="63" priority="34" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="60" priority="64" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="57" priority="61" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="48" priority="52" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="45" priority="49" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
     <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C56)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C57 C59">
+    <cfRule type="containsText" dxfId="33" priority="37" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57:C58">
+      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Finalisation de l'API et validation par les tests unitaires
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEA6326-9122-C447-BBD5-8D712F6D7416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55296CF5-4DB7-BE4D-8DCB-6864B3D4570D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -261,7 +261,7 @@
     <t>Mise à jour des relations Neo4j (Cypher)</t>
   </si>
   <si>
-    <t>Création des endpoints /categories</t>
+    <t>Ajout des catégories aux ressources</t>
   </si>
 </sst>
 </file>
@@ -526,397 +526,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="489">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="450">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5729,9 +5339,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D63" sqref="D63"/>
+      <selection pane="topRight" activeCell="H54" sqref="H54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6776,20 +6386,20 @@
         <v>12</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D50" s="9">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E50">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F50" s="8">
-        <f t="shared" ref="F50" si="16">E50/D50</f>
-        <v>2</v>
+        <f>E50/D50</f>
+        <v>0.9375</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -6797,7 +6407,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>2</v>
@@ -6806,11 +6416,11 @@
         <v>2</v>
       </c>
       <c r="E51">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F51" s="8">
-        <f t="shared" ref="F51:F59" si="17">E51/D51</f>
-        <v>1.5</v>
+        <f t="shared" ref="F51" si="16">E51/D51</f>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -6818,20 +6428,20 @@
         <v>12</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D52" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F52" s="8">
-        <f t="shared" si="17"/>
-        <v>1</v>
+        <f t="shared" ref="F52:F59" si="17">E52/D52</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -6839,20 +6449,20 @@
         <v>12</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D53" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E53">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" si="17"/>
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -6860,20 +6470,20 @@
         <v>12</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D54" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E54">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F54" s="8">
-        <f t="shared" ref="F54" si="18">E54/D54</f>
-        <v>1.25</v>
+        <f t="shared" si="17"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
@@ -6881,7 +6491,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>2</v>
@@ -6890,11 +6500,11 @@
         <v>4</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F55" s="8">
-        <f t="shared" si="17"/>
-        <v>0.75</v>
+        <f t="shared" ref="F55" si="18">E55/D55</f>
+        <v>1.25</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -6902,16 +6512,16 @@
         <v>12</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D56" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F56" s="8">
         <f t="shared" si="17"/>
@@ -6923,20 +6533,20 @@
         <v>12</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D57" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F57" s="8">
-        <f t="shared" ref="F57" si="19">E57/D57</f>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>0.75</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -6944,20 +6554,20 @@
         <v>12</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="D58" s="9">
         <v>4</v>
       </c>
       <c r="E58">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F58" s="8">
-        <f t="shared" si="17"/>
-        <v>0.75</v>
+        <f t="shared" ref="F58" si="19">E58/D58</f>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -7031,7 +6641,7 @@
         <v>22</v>
       </c>
       <c r="D63" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="8">
@@ -7056,15 +6666,15 @@
       </c>
       <c r="D65" s="14">
         <f>SUM(D2:D64)</f>
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="E65" s="14">
         <f>SUM(E2:E64)</f>
-        <v>226.5</v>
+        <v>238.5</v>
       </c>
       <c r="F65" s="15">
         <f>E65/D65</f>
-        <v>0.5055803571428571</v>
+        <v>0.53</v>
       </c>
       <c r="H65" s="1"/>
     </row>
@@ -7074,2088 +6684,2088 @@
     <mergeCell ref="B64:F64"/>
   </mergeCells>
   <conditionalFormatting sqref="C66:C1048576 C1:C7 C11:C13 C9 C61:C63">
-    <cfRule type="cellIs" dxfId="488" priority="890" operator="equal">
+    <cfRule type="cellIs" dxfId="449" priority="890" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65:C1048576 C1:C7 C11:C13 C9 C61:C63">
-    <cfRule type="containsText" dxfId="487" priority="888" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="448" priority="888" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C7 C11:C13 C9 C61:C1048576">
-    <cfRule type="containsText" dxfId="486" priority="887" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="447" priority="887" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="485" priority="882" operator="equal">
+    <cfRule type="cellIs" dxfId="446" priority="882" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="484" priority="881" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="445" priority="881" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="483" priority="880" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="444" priority="880" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="482" priority="870" operator="equal">
+    <cfRule type="cellIs" dxfId="443" priority="870" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="481" priority="869" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="442" priority="869" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="480" priority="868" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="441" priority="868" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="479" priority="861" operator="equal">
+    <cfRule type="cellIs" dxfId="440" priority="861" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="478" priority="860" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="439" priority="860" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="477" priority="859" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="438" priority="859" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="476" priority="858" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="858" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="475" priority="857" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="436" priority="857" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="474" priority="856" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="435" priority="856" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="473" priority="837" operator="equal">
+    <cfRule type="cellIs" dxfId="434" priority="837" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="472" priority="836" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="433" priority="836" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="471" priority="835" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="432" priority="835" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="470" priority="828" operator="equal">
+    <cfRule type="cellIs" dxfId="431" priority="828" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="469" priority="827" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="430" priority="827" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="468" priority="826" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="429" priority="826" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="467" priority="807" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="807" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="466" priority="806" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="427" priority="806" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="465" priority="805" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="426" priority="805" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="464" priority="804" operator="equal">
+    <cfRule type="cellIs" dxfId="425" priority="804" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="463" priority="803" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="424" priority="803" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="462" priority="802" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="423" priority="802" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="461" priority="789" operator="equal">
+    <cfRule type="cellIs" dxfId="422" priority="789" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="460" priority="788" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="421" priority="788" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="459" priority="787" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="420" priority="787" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="458" priority="786" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="786" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="457" priority="785" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="418" priority="785" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="456" priority="784" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="417" priority="784" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="455" priority="783" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="783" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="454" priority="782" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="415" priority="782" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="453" priority="781" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="414" priority="781" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="452" priority="780" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="780" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="451" priority="779" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="412" priority="779" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="450" priority="778" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="411" priority="778" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="449" priority="777" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="777" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="448" priority="776" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="409" priority="776" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="447" priority="775" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="408" priority="775" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="446" priority="774" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="774" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="445" priority="773" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="406" priority="773" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="444" priority="772" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="405" priority="772" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="443" priority="771" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="771" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="442" priority="770" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="403" priority="770" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="441" priority="769" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="402" priority="769" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="440" priority="768" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="768" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="439" priority="767" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="400" priority="767" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="438" priority="766" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="399" priority="766" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="437" priority="765" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="765" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="436" priority="764" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="397" priority="764" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="435" priority="763" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="396" priority="763" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="434" priority="762" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="762" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="433" priority="761" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="394" priority="761" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="432" priority="760" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="393" priority="760" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="431" priority="759" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="759" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="430" priority="758" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="391" priority="758" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="429" priority="757" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="390" priority="757" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="428" priority="756" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="756" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="427" priority="755" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="388" priority="755" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="426" priority="754" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="387" priority="754" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="425" priority="753" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="753" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="424" priority="752" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="385" priority="752" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="423" priority="751" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="384" priority="751" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="422" priority="750" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="750" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="421" priority="749" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="749" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="420" priority="748" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="748" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="419" priority="747" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="747" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="418" priority="746" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="746" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="417" priority="745" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="745" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="416" priority="744" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="744" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="415" priority="743" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="743" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="414" priority="742" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="742" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="413" priority="741" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="741" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="412" priority="740" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="740" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="411" priority="739" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="739" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="410" priority="738" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="738" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="409" priority="737" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="737" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="408" priority="736" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="736" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="407" priority="735" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="735" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="406" priority="734" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="734" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="405" priority="733" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="733" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="404" priority="732" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="732" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="403" priority="731" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="731" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="402" priority="730" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="730" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="401" priority="729" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="729" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="400" priority="728" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="728" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="399" priority="727" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="727" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="398" priority="726" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="726" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="397" priority="725" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="358" priority="725" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="396" priority="724" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="357" priority="724" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="395" priority="723" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="723" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="394" priority="722" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="355" priority="722" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="393" priority="721" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="354" priority="721" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="392" priority="720" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="720" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="391" priority="719" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="719" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="390" priority="718" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="718" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="389" priority="717" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="717" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="388" priority="716" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="716" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="387" priority="715" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="715" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="386" priority="714" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="714" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="385" priority="713" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="713" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="384" priority="712" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="712" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="383" priority="678" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="678" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="382" priority="677" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="677" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="381" priority="676" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="676" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="380" priority="708" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="708" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="379" priority="707" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="707" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="378" priority="706" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="706" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="377" priority="705" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="705" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="376" priority="704" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="704" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="375" priority="703" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="703" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="374" priority="702" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="702" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="373" priority="701" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="701" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="372" priority="700" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="700" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="371" priority="699" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="699" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="370" priority="698" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="698" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="369" priority="697" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="697" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="368" priority="696" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="696" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="367" priority="695" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="695" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="366" priority="694" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="694" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="365" priority="693" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="693" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="364" priority="692" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="692" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="363" priority="691" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="691" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="362" priority="690" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="690" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="361" priority="689" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="689" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="360" priority="688" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="688" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="359" priority="687" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="687" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="358" priority="686" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="686" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="357" priority="685" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="685" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="356" priority="684" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="684" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="355" priority="683" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="683" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="354" priority="682" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="682" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="353" priority="681" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="681" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="352" priority="680" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="680" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="351" priority="679" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="679" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="350" priority="675" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="675" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="349" priority="674" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="674" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="348" priority="673" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="673" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="347" priority="672" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="672" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="346" priority="671" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="671" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="345" priority="670" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="670" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="344" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="606" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="343" priority="605" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="605" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="342" priority="604" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="604" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="341" priority="636" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="636" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="340" priority="635" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="635" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="339" priority="634" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="634" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="338" priority="633" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="633" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="337" priority="632" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="632" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="336" priority="631" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="631" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="335" priority="630" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="334" priority="629" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="333" priority="628" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="332" priority="627" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="331" priority="626" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="330" priority="625" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="329" priority="624" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="624" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="328" priority="623" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="623" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="327" priority="622" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="622" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="326" priority="621" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="621" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="325" priority="620" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="620" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="324" priority="619" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="619" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="323" priority="618" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="322" priority="617" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="321" priority="616" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="320" priority="615" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="615" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="319" priority="614" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="614" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="318" priority="613" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="613" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="317" priority="612" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="612" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="316" priority="611" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="611" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="315" priority="610" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="610" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="314" priority="609" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="609" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="313" priority="608" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="608" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="312" priority="607" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="607" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="311" priority="501" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="501" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="310" priority="500" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="500" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="309" priority="499" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="499" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="308" priority="531" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="531" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="307" priority="530" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="530" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="306" priority="529" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="529" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="305" priority="528" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="528" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="304" priority="527" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="527" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="303" priority="526" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="526" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="302" priority="525" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="525" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="301" priority="524" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="524" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="300" priority="523" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="523" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="299" priority="522" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="522" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="298" priority="521" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="521" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="297" priority="520" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="520" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="296" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="519" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="295" priority="518" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="518" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="294" priority="517" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="517" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="293" priority="516" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="516" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="292" priority="515" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="515" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="291" priority="514" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="514" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="290" priority="513" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="513" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="289" priority="512" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="512" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="288" priority="511" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="511" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="287" priority="510" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="510" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="286" priority="509" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="509" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="285" priority="508" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="508" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="284" priority="507" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="507" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="283" priority="506" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="506" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="282" priority="505" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="505" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="281" priority="504" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="504" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="280" priority="503" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="503" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="279" priority="502" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="502" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="278" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="498" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="277" priority="497" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="497" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="276" priority="496" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="496" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="275" priority="465" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="274" priority="464" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="273" priority="463" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="272" priority="495" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="495" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="271" priority="494" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="494" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="270" priority="493" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="493" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="269" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="492" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="268" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="491" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="267" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="490" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="266" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="489" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="265" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="488" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="264" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="487" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="263" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="486" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="262" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="485" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="261" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="484" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="260" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="483" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="259" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="482" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="258" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="481" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="257" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="480" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="256" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="479" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="255" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="478" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="254" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="477" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="253" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="476" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="252" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="475" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="251" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="474" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="250" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="473" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="249" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="472" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="248" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="471" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="247" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="470" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="246" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="469" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="245" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="468" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="244" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="467" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="243" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="466" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="242" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="396" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="241" priority="395" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="395" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="240" priority="394" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="394" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="239" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="426" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="238" priority="425" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="425" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="237" priority="424" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="424" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="236" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="423" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="235" priority="422" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="234" priority="421" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="233" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="420" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="232" priority="419" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="231" priority="418" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="230" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="417" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="229" priority="416" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="228" priority="415" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="227" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="414" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="226" priority="413" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="225" priority="412" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="224" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="411" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="223" priority="410" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="222" priority="409" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="221" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="408" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="220" priority="407" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="219" priority="406" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="218" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="405" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="217" priority="404" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="216" priority="403" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="215" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="402" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="214" priority="401" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="213" priority="400" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="212" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="399" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="211" priority="398" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="210" priority="397" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="209" priority="294" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="208" priority="293" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="170" priority="294" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="169" priority="293" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="207" priority="292" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="168" priority="292" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="206" priority="324" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="205" priority="323" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="167" priority="324" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="166" priority="323" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="204" priority="322" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="165" priority="322" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="203" priority="321" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="202" priority="320" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="164" priority="321" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="163" priority="320" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="201" priority="319" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="162" priority="319" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="200" priority="318" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="199" priority="317" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="161" priority="318" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="160" priority="317" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="198" priority="316" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="159" priority="316" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="197" priority="315" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="196" priority="314" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="158" priority="315" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="157" priority="314" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="195" priority="313" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="156" priority="313" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="194" priority="312" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="193" priority="311" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="155" priority="312" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="154" priority="311" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="192" priority="310" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="153" priority="310" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="191" priority="309" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="190" priority="308" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="152" priority="309" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="151" priority="308" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="189" priority="307" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="150" priority="307" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="188" priority="306" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="187" priority="305" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="149" priority="306" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="148" priority="305" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="186" priority="304" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="147" priority="304" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="185" priority="303" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="184" priority="302" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="146" priority="303" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="145" priority="302" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="183" priority="301" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="144" priority="301" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="182" priority="300" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="181" priority="299" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="143" priority="300" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="142" priority="299" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="180" priority="298" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="141" priority="298" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="cellIs" dxfId="179" priority="297" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="178" priority="296" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="cellIs" dxfId="140" priority="297" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="139" priority="296" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49:C53">
-    <cfRule type="containsText" dxfId="177" priority="295" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C49:C54">
+    <cfRule type="containsText" dxfId="138" priority="295" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="173" priority="180" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="172" priority="179" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="171" priority="178" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="170" priority="210" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="169" priority="209" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="168" priority="208" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="167" priority="207" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="166" priority="206" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="165" priority="205" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="164" priority="204" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="163" priority="203" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="162" priority="202" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="161" priority="201" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="160" priority="200" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="159" priority="199" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="158" priority="198" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="157" priority="197" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="156" priority="196" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="155" priority="195" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="154" priority="194" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="153" priority="193" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="152" priority="192" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="151" priority="191" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="150" priority="190" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="149" priority="189" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="148" priority="188" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="147" priority="187" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="146" priority="186" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="145" priority="185" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="144" priority="184" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="cellIs" dxfId="143" priority="183" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="142" priority="182" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C54:C56">
-    <cfRule type="containsText" dxfId="141" priority="181" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C54)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="107" priority="108" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="106" priority="107" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="137" priority="180" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="136" priority="179" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="135" priority="178" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="134" priority="210" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="133" priority="209" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="132" priority="208" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="131" priority="207" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="130" priority="206" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="129" priority="205" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="128" priority="204" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="127" priority="203" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="126" priority="202" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="125" priority="201" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="124" priority="200" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="123" priority="199" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="122" priority="198" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="121" priority="197" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="120" priority="196" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="119" priority="195" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="118" priority="194" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="117" priority="193" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="116" priority="192" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="115" priority="191" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="114" priority="190" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="113" priority="189" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="112" priority="188" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="111" priority="187" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="110" priority="186" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="109" priority="185" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="108" priority="184" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="cellIs" dxfId="107" priority="183" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="106" priority="182" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C55:C57">
+    <cfRule type="containsText" dxfId="105" priority="181" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="104" priority="108" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="103" priority="107" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="102" priority="106" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="101" priority="75" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="100" priority="74" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="99" priority="73" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="98" priority="105" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="97" priority="104" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="96" priority="103" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="95" priority="102" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="94" priority="101" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="93" priority="100" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="92" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="91" priority="98" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="90" priority="97" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="89" priority="96" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="88" priority="95" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="87" priority="94" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="86" priority="93" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="85" priority="92" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="84" priority="91" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="83" priority="90" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="82" priority="89" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="81" priority="88" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="80" priority="87" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="79" priority="86" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="78" priority="85" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="77" priority="84" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="76" priority="83" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="75" priority="82" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="74" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="73" priority="80" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="72" priority="79" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="cellIs" dxfId="71" priority="78" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="70" priority="77" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C60">
+    <cfRule type="containsText" dxfId="69" priority="76" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="68" priority="42" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="67" priority="41" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="66" priority="40" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="65" priority="72" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="64" priority="71" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="63" priority="70" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="62" priority="69" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="61" priority="68" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="60" priority="67" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="58" priority="65" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="57" priority="64" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="55" priority="62" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="54" priority="61" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="53" priority="60" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="52" priority="59" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="51" priority="58" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="50" priority="57" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="49" priority="56" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="48" priority="55" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="47" priority="54" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="46" priority="53" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="45" priority="52" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="43" priority="50" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="42" priority="49" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="41" priority="48" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="40" priority="47" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="39" priority="46" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="38" priority="45" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="37" priority="44" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="105" priority="106" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C58">
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="104" priority="75" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="103" priority="74" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="102" priority="73" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="101" priority="105" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="100" priority="104" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="99" priority="103" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="98" priority="102" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="96" priority="100" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="95" priority="99" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="93" priority="97" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="87" priority="91" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="86" priority="90" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="84" priority="88" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="83" priority="87" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="81" priority="85" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="78" priority="82" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="77" priority="81" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="75" priority="79" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="cellIs" dxfId="74" priority="78" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="73" priority="77" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58 C60">
-    <cfRule type="containsText" dxfId="72" priority="76" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="71" priority="42" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="70" priority="41" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="69" priority="40" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="68" priority="72" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="67" priority="71" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="66" priority="70" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="60" priority="64" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="57" priority="61" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="48" priority="52" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="45" priority="49" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C57)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C57)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
[S2] Epic 1 : Création d’un compte et authentification
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411F54C5-E507-9945-9547-C1EB22D7C535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40D2174-3E4B-4E4E-9C27-8A97DBBDF5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="77">
   <si>
     <t>Tâche</t>
   </si>
@@ -204,9 +204,6 @@
     <t>Mise en place d'Express</t>
   </si>
   <si>
-    <t>Mise en place d'Angular + test de déploiement</t>
-  </si>
-  <si>
     <t>Logotype</t>
   </si>
   <si>
@@ -264,7 +261,13 @@
     <t>Ajout des catégories aux ressources</t>
   </si>
   <si>
-    <t>Déploiement de l'API Express</t>
+    <t>Mise en place front-end + test de déploiement</t>
+  </si>
+  <si>
+    <t>Déploiement de l'API Express (+Dockerize)</t>
+  </si>
+  <si>
+    <t>[S2] Epic 1 : Création d’un compte et authentification</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,727 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="489">
+  <dxfs count="561">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5730,11 +6453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H61" sqref="H61"/>
+      <selection pane="topRight" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6548,7 +7271,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>2</v>
@@ -6590,7 +7313,7 @@
         <v>12</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>2</v>
@@ -6611,7 +7334,7 @@
         <v>10</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>22</v>
@@ -6632,7 +7355,7 @@
         <v>10</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>22</v>
@@ -6653,7 +7376,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>22</v>
@@ -6674,7 +7397,7 @@
         <v>12</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>2</v>
@@ -6695,7 +7418,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>2</v>
@@ -6716,7 +7439,7 @@
         <v>12</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>2</v>
@@ -6737,7 +7460,7 @@
         <v>12</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>53</v>
@@ -6746,19 +7469,19 @@
         <v>4</v>
       </c>
       <c r="E48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F48" s="8">
         <f t="shared" si="10"/>
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>2</v>
@@ -6774,12 +7497,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>2</v>
@@ -6795,12 +7518,12 @@
         <v>0.9375</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>2</v>
@@ -6816,12 +7539,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>2</v>
@@ -6833,16 +7556,16 @@
         <v>3</v>
       </c>
       <c r="F52" s="8">
-        <f t="shared" ref="F52:F60" si="17">E52/D52</f>
+        <f t="shared" ref="F52:F57" si="17">E52/D52</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>2</v>
@@ -6858,12 +7581,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>2</v>
@@ -6879,12 +7602,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>2</v>
@@ -6900,12 +7623,12 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>2</v>
@@ -6921,12 +7644,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>2</v>
@@ -6942,12 +7665,12 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>22</v>
@@ -6963,12 +7686,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>2</v>
@@ -6984,7 +7707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>12</v>
       </c>
@@ -7005,2361 +7728,2562 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="7"/>
-      <c r="B61" s="9"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="9"/>
-      <c r="F61" s="8"/>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="9">
+        <v>8</v>
+      </c>
+      <c r="E61">
+        <v>8</v>
+      </c>
+      <c r="F61" s="8">
+        <f>E61/D61</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="7" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="7"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="7" t="s">
         <v>10</v>
-      </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="2">
-        <v>15</v>
-      </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="8">
-        <f t="shared" ref="F62:F64" si="20">E62/D62</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
-        <v>12</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D63" s="2">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="8">
-        <f t="shared" si="20"/>
+        <f>E63/D63</f>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D64" s="2">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="8">
-        <f t="shared" si="20"/>
+        <f>E64/D64</f>
         <v>0</v>
       </c>
-      <c r="H64"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="10"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-      <c r="E65" s="17"/>
-      <c r="F65" s="18"/>
+    <row r="65" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D65" s="2">
+        <v>40</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="8">
+        <f>E65/D65</f>
+        <v>0</v>
+      </c>
+      <c r="H65"/>
     </row>
-    <row r="66" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="13" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="10"/>
+      <c r="B66" s="17"/>
+      <c r="C66" s="17"/>
+      <c r="D66" s="17"/>
+      <c r="E66" s="17"/>
+      <c r="F66" s="18"/>
+    </row>
+    <row r="67" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="11"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D66" s="14">
-        <f>SUM(D2:D65)</f>
-        <v>452</v>
-      </c>
-      <c r="E66" s="14">
-        <f>SUM(E2:E65)</f>
-        <v>240.5</v>
-      </c>
-      <c r="F66" s="15">
-        <f>E66/D66</f>
-        <v>0.53207964601769908</v>
-      </c>
-      <c r="H66" s="1"/>
+      <c r="D67" s="14">
+        <f>SUM(D2:D66)</f>
+        <v>450</v>
+      </c>
+      <c r="E67" s="14">
+        <f>SUM(E2:E66)</f>
+        <v>250.5</v>
+      </c>
+      <c r="F67" s="15">
+        <f>E67/D67</f>
+        <v>0.55666666666666664</v>
+      </c>
+      <c r="H67" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F64" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F65" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B66:F66"/>
   </mergeCells>
-  <conditionalFormatting sqref="C67:C1048576 C1:C7 C11:C13 C9 C62:C64">
-    <cfRule type="cellIs" dxfId="488" priority="962" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C1048576 C1:C7 C11:C13 C9 C62:C64">
-    <cfRule type="containsText" dxfId="487" priority="960" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C68:C1048576 C1:C7 C11:C13 C9 C63:C65">
+    <cfRule type="cellIs" dxfId="560" priority="1034" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C67:C1048576 C1:C7 C11:C13 C9 C63:C65">
+    <cfRule type="containsText" dxfId="559" priority="1032" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C62:C1048576">
-    <cfRule type="containsText" dxfId="486" priority="959" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C63:C1048576">
+    <cfRule type="containsText" dxfId="558" priority="1031" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="485" priority="954" operator="equal">
+    <cfRule type="cellIs" dxfId="557" priority="1026" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="484" priority="953" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="556" priority="1025" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="483" priority="952" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="555" priority="1024" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="482" priority="942" operator="equal">
+    <cfRule type="cellIs" dxfId="554" priority="1014" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="481" priority="941" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="553" priority="1013" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="480" priority="940" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="552" priority="1012" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="479" priority="933" operator="equal">
+    <cfRule type="cellIs" dxfId="551" priority="1005" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="478" priority="932" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="550" priority="1004" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="477" priority="931" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="549" priority="1003" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="476" priority="930" operator="equal">
+    <cfRule type="cellIs" dxfId="548" priority="1002" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="475" priority="929" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="547" priority="1001" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="474" priority="928" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="546" priority="1000" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="473" priority="909" operator="equal">
+    <cfRule type="cellIs" dxfId="545" priority="981" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="472" priority="908" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="544" priority="980" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="471" priority="907" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="543" priority="979" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="470" priority="900" operator="equal">
+    <cfRule type="cellIs" dxfId="542" priority="972" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="469" priority="899" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="541" priority="971" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="468" priority="898" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="540" priority="970" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="467" priority="879" operator="equal">
+    <cfRule type="cellIs" dxfId="539" priority="951" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="466" priority="878" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="538" priority="950" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="465" priority="877" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="537" priority="949" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="464" priority="876" operator="equal">
+    <cfRule type="cellIs" dxfId="536" priority="948" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="463" priority="875" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="535" priority="947" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="462" priority="874" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="534" priority="946" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
+    <cfRule type="cellIs" dxfId="533" priority="933" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C37">
+    <cfRule type="containsText" dxfId="532" priority="932" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C37">
+    <cfRule type="containsText" dxfId="531" priority="931" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="cellIs" dxfId="530" priority="930" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="containsText" dxfId="529" priority="929" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C42">
+    <cfRule type="containsText" dxfId="528" priority="928" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="527" priority="927" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="526" priority="926" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="525" priority="925" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="524" priority="924" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="523" priority="923" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="containsText" dxfId="522" priority="922" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="521" priority="921" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="520" priority="920" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="519" priority="919" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="518" priority="918" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="517" priority="917" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="516" priority="916" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="515" priority="915" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="514" priority="914" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="513" priority="913" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="512" priority="912" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="511" priority="911" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="510" priority="910" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="509" priority="909" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="508" priority="908" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="507" priority="907" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="506" priority="906" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="505" priority="905" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="containsText" dxfId="504" priority="904" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="503" priority="903" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="502" priority="902" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="501" priority="901" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="500" priority="900" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="499" priority="899" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="498" priority="898" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="497" priority="897" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="496" priority="896" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="495" priority="895" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="494" priority="894" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="493" priority="893" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="492" priority="892" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="491" priority="891" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="490" priority="890" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="489" priority="889" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="488" priority="888" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="487" priority="887" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="486" priority="886" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="485" priority="885" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="484" priority="884" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="containsText" dxfId="483" priority="883" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="482" priority="882" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="481" priority="881" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="480" priority="880" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="479" priority="879" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="478" priority="878" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="477" priority="877" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="476" priority="876" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="475" priority="875" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="474" priority="874" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="473" priority="873" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="472" priority="872" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="471" priority="871" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="470" priority="870" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="469" priority="869" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="468" priority="868" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="467" priority="867" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="466" priority="866" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="465" priority="865" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="cellIs" dxfId="464" priority="864" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="463" priority="863" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="462" priority="862" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="461" priority="861" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C37">
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="460" priority="860" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35:C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="459" priority="859" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="458" priority="858" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="457" priority="857" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
     <cfRule type="containsText" dxfId="456" priority="856" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="455" priority="855" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="454" priority="854" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="453" priority="853" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="cellIs" dxfId="455" priority="822" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="454" priority="821" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
+    <cfRule type="containsText" dxfId="453" priority="820" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="452" priority="852" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="451" priority="851" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="450" priority="850" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="449" priority="849" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="448" priority="848" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="447" priority="847" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="446" priority="846" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="445" priority="845" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="444" priority="844" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="443" priority="843" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="442" priority="842" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="441" priority="841" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="440" priority="840" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="439" priority="839" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="438" priority="838" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="437" priority="837" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="436" priority="836" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="435" priority="835" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="434" priority="834" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="433" priority="833" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="432" priority="832" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="431" priority="831" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="430" priority="830" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="429" priority="829" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="428" priority="828" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="427" priority="827" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="426" priority="826" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="cellIs" dxfId="425" priority="825" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="424" priority="824" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C40">
     <cfRule type="containsText" dxfId="423" priority="823" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="422" priority="822" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="421" priority="821" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="420" priority="820" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="419" priority="819" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="418" priority="818" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="417" priority="817" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="416" priority="816" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="415" priority="815" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="414" priority="814" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="413" priority="813" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="412" priority="812" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="411" priority="811" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="410" priority="810" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="409" priority="809" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="408" priority="808" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="407" priority="807" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="406" priority="806" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="405" priority="805" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="404" priority="804" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="403" priority="803" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="402" priority="802" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="401" priority="801" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="400" priority="800" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="399" priority="799" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="398" priority="798" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="397" priority="797" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="396" priority="796" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="395" priority="795" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="394" priority="794" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="393" priority="793" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="392" priority="792" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="391" priority="791" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="390" priority="790" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="389" priority="789" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="388" priority="788" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="387" priority="787" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="386" priority="786" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="385" priority="785" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="384" priority="784" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="383" priority="750" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="382" priority="749" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="381" priority="748" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="380" priority="780" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="379" priority="779" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="378" priority="778" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="377" priority="777" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="376" priority="776" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="375" priority="775" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="374" priority="774" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="373" priority="773" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="372" priority="772" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="371" priority="771" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="370" priority="770" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="369" priority="769" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="368" priority="768" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="367" priority="767" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="366" priority="766" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="365" priority="765" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="364" priority="764" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="363" priority="763" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="362" priority="762" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="361" priority="761" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="360" priority="760" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="359" priority="759" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="358" priority="758" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="357" priority="757" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="356" priority="756" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="355" priority="755" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="354" priority="754" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="353" priority="753" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="352" priority="752" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="351" priority="751" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="350" priority="747" operator="equal">
+    <cfRule type="cellIs" dxfId="422" priority="819" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="349" priority="746" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="421" priority="818" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="348" priority="745" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="420" priority="817" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="347" priority="744" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="816" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="346" priority="743" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="418" priority="815" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="345" priority="742" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="417" priority="814" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="344" priority="678" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="750" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="343" priority="677" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="415" priority="749" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="342" priority="676" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="414" priority="748" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="341" priority="708" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="780" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="340" priority="707" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="412" priority="779" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="339" priority="706" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="411" priority="778" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="338" priority="705" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="777" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="337" priority="704" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="409" priority="776" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="336" priority="703" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="408" priority="775" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="335" priority="702" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="774" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="334" priority="701" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="406" priority="773" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="333" priority="700" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="405" priority="772" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="332" priority="699" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="771" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="331" priority="698" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="403" priority="770" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="330" priority="697" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="402" priority="769" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="329" priority="696" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="768" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="328" priority="695" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="400" priority="767" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="327" priority="694" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="399" priority="766" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="326" priority="693" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="765" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="325" priority="692" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="397" priority="764" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="324" priority="691" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="396" priority="763" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="323" priority="690" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="762" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="322" priority="689" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="394" priority="761" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="321" priority="688" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="393" priority="760" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="320" priority="687" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="759" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="319" priority="686" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="391" priority="758" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="318" priority="685" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="390" priority="757" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="317" priority="684" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="756" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="316" priority="683" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="388" priority="755" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="315" priority="682" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="387" priority="754" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="314" priority="681" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="753" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="313" priority="680" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="385" priority="752" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="312" priority="679" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="384" priority="751" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="311" priority="573" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="645" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="310" priority="572" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="644" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="309" priority="571" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="643" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="308" priority="603" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="675" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="307" priority="602" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="674" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="306" priority="601" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="673" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="305" priority="600" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="672" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="304" priority="599" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="671" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="303" priority="598" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="670" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="302" priority="597" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="669" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="301" priority="596" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="668" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="300" priority="595" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="667" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="299" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="666" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="298" priority="593" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="665" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="297" priority="592" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="664" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="296" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="663" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="295" priority="590" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="662" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="294" priority="589" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="661" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="293" priority="588" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="660" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="292" priority="587" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="659" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="291" priority="586" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="658" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="290" priority="585" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="657" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="289" priority="584" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="656" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="288" priority="583" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="655" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="287" priority="582" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="654" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="286" priority="581" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="358" priority="653" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="285" priority="580" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="357" priority="652" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="284" priority="579" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="651" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="283" priority="578" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="355" priority="650" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="282" priority="577" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="354" priority="649" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="281" priority="576" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="648" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="280" priority="575" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="647" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="279" priority="574" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="646" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="278" priority="570" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="642" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="277" priority="569" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="641" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="276" priority="568" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="640" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="275" priority="537" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="609" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="274" priority="536" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="608" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="273" priority="535" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="607" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="272" priority="567" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="639" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="271" priority="566" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="638" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="270" priority="565" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="637" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="269" priority="564" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="636" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="268" priority="563" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="635" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="267" priority="562" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="634" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="266" priority="561" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="633" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="265" priority="560" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="632" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="264" priority="559" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="631" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="263" priority="558" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="262" priority="557" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="261" priority="556" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="260" priority="555" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="259" priority="554" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="258" priority="553" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="257" priority="552" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="624" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="256" priority="551" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="623" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="255" priority="550" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="622" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="254" priority="549" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="621" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="253" priority="548" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="620" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="252" priority="547" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="619" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="251" priority="546" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="250" priority="545" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="249" priority="544" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="248" priority="543" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="615" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="247" priority="542" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="614" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="246" priority="541" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="613" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="245" priority="540" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="612" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="244" priority="539" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="611" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="243" priority="538" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="610" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="242" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="540" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="241" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="539" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="240" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="538" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="239" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="570" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="238" priority="497" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="569" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="237" priority="496" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="568" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="236" priority="495" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="567" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="235" priority="494" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="566" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="234" priority="493" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="565" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="233" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="564" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="232" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="563" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="231" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="562" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="230" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="561" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="229" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="560" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="228" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="559" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="227" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="558" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="226" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="557" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="225" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="556" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="224" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="555" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="223" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="554" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="222" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="553" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="221" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="552" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="220" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="551" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="219" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="550" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="218" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="549" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="217" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="548" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="216" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="547" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="215" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="546" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="214" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="286" priority="545" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="213" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="285" priority="544" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="212" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="543" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="211" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="283" priority="542" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="210" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="282" priority="541" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="209" priority="366" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="438" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="208" priority="365" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="280" priority="437" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="207" priority="364" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="279" priority="436" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="206" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="468" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="205" priority="395" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="277" priority="467" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="204" priority="394" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="276" priority="466" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="203" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="465" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="202" priority="392" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="274" priority="464" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="201" priority="391" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="273" priority="463" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="200" priority="390" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="462" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="199" priority="389" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="271" priority="461" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="198" priority="388" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="270" priority="460" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="197" priority="387" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="459" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="196" priority="386" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="268" priority="458" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="195" priority="385" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="267" priority="457" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="194" priority="384" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="456" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="193" priority="383" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="265" priority="455" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="192" priority="382" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="264" priority="454" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="191" priority="381" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="453" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="190" priority="380" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="262" priority="452" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="189" priority="379" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="261" priority="451" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="188" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="450" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="187" priority="377" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="259" priority="449" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="186" priority="376" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="258" priority="448" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="185" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="447" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="184" priority="374" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="256" priority="446" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="183" priority="373" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="255" priority="445" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="182" priority="372" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="444" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="181" priority="371" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="253" priority="443" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="180" priority="370" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="252" priority="442" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="179" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="441" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="178" priority="368" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="440" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="177" priority="367" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="439" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="176" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="324" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="175" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="323" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="174" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="322" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="173" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="354" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="172" priority="281" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="353" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="171" priority="280" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="352" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="170" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="351" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="169" priority="278" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="350" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="168" priority="277" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="349" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="167" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="348" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="166" priority="275" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="347" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="165" priority="274" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="346" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="164" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="345" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="163" priority="272" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="344" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="162" priority="271" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="343" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="161" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="342" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="160" priority="269" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="341" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="159" priority="268" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="340" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="158" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="339" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="157" priority="266" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="338" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="156" priority="265" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="337" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="155" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="336" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="154" priority="263" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="335" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="153" priority="262" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="334" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="152" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="333" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="151" priority="260" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="332" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="150" priority="259" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="331" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="149" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="330" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="148" priority="257" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="329" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="147" priority="256" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="328" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="146" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="327" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="145" priority="254" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="326" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="144" priority="253" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="325" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="143" priority="180" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="142" priority="179" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="215" priority="252" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="214" priority="251" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="141" priority="178" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="213" priority="250" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="140" priority="147" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="139" priority="146" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="212" priority="219" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="211" priority="218" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="138" priority="145" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="210" priority="217" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="137" priority="177" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="136" priority="176" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="209" priority="249" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="208" priority="248" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="135" priority="175" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="207" priority="247" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="134" priority="174" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="133" priority="173" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="206" priority="246" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="205" priority="245" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="132" priority="172" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="204" priority="244" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="131" priority="171" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="130" priority="170" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="203" priority="243" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="202" priority="242" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="129" priority="169" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="201" priority="241" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="128" priority="168" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="127" priority="167" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="200" priority="240" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="199" priority="239" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="126" priority="166" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="198" priority="238" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="125" priority="165" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="124" priority="164" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="197" priority="237" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="196" priority="236" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="123" priority="163" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="195" priority="235" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="122" priority="162" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="121" priority="161" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="194" priority="234" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="193" priority="233" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="120" priority="160" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="192" priority="232" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="119" priority="159" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="118" priority="158" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="191" priority="231" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="190" priority="230" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="117" priority="157" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="189" priority="229" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="116" priority="156" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="115" priority="155" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="188" priority="228" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="187" priority="227" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="114" priority="154" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="186" priority="226" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="113" priority="153" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="112" priority="152" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="185" priority="225" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="184" priority="224" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="111" priority="151" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="183" priority="223" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="cellIs" dxfId="110" priority="150" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="109" priority="149" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="cellIs" dxfId="182" priority="222" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="181" priority="221" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C61">
-    <cfRule type="containsText" dxfId="108" priority="148" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C62">
+    <cfRule type="containsText" dxfId="180" priority="220" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="107" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="106" priority="113" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="105" priority="112" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="104" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="216" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="103" priority="143" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="215" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="102" priority="142" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="214" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="101" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="213" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="100" priority="140" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="212" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="99" priority="139" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="211" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="98" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="210" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="97" priority="137" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="209" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="96" priority="136" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="208" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="95" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="207" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="94" priority="134" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="206" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="93" priority="133" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="205" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="92" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="91" priority="131" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="90" priority="130" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="89" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="88" priority="128" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="87" priority="127" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="86" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="198" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="85" priority="125" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="197" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="84" priority="124" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="196" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="83" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="195" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="82" priority="122" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="194" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="81" priority="121" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="193" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="80" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="192" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="79" priority="119" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="191" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="78" priority="118" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="190" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="77" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="189" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="76" priority="116" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="188" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="75" priority="115" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="187" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="147" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="108" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="142" priority="107" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="141" priority="106" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="75" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="139" priority="74" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="138" priority="73" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="137" priority="105" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="136" priority="104" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="135" priority="103" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="134" priority="102" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="133" priority="101" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="132" priority="100" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="131" priority="99" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="130" priority="98" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="129" priority="97" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="128" priority="96" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="127" priority="95" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="126" priority="94" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="125" priority="93" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="124" priority="92" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="123" priority="91" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="122" priority="90" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="121" priority="89" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="120" priority="88" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="119" priority="87" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="118" priority="86" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="117" priority="85" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="116" priority="84" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="115" priority="83" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="114" priority="82" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="113" priority="81" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="112" priority="80" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="111" priority="79" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="cellIs" dxfId="110" priority="78" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="109" priority="77" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="containsText" dxfId="108" priority="76" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="34" priority="5" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="cellIs" dxfId="32" priority="36" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="31" priority="35" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="30" priority="34" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
     <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Dashboard, navigation, header, footer, pages
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E266AB-7246-8145-B208-5BF18285FC1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323314FA-BB24-164C-9ACE-89CF43FC5219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planning &amp; Journal" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Planning &amp; Journal'!$C$1:$F$69</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="81">
   <si>
     <t>Tâche</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>[S2] Epic 2 : Gestion de profil</t>
+  </si>
+  <si>
+    <t>Mise en place du dashboard et de la navigation</t>
   </si>
 </sst>
 </file>
@@ -7182,11 +7185,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K59" sqref="K59"/>
+      <selection pane="topRight" activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8432,7 +8435,7 @@
         <v>2</v>
       </c>
       <c r="F59" s="8">
-        <f>E59/D59</f>
+        <f t="shared" ref="F59:F65" si="20">E59/D59</f>
         <v>1</v>
       </c>
     </row>
@@ -8453,7 +8456,7 @@
         <v>2</v>
       </c>
       <c r="F60" s="8">
-        <f>E60/D60</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
@@ -8474,7 +8477,7 @@
         <v>8</v>
       </c>
       <c r="F61" s="8">
-        <f>E61/D61</f>
+        <f t="shared" si="20"/>
         <v>1</v>
       </c>
     </row>
@@ -8495,7 +8498,7 @@
         <v>1</v>
       </c>
       <c r="F62" s="8">
-        <f>E62/D62</f>
+        <f t="shared" si="20"/>
         <v>0.5</v>
       </c>
     </row>
@@ -8516,7 +8519,7 @@
         <v>5</v>
       </c>
       <c r="F63" s="8">
-        <f>E63/D63</f>
+        <f t="shared" si="20"/>
         <v>1.25</v>
       </c>
     </row>
@@ -8525,56 +8528,60 @@
         <v>12</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C64" s="9" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="D64" s="9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F64" s="8">
-        <f>E64/D64</f>
-        <v>0</v>
+        <f t="shared" ref="F64" si="21">E64/D64</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="7"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="9"/>
-      <c r="F65" s="8"/>
+      <c r="A65" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65" s="9">
+        <v>8</v>
+      </c>
+      <c r="E65">
+        <v>2</v>
+      </c>
+      <c r="F65" s="8">
+        <f t="shared" si="20"/>
+        <v>0.25</v>
+      </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D66" s="2">
-        <v>15</v>
-      </c>
-      <c r="E66" s="2"/>
-      <c r="F66" s="8">
-        <f>E66/D66</f>
-        <v>0</v>
-      </c>
+      <c r="A66" s="7"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9"/>
+      <c r="F66" s="8"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D67" s="2">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="8">
@@ -8582,3040 +8589,3057 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="9" t="s">
         <v>22</v>
       </c>
       <c r="D68" s="2">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="E68" s="2"/>
       <c r="F68" s="8">
         <f>E68/D68</f>
         <v>0</v>
       </c>
-      <c r="H68"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="10"/>
-      <c r="B69" s="17"/>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-      <c r="E69" s="17"/>
-      <c r="F69" s="18"/>
+    <row r="69" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D69" s="2">
+        <v>40</v>
+      </c>
+      <c r="E69" s="2"/>
+      <c r="F69" s="8">
+        <f>E69/D69</f>
+        <v>0</v>
+      </c>
+      <c r="H69"/>
     </row>
-    <row r="70" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="13" t="s">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="10"/>
+      <c r="B70" s="17"/>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17"/>
+      <c r="E70" s="17"/>
+      <c r="F70" s="18"/>
+    </row>
+    <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="11"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D70" s="14">
-        <f>SUM(D2:D69)</f>
-        <v>464</v>
-      </c>
-      <c r="E70" s="14">
-        <f>SUM(E2:E69)</f>
-        <v>256.5</v>
-      </c>
-      <c r="F70" s="15">
-        <f>E70/D70</f>
-        <v>0.55280172413793105</v>
-      </c>
-      <c r="H70" s="1"/>
+      <c r="D71" s="14">
+        <f>SUM(D2:D70)</f>
+        <v>468</v>
+      </c>
+      <c r="E71" s="14">
+        <f>SUM(E2:E70)</f>
+        <v>260.5</v>
+      </c>
+      <c r="F71" s="15">
+        <f>E71/D71</f>
+        <v>0.55662393162393164</v>
+      </c>
+      <c r="H71" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:F68" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
+  <autoFilter ref="C1:F69" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B69:F69"/>
+    <mergeCell ref="B70:F70"/>
   </mergeCells>
-  <conditionalFormatting sqref="C71:C1048576 C1:C7 C11:C13 C9 C66:C68">
-    <cfRule type="cellIs" dxfId="632" priority="1178" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C70:C1048576 C1:C7 C11:C13 C9 C66:C68">
-    <cfRule type="containsText" dxfId="631" priority="1176" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C72:C1048576 C1:C7 C11:C13 C9 C67:C69">
+    <cfRule type="cellIs" dxfId="632" priority="1214" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71:C1048576 C1:C7 C11:C13 C9 C67:C69">
+    <cfRule type="containsText" dxfId="631" priority="1212" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C66:C1048576">
-    <cfRule type="containsText" dxfId="630" priority="1175" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C67:C1048576">
+    <cfRule type="containsText" dxfId="630" priority="1211" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="629" priority="1170" operator="equal">
+    <cfRule type="cellIs" dxfId="629" priority="1206" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="628" priority="1169" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="628" priority="1205" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="627" priority="1168" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="627" priority="1204" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="626" priority="1158" operator="equal">
+    <cfRule type="cellIs" dxfId="626" priority="1194" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="625" priority="1157" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="625" priority="1193" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="624" priority="1156" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="624" priority="1192" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="623" priority="1149" operator="equal">
+    <cfRule type="cellIs" dxfId="623" priority="1185" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="622" priority="1148" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="622" priority="1184" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="621" priority="1147" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="621" priority="1183" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="620" priority="1146" operator="equal">
+    <cfRule type="cellIs" dxfId="620" priority="1182" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="619" priority="1145" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="619" priority="1181" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="618" priority="1144" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="618" priority="1180" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="617" priority="1125" operator="equal">
+    <cfRule type="cellIs" dxfId="617" priority="1161" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="616" priority="1124" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="616" priority="1160" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="615" priority="1123" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="615" priority="1159" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="614" priority="1116" operator="equal">
+    <cfRule type="cellIs" dxfId="614" priority="1152" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="613" priority="1115" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="613" priority="1151" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="612" priority="1114" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="612" priority="1150" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="611" priority="1095" operator="equal">
+    <cfRule type="cellIs" dxfId="611" priority="1131" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="610" priority="1094" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="610" priority="1130" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="609" priority="1093" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="609" priority="1129" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="608" priority="1092" operator="equal">
+    <cfRule type="cellIs" dxfId="608" priority="1128" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="607" priority="1091" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="607" priority="1127" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="606" priority="1090" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="606" priority="1126" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="605" priority="1077" operator="equal">
+    <cfRule type="cellIs" dxfId="605" priority="1113" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="604" priority="1076" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="604" priority="1112" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="603" priority="1075" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="603" priority="1111" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="602" priority="1074" operator="equal">
+    <cfRule type="cellIs" dxfId="602" priority="1110" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="601" priority="1073" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="601" priority="1109" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="600" priority="1072" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="600" priority="1108" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="599" priority="1071" operator="equal">
+    <cfRule type="cellIs" dxfId="599" priority="1107" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="598" priority="1070" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="598" priority="1106" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="597" priority="1069" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="597" priority="1105" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="596" priority="1068" operator="equal">
+    <cfRule type="cellIs" dxfId="596" priority="1104" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="595" priority="1067" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="595" priority="1103" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="594" priority="1066" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="594" priority="1102" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="593" priority="1065" operator="equal">
+    <cfRule type="cellIs" dxfId="593" priority="1101" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="592" priority="1064" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="592" priority="1100" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="591" priority="1063" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="591" priority="1099" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="590" priority="1062" operator="equal">
+    <cfRule type="cellIs" dxfId="590" priority="1098" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="589" priority="1061" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="589" priority="1097" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="588" priority="1060" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="588" priority="1096" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="587" priority="1059" operator="equal">
+    <cfRule type="cellIs" dxfId="587" priority="1095" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="586" priority="1058" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="586" priority="1094" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="585" priority="1057" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="585" priority="1093" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="584" priority="1056" operator="equal">
+    <cfRule type="cellIs" dxfId="584" priority="1092" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="583" priority="1055" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="583" priority="1091" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="582" priority="1054" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="582" priority="1090" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="581" priority="1053" operator="equal">
+    <cfRule type="cellIs" dxfId="581" priority="1089" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="580" priority="1052" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="580" priority="1088" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="579" priority="1051" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="579" priority="1087" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="578" priority="1050" operator="equal">
+    <cfRule type="cellIs" dxfId="578" priority="1086" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="577" priority="1049" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="577" priority="1085" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="576" priority="1048" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="576" priority="1084" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="575" priority="1047" operator="equal">
+    <cfRule type="cellIs" dxfId="575" priority="1083" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="574" priority="1046" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="574" priority="1082" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="573" priority="1045" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="573" priority="1081" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="572" priority="1044" operator="equal">
+    <cfRule type="cellIs" dxfId="572" priority="1080" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="571" priority="1043" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="571" priority="1079" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="570" priority="1042" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="570" priority="1078" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="569" priority="1041" operator="equal">
+    <cfRule type="cellIs" dxfId="569" priority="1077" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="568" priority="1040" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="568" priority="1076" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="567" priority="1039" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="567" priority="1075" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="566" priority="1038" operator="equal">
+    <cfRule type="cellIs" dxfId="566" priority="1074" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="565" priority="1037" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="565" priority="1073" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="564" priority="1036" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="564" priority="1072" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="563" priority="1035" operator="equal">
+    <cfRule type="cellIs" dxfId="563" priority="1071" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="562" priority="1034" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="562" priority="1070" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="561" priority="1033" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="561" priority="1069" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="560" priority="1032" operator="equal">
+    <cfRule type="cellIs" dxfId="560" priority="1068" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="559" priority="1031" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="559" priority="1067" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="558" priority="1030" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="558" priority="1066" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="557" priority="1029" operator="equal">
+    <cfRule type="cellIs" dxfId="557" priority="1065" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="556" priority="1028" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="556" priority="1064" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="555" priority="1027" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="555" priority="1063" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="554" priority="1026" operator="equal">
+    <cfRule type="cellIs" dxfId="554" priority="1062" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="553" priority="1025" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="553" priority="1061" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="552" priority="1024" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="552" priority="1060" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="551" priority="1023" operator="equal">
+    <cfRule type="cellIs" dxfId="551" priority="1059" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="550" priority="1022" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="550" priority="1058" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="549" priority="1021" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="549" priority="1057" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="548" priority="1020" operator="equal">
+    <cfRule type="cellIs" dxfId="548" priority="1056" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="547" priority="1019" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="547" priority="1055" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="546" priority="1018" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="546" priority="1054" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="545" priority="1017" operator="equal">
+    <cfRule type="cellIs" dxfId="545" priority="1053" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="544" priority="1016" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="544" priority="1052" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="543" priority="1015" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="543" priority="1051" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="542" priority="1014" operator="equal">
+    <cfRule type="cellIs" dxfId="542" priority="1050" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="541" priority="1013" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="541" priority="1049" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="540" priority="1012" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="540" priority="1048" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="539" priority="1011" operator="equal">
+    <cfRule type="cellIs" dxfId="539" priority="1047" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="538" priority="1010" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="538" priority="1046" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="537" priority="1009" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="537" priority="1045" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="536" priority="1008" operator="equal">
+    <cfRule type="cellIs" dxfId="536" priority="1044" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="535" priority="1007" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="535" priority="1043" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="534" priority="1006" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="534" priority="1042" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="533" priority="1005" operator="equal">
+    <cfRule type="cellIs" dxfId="533" priority="1041" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="532" priority="1004" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="532" priority="1040" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="531" priority="1003" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="531" priority="1039" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="530" priority="1002" operator="equal">
+    <cfRule type="cellIs" dxfId="530" priority="1038" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="529" priority="1001" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="529" priority="1037" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="528" priority="1000" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="528" priority="1036" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="527" priority="966" operator="equal">
+    <cfRule type="cellIs" dxfId="527" priority="1002" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="526" priority="965" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="526" priority="1001" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="525" priority="964" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="525" priority="1000" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="524" priority="996" operator="equal">
+    <cfRule type="cellIs" dxfId="524" priority="1032" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="523" priority="995" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="523" priority="1031" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="522" priority="994" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="522" priority="1030" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="521" priority="993" operator="equal">
+    <cfRule type="cellIs" dxfId="521" priority="1029" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="520" priority="992" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="520" priority="1028" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="519" priority="991" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="519" priority="1027" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="518" priority="990" operator="equal">
+    <cfRule type="cellIs" dxfId="518" priority="1026" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="517" priority="989" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="517" priority="1025" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="516" priority="988" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="516" priority="1024" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="515" priority="987" operator="equal">
+    <cfRule type="cellIs" dxfId="515" priority="1023" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="514" priority="986" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="514" priority="1022" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="513" priority="985" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="513" priority="1021" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="512" priority="984" operator="equal">
+    <cfRule type="cellIs" dxfId="512" priority="1020" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="511" priority="983" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="511" priority="1019" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="510" priority="982" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="510" priority="1018" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="509" priority="981" operator="equal">
+    <cfRule type="cellIs" dxfId="509" priority="1017" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="508" priority="980" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="508" priority="1016" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="507" priority="979" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="507" priority="1015" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="506" priority="978" operator="equal">
+    <cfRule type="cellIs" dxfId="506" priority="1014" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="505" priority="977" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="505" priority="1013" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="504" priority="976" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="504" priority="1012" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="503" priority="975" operator="equal">
+    <cfRule type="cellIs" dxfId="503" priority="1011" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="502" priority="974" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="502" priority="1010" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="501" priority="973" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="501" priority="1009" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="500" priority="972" operator="equal">
+    <cfRule type="cellIs" dxfId="500" priority="1008" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="499" priority="971" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="499" priority="1007" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="498" priority="970" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="498" priority="1006" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="497" priority="969" operator="equal">
+    <cfRule type="cellIs" dxfId="497" priority="1005" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="496" priority="968" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="496" priority="1004" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="495" priority="967" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="495" priority="1003" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="494" priority="963" operator="equal">
+    <cfRule type="cellIs" dxfId="494" priority="999" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="493" priority="962" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="493" priority="998" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="492" priority="961" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="492" priority="997" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="491" priority="960" operator="equal">
+    <cfRule type="cellIs" dxfId="491" priority="996" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="490" priority="959" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="490" priority="995" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="489" priority="958" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="489" priority="994" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="488" priority="894" operator="equal">
+    <cfRule type="cellIs" dxfId="488" priority="930" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="487" priority="893" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="487" priority="929" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="486" priority="892" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="486" priority="928" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="485" priority="924" operator="equal">
+    <cfRule type="cellIs" dxfId="485" priority="960" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="484" priority="923" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="484" priority="959" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="483" priority="922" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="483" priority="958" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="482" priority="921" operator="equal">
+    <cfRule type="cellIs" dxfId="482" priority="957" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="481" priority="920" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="481" priority="956" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="480" priority="919" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="480" priority="955" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="479" priority="918" operator="equal">
+    <cfRule type="cellIs" dxfId="479" priority="954" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="478" priority="917" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="478" priority="953" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="477" priority="916" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="477" priority="952" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="476" priority="915" operator="equal">
+    <cfRule type="cellIs" dxfId="476" priority="951" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="475" priority="914" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="475" priority="950" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="474" priority="913" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="474" priority="949" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="473" priority="912" operator="equal">
+    <cfRule type="cellIs" dxfId="473" priority="948" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="472" priority="911" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="472" priority="947" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="471" priority="910" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="471" priority="946" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="470" priority="909" operator="equal">
+    <cfRule type="cellIs" dxfId="470" priority="945" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="469" priority="908" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="469" priority="944" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="468" priority="907" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="468" priority="943" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="467" priority="906" operator="equal">
+    <cfRule type="cellIs" dxfId="467" priority="942" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="466" priority="905" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="466" priority="941" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="465" priority="904" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="465" priority="940" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="464" priority="903" operator="equal">
+    <cfRule type="cellIs" dxfId="464" priority="939" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="463" priority="902" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="463" priority="938" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="462" priority="901" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="462" priority="937" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="461" priority="900" operator="equal">
+    <cfRule type="cellIs" dxfId="461" priority="936" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="460" priority="899" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="460" priority="935" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="459" priority="898" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="459" priority="934" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="458" priority="897" operator="equal">
+    <cfRule type="cellIs" dxfId="458" priority="933" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="457" priority="896" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="457" priority="932" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="456" priority="895" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="456" priority="931" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="455" priority="789" operator="equal">
+    <cfRule type="cellIs" dxfId="455" priority="825" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="454" priority="788" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="454" priority="824" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="453" priority="787" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="453" priority="823" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="452" priority="819" operator="equal">
+    <cfRule type="cellIs" dxfId="452" priority="855" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="451" priority="818" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="451" priority="854" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="450" priority="817" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="450" priority="853" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="449" priority="816" operator="equal">
+    <cfRule type="cellIs" dxfId="449" priority="852" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="448" priority="815" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="448" priority="851" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="447" priority="814" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="447" priority="850" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="446" priority="813" operator="equal">
+    <cfRule type="cellIs" dxfId="446" priority="849" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="445" priority="812" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="445" priority="848" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="444" priority="811" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="444" priority="847" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="443" priority="810" operator="equal">
+    <cfRule type="cellIs" dxfId="443" priority="846" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="442" priority="809" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="442" priority="845" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="441" priority="808" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="441" priority="844" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="440" priority="807" operator="equal">
+    <cfRule type="cellIs" dxfId="440" priority="843" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="439" priority="806" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="439" priority="842" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="438" priority="805" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="438" priority="841" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="437" priority="804" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="840" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="436" priority="803" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="436" priority="839" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="435" priority="802" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="435" priority="838" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="434" priority="801" operator="equal">
+    <cfRule type="cellIs" dxfId="434" priority="837" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="433" priority="800" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="433" priority="836" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="432" priority="799" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="432" priority="835" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="431" priority="798" operator="equal">
+    <cfRule type="cellIs" dxfId="431" priority="834" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="430" priority="797" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="430" priority="833" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="429" priority="796" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="429" priority="832" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="428" priority="795" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="831" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="427" priority="794" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="427" priority="830" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="426" priority="793" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="426" priority="829" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="425" priority="792" operator="equal">
+    <cfRule type="cellIs" dxfId="425" priority="828" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="424" priority="791" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="424" priority="827" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="423" priority="790" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="423" priority="826" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="422" priority="786" operator="equal">
+    <cfRule type="cellIs" dxfId="422" priority="822" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="421" priority="785" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="421" priority="821" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="420" priority="784" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="420" priority="820" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="419" priority="753" operator="equal">
+    <cfRule type="cellIs" dxfId="419" priority="789" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="418" priority="752" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="418" priority="788" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="417" priority="751" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="417" priority="787" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="416" priority="783" operator="equal">
+    <cfRule type="cellIs" dxfId="416" priority="819" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="415" priority="782" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="415" priority="818" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="414" priority="781" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="414" priority="817" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="413" priority="780" operator="equal">
+    <cfRule type="cellIs" dxfId="413" priority="816" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="412" priority="779" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="412" priority="815" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="411" priority="778" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="411" priority="814" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="410" priority="777" operator="equal">
+    <cfRule type="cellIs" dxfId="410" priority="813" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="409" priority="776" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="409" priority="812" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="408" priority="775" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="408" priority="811" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="407" priority="774" operator="equal">
+    <cfRule type="cellIs" dxfId="407" priority="810" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="406" priority="773" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="406" priority="809" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="405" priority="772" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="405" priority="808" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="404" priority="771" operator="equal">
+    <cfRule type="cellIs" dxfId="404" priority="807" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="403" priority="770" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="403" priority="806" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="402" priority="769" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="402" priority="805" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="401" priority="768" operator="equal">
+    <cfRule type="cellIs" dxfId="401" priority="804" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="400" priority="767" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="400" priority="803" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="399" priority="766" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="399" priority="802" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="398" priority="765" operator="equal">
+    <cfRule type="cellIs" dxfId="398" priority="801" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="397" priority="764" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="397" priority="800" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="396" priority="763" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="396" priority="799" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="395" priority="762" operator="equal">
+    <cfRule type="cellIs" dxfId="395" priority="798" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="394" priority="761" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="394" priority="797" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="393" priority="760" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="393" priority="796" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="392" priority="759" operator="equal">
+    <cfRule type="cellIs" dxfId="392" priority="795" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="391" priority="758" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="391" priority="794" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="390" priority="757" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="390" priority="793" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="389" priority="756" operator="equal">
+    <cfRule type="cellIs" dxfId="389" priority="792" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="388" priority="755" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="388" priority="791" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="387" priority="754" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="387" priority="790" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="386" priority="684" operator="equal">
+    <cfRule type="cellIs" dxfId="386" priority="720" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="385" priority="683" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="385" priority="719" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="384" priority="682" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="384" priority="718" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="383" priority="714" operator="equal">
+    <cfRule type="cellIs" dxfId="383" priority="750" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="382" priority="713" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="382" priority="749" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="381" priority="712" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="381" priority="748" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="380" priority="711" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="747" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="379" priority="710" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="379" priority="746" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="378" priority="709" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="378" priority="745" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="377" priority="708" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="744" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="376" priority="707" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="376" priority="743" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="375" priority="706" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="375" priority="742" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="374" priority="705" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="741" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="373" priority="704" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="373" priority="740" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="372" priority="703" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="372" priority="739" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="371" priority="702" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="738" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="370" priority="701" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="370" priority="737" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="369" priority="700" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="369" priority="736" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="368" priority="699" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="735" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="367" priority="698" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="367" priority="734" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="366" priority="697" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="366" priority="733" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="365" priority="696" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="732" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="364" priority="695" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="364" priority="731" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="363" priority="694" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="363" priority="730" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="362" priority="693" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="729" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="361" priority="692" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="361" priority="728" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="360" priority="691" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="360" priority="727" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="359" priority="690" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="726" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="358" priority="689" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="358" priority="725" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="357" priority="688" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="357" priority="724" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="356" priority="687" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="723" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="355" priority="686" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="355" priority="722" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="354" priority="685" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="354" priority="721" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="353" priority="582" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="618" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="352" priority="581" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="352" priority="617" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="351" priority="580" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="351" priority="616" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="350" priority="612" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="648" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="349" priority="611" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="349" priority="647" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="348" priority="610" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="348" priority="646" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="347" priority="609" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="645" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="346" priority="608" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="346" priority="644" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="345" priority="607" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="345" priority="643" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="344" priority="606" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="642" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="343" priority="605" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="343" priority="641" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="342" priority="604" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="342" priority="640" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="341" priority="603" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="639" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="340" priority="602" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="340" priority="638" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="339" priority="601" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="339" priority="637" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="338" priority="600" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="636" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="337" priority="599" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="337" priority="635" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="336" priority="598" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="336" priority="634" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="335" priority="597" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="633" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="334" priority="596" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="334" priority="632" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="333" priority="595" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="333" priority="631" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="332" priority="594" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="630" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="331" priority="593" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="331" priority="629" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="330" priority="592" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="330" priority="628" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="329" priority="591" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="627" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="328" priority="590" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="328" priority="626" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="327" priority="589" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="327" priority="625" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="326" priority="588" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="624" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="325" priority="587" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="325" priority="623" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="324" priority="586" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="324" priority="622" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="cellIs" dxfId="323" priority="585" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="621" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="322" priority="584" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="322" priority="620" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49:C54">
-    <cfRule type="containsText" dxfId="321" priority="583" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="321" priority="619" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="320" priority="468" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="504" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="319" priority="467" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="319" priority="503" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="318" priority="466" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="318" priority="502" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="317" priority="498" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="534" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="316" priority="497" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="316" priority="533" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="315" priority="496" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="315" priority="532" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="314" priority="495" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="531" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="313" priority="494" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="313" priority="530" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="312" priority="493" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="312" priority="529" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="311" priority="492" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="528" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="310" priority="491" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="310" priority="527" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="309" priority="490" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="309" priority="526" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="308" priority="489" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="525" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="307" priority="488" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="307" priority="524" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="306" priority="487" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="306" priority="523" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="305" priority="486" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="522" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="304" priority="485" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="304" priority="521" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="303" priority="484" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="303" priority="520" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="302" priority="483" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="519" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="301" priority="482" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="301" priority="518" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="300" priority="481" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="300" priority="517" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="299" priority="480" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="516" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="298" priority="479" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="298" priority="515" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="297" priority="478" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="297" priority="514" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="296" priority="477" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="513" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="295" priority="476" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="295" priority="512" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="294" priority="475" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="294" priority="511" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="293" priority="474" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="510" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="292" priority="473" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="292" priority="509" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="291" priority="472" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="291" priority="508" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="cellIs" dxfId="290" priority="471" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="507" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="289" priority="470" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="289" priority="506" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C55:C57">
-    <cfRule type="containsText" dxfId="288" priority="469" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="288" priority="505" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="287" priority="396" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="286" priority="395" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="287" priority="432" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="286" priority="431" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="285" priority="394" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="285" priority="430" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="284" priority="363" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="283" priority="362" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="284" priority="399" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="283" priority="398" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="282" priority="361" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="282" priority="397" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="281" priority="393" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="280" priority="392" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="281" priority="429" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="280" priority="428" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="279" priority="391" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="279" priority="427" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="278" priority="390" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="277" priority="389" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="278" priority="426" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="277" priority="425" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="276" priority="388" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="276" priority="424" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="275" priority="387" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="274" priority="386" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="275" priority="423" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="274" priority="422" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="273" priority="385" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="273" priority="421" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="272" priority="384" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="271" priority="383" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="272" priority="420" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="271" priority="419" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="270" priority="382" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="270" priority="418" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="269" priority="381" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="268" priority="380" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="269" priority="417" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="268" priority="416" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="267" priority="379" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="267" priority="415" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="266" priority="378" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="265" priority="377" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="266" priority="414" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="265" priority="413" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="264" priority="376" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="264" priority="412" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="263" priority="375" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="262" priority="374" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="263" priority="411" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="262" priority="410" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="261" priority="373" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="261" priority="409" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="260" priority="372" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="259" priority="371" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="260" priority="408" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="259" priority="407" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="258" priority="370" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="258" priority="406" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="257" priority="369" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="256" priority="368" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="257" priority="405" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="256" priority="404" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="255" priority="367" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="255" priority="403" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="cellIs" dxfId="254" priority="366" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="253" priority="365" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="cellIs" dxfId="254" priority="402" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="253" priority="401" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50 C65">
-    <cfRule type="containsText" dxfId="252" priority="364" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C50 C66">
+    <cfRule type="containsText" dxfId="252" priority="400" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C50)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="251" priority="330" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="366" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="250" priority="329" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="250" priority="365" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="249" priority="328" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="249" priority="364" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="248" priority="360" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="396" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="247" priority="359" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="247" priority="395" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="246" priority="358" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="246" priority="394" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="245" priority="357" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="393" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="244" priority="356" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="244" priority="392" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="243" priority="355" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="243" priority="391" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="242" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="390" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="241" priority="353" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="241" priority="389" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="240" priority="352" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="240" priority="388" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="239" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="387" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="238" priority="350" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="238" priority="386" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="237" priority="349" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="237" priority="385" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="236" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="384" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="235" priority="347" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="235" priority="383" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="234" priority="346" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="234" priority="382" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="233" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="381" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="232" priority="344" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="232" priority="380" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="231" priority="343" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="231" priority="379" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="230" priority="342" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="378" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="229" priority="341" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="229" priority="377" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="228" priority="340" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="228" priority="376" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="227" priority="339" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="375" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="226" priority="338" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="226" priority="374" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="225" priority="337" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="225" priority="373" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="224" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="372" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="223" priority="335" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="223" priority="371" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="222" priority="334" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="222" priority="370" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="221" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="369" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="220" priority="332" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="220" priority="368" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="containsText" dxfId="219" priority="331" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="219" priority="367" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C59)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="cellIs" dxfId="218" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="327" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="containsText" dxfId="217" priority="290" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="217" priority="326" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58:C59">
-    <cfRule type="containsText" dxfId="216" priority="289" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="216" priority="325" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="215" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="288" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="214" priority="251" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="214" priority="287" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="213" priority="250" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="213" priority="286" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="212" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="255" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="211" priority="218" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="211" priority="254" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="210" priority="217" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="210" priority="253" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="209" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="285" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="208" priority="248" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="208" priority="284" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="207" priority="247" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="207" priority="283" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="206" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="282" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="205" priority="245" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="205" priority="281" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="204" priority="244" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="204" priority="280" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="203" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="279" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="202" priority="242" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="202" priority="278" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="201" priority="241" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="201" priority="277" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="200" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="276" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="199" priority="239" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="199" priority="275" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="198" priority="238" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="198" priority="274" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="197" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="273" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="196" priority="236" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="196" priority="272" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="195" priority="235" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="195" priority="271" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="194" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="270" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="193" priority="233" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="193" priority="269" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="192" priority="232" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="192" priority="268" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="191" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="267" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="190" priority="230" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="190" priority="266" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="189" priority="229" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="189" priority="265" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="188" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="264" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="187" priority="227" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="187" priority="263" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="186" priority="226" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="186" priority="262" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="185" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="261" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="184" priority="224" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="184" priority="260" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="183" priority="223" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="183" priority="259" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="cellIs" dxfId="182" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="258" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="181" priority="221" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="181" priority="257" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="containsText" dxfId="180" priority="220" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="180" priority="256" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C60)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="179" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="186" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="178" priority="149" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="178" priority="185" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="177" priority="148" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="177" priority="184" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="176" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="216" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="175" priority="179" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="175" priority="215" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="174" priority="178" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="174" priority="214" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="173" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="213" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="172" priority="176" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="172" priority="212" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="171" priority="175" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="171" priority="211" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="170" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="210" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="169" priority="173" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="169" priority="209" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="168" priority="172" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="168" priority="208" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="167" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="207" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="166" priority="170" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="166" priority="206" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="165" priority="169" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="165" priority="205" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="164" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="204" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="163" priority="167" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="163" priority="203" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="162" priority="166" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="162" priority="202" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="161" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="201" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="160" priority="164" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="160" priority="200" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="159" priority="163" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="159" priority="199" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="158" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="198" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="157" priority="161" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="157" priority="197" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="156" priority="160" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="156" priority="196" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="155" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="195" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="154" priority="158" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="154" priority="194" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="153" priority="157" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="153" priority="193" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="152" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="192" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="151" priority="155" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="151" priority="191" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="150" priority="154" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="150" priority="190" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="149" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="189" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="148" priority="152" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="148" priority="188" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="147" priority="151" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="147" priority="187" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="cellIs" dxfId="146" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="183" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="145" priority="146" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="145" priority="182" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="containsText" dxfId="144" priority="145" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="144" priority="181" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="143" priority="114" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="142" priority="113" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="143" priority="150" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="142" priority="149" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="141" priority="112" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="141" priority="148" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="140" priority="144" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="139" priority="143" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="140" priority="180" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="139" priority="179" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="138" priority="142" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="138" priority="178" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="137" priority="141" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="136" priority="140" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="137" priority="177" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="136" priority="176" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="135" priority="139" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="135" priority="175" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="134" priority="138" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="133" priority="137" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="134" priority="174" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="133" priority="173" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="132" priority="136" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="132" priority="172" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="131" priority="135" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="130" priority="134" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="131" priority="171" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="130" priority="170" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="129" priority="133" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="129" priority="169" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="128" priority="132" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="127" priority="131" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="128" priority="168" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="127" priority="167" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="126" priority="130" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="126" priority="166" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="125" priority="129" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="124" priority="128" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="125" priority="165" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="124" priority="164" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="123" priority="127" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="123" priority="163" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="122" priority="126" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="121" priority="125" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="122" priority="162" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="121" priority="161" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="120" priority="124" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="120" priority="160" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="119" priority="123" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="118" priority="122" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="119" priority="159" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="118" priority="158" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="117" priority="121" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="117" priority="157" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="116" priority="120" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="115" priority="119" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="116" priority="156" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="115" priority="155" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="114" priority="118" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="114" priority="154" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="113" priority="117" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="112" priority="116" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="113" priority="153" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="112" priority="152" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="111" priority="115" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="111" priority="151" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="cellIs" dxfId="110" priority="111" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="109" priority="110" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="110" priority="147" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="109" priority="146" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="containsText" dxfId="108" priority="109" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="containsText" dxfId="108" priority="145" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="107" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="114" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="106" priority="77" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="106" priority="113" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="105" priority="76" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="105" priority="112" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="104" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="144" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="103" priority="107" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="103" priority="143" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="102" priority="106" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="102" priority="142" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="101" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="141" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="100" priority="104" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="100" priority="140" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="99" priority="103" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="99" priority="139" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="98" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="138" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="97" priority="137" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="96" priority="100" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="96" priority="136" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="95" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="135" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="94" priority="134" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="93" priority="97" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="93" priority="133" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="92" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="132" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="91" priority="95" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="91" priority="131" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="90" priority="130" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="89" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="129" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="88" priority="128" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="87" priority="91" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="87" priority="127" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="86" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="126" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="85" priority="89" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="85" priority="125" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="84" priority="88" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="84" priority="124" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="83" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="123" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="82" priority="86" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="82" priority="122" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="81" priority="85" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="81" priority="121" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="80" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="120" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="79" priority="83" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="79" priority="119" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="78" priority="82" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="78" priority="118" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="77" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="117" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="76" priority="80" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="76" priority="116" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="75" priority="79" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="75" priority="115" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="74" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="111" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="73" priority="110" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="72" priority="109" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C62)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="35" priority="36" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="31" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="30" priority="1" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="28" priority="32" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="24" priority="28" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="21" priority="25" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="20" priority="24" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="14" priority="18" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="13" priority="17" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="10" priority="14" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C64)))</formula>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="71" priority="72" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="68" priority="39" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="67" priority="38" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="66" priority="37" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="64" priority="68" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="63" priority="67" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="62" priority="66" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="61" priority="65" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="60" priority="64" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="58" priority="62" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="57" priority="61" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="56" priority="60" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="55" priority="59" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="54" priority="58" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="53" priority="57" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="51" priority="55" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="49" priority="53" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="48" priority="52" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="46" priority="50" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="45" priority="49" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="43" priority="47" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="42" priority="46" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="40" priority="44" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="cellIs" dxfId="38" priority="42" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",C65)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="containsText" dxfId="36" priority="40" operator="containsText" text="à faire">
+      <formula>NOT(ISERROR(SEARCH("à faire",C65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
[S2] Epic 2 : Gestion de profil
Point 1 & 2
</commit_message>
<xml_diff>
--- a/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
+++ b/2.Documentation/Annexes/TB_Planning_Alt-Thibaud.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thibaud/Documents/HEIG/TB/2.Documentation/Annexes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323314FA-BB24-164C-9ACE-89CF43FC5219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB844809-2CA8-1641-9FF9-D1B0B28E028C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19720" xr2:uid="{7F10193E-5A70-1947-998D-BED32ABC87A4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Tâche</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>Mise en place du dashboard et de la navigation</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -7185,11 +7188,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F44D29CA-69C2-AF43-823B-122E05E7E4AF}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I62" sqref="I62"/>
+      <selection pane="topRight" activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7403,11 +7406,11 @@
         <v>8</v>
       </c>
       <c r="E10" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F10" s="8">
         <f t="shared" si="1"/>
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -7739,11 +7742,11 @@
         <v>8</v>
       </c>
       <c r="E26" s="9">
-        <v>7</v>
+        <v>9.5</v>
       </c>
       <c r="F26" s="8">
         <f>E26/D26</f>
-        <v>0.875</v>
+        <v>1.1875</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -8195,17 +8198,17 @@
         <v>74</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="D48" s="9">
         <v>4</v>
       </c>
       <c r="E48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F48" s="8">
         <f t="shared" si="10"/>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -8537,11 +8540,11 @@
         <v>4</v>
       </c>
       <c r="E64">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F64" s="8">
         <f t="shared" ref="F64" si="21">E64/D64</f>
-        <v>0.5</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -8555,14 +8558,14 @@
         <v>53</v>
       </c>
       <c r="D65" s="9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E65">
-        <v>2</v>
+        <v>6.5</v>
       </c>
       <c r="F65" s="8">
         <f t="shared" si="20"/>
-        <v>0.25</v>
+        <v>0.40625</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -8580,14 +8583,11 @@
       <c r="C67" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D67" s="2">
-        <v>15</v>
-      </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="8">
-        <f>E67/D67</f>
-        <v>0</v>
-      </c>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2">
+        <v>10</v>
+      </c>
+      <c r="F67" s="8"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
@@ -8597,16 +8597,13 @@
       <c r="C68" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D68" s="2">
-        <v>120</v>
-      </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="8">
-        <f>E68/D68</f>
-        <v>0</v>
-      </c>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2">
+        <v>90</v>
+      </c>
+      <c r="F68" s="8"/>
     </row>
-    <row r="69" spans="1:8" s="16" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>13</v>
       </c>
@@ -8614,3032 +8611,2879 @@
       <c r="C69" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69" s="2"/>
+      <c r="E69" s="2">
         <v>40</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="8">
-        <f>E69/D69</f>
-        <v>0</v>
-      </c>
+      <c r="F69" s="8"/>
       <c r="H69"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="10"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="17"/>
-      <c r="D70" s="17"/>
-      <c r="E70" s="17"/>
-      <c r="F70" s="18"/>
+    <row r="70" spans="1:8" s="16" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2">
+        <v>40</v>
+      </c>
+      <c r="F70" s="8"/>
+      <c r="H70"/>
     </row>
-    <row r="71" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71" s="12"/>
-      <c r="C71" s="13" t="s">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="10"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="17"/>
+      <c r="F71" s="18"/>
+    </row>
+    <row r="72" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="11"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D71" s="14">
-        <f>SUM(D2:D70)</f>
-        <v>468</v>
-      </c>
-      <c r="E71" s="14">
-        <f>SUM(E2:E70)</f>
-        <v>260.5</v>
-      </c>
-      <c r="F71" s="15">
-        <f>E71/D71</f>
-        <v>0.55662393162393164</v>
-      </c>
-      <c r="H71" s="1"/>
+      <c r="D72" s="14">
+        <f>SUM(D2:D71)</f>
+        <v>301</v>
+      </c>
+      <c r="E72" s="14">
+        <f>SUM(E2:E71)</f>
+        <v>450</v>
+      </c>
+      <c r="F72" s="15">
+        <f>E72/D72</f>
+        <v>1.4950166112956811</v>
+      </c>
+      <c r="H72" s="1"/>
     </row>
   </sheetData>
   <autoFilter ref="C1:F69" xr:uid="{7CC50BEF-57F7-764B-86D8-6AC718604565}"/>
   <mergeCells count="1">
-    <mergeCell ref="B70:F70"/>
+    <mergeCell ref="B71:F71"/>
   </mergeCells>
+  <conditionalFormatting sqref="C73:C1048576 C1:C7 C11:C13 C9 C67:C69">
+    <cfRule type="cellIs" dxfId="599" priority="1217" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C72:C1048576 C1:C7 C11:C13 C9 C67:C69">
-    <cfRule type="cellIs" dxfId="632" priority="1214" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71:C1048576 C1:C7 C11:C13 C9 C67:C69">
-    <cfRule type="containsText" dxfId="631" priority="1212" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="598" priority="1215" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C67:C1048576">
-    <cfRule type="containsText" dxfId="630" priority="1211" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C1:C7 C11:C13 C9 C67:C69 C71:C1048576">
+    <cfRule type="containsText" dxfId="597" priority="1214" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="629" priority="1206" operator="equal">
+    <cfRule type="cellIs" dxfId="596" priority="1209" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="628" priority="1205" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="595" priority="1208" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="containsText" dxfId="627" priority="1204" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="594" priority="1207" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="cellIs" dxfId="626" priority="1194" operator="equal">
+    <cfRule type="cellIs" dxfId="593" priority="1197" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="625" priority="1193" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="592" priority="1196" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C21">
-    <cfRule type="containsText" dxfId="624" priority="1192" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="591" priority="1195" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="cellIs" dxfId="623" priority="1185" operator="equal">
+    <cfRule type="cellIs" dxfId="590" priority="1188" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="622" priority="1184" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="589" priority="1187" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C28">
-    <cfRule type="containsText" dxfId="621" priority="1183" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="588" priority="1186" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="cellIs" dxfId="620" priority="1182" operator="equal">
+    <cfRule type="cellIs" dxfId="587" priority="1185" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="619" priority="1181" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="586" priority="1184" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29">
-    <cfRule type="containsText" dxfId="618" priority="1180" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="585" priority="1183" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="617" priority="1161" operator="equal">
+    <cfRule type="cellIs" dxfId="584" priority="1164" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="616" priority="1160" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="583" priority="1163" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="615" priority="1159" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="582" priority="1162" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="cellIs" dxfId="614" priority="1152" operator="equal">
+    <cfRule type="cellIs" dxfId="581" priority="1155" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="613" priority="1151" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="580" priority="1154" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30:C33">
-    <cfRule type="containsText" dxfId="612" priority="1150" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="579" priority="1153" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="611" priority="1131" operator="equal">
+    <cfRule type="cellIs" dxfId="578" priority="1134" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="610" priority="1130" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="577" priority="1133" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="609" priority="1129" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="576" priority="1132" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="608" priority="1128" operator="equal">
+    <cfRule type="cellIs" dxfId="575" priority="1131" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="607" priority="1127" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="574" priority="1130" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="606" priority="1126" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="573" priority="1129" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="cellIs" dxfId="605" priority="1113" operator="equal">
+    <cfRule type="cellIs" dxfId="572" priority="1116" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="604" priority="1112" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="571" priority="1115" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35:C37">
-    <cfRule type="containsText" dxfId="603" priority="1111" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="570" priority="1114" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="602" priority="1110" operator="equal">
+    <cfRule type="cellIs" dxfId="569" priority="1113" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="601" priority="1109" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="568" priority="1112" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="containsText" dxfId="600" priority="1108" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="567" priority="1111" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C42)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="599" priority="1107" operator="equal">
+    <cfRule type="cellIs" dxfId="566" priority="1110" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="598" priority="1106" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="565" priority="1109" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40">
-    <cfRule type="containsText" dxfId="597" priority="1105" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="564" priority="1108" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="596" priority="1104" operator="equal">
+    <cfRule type="cellIs" dxfId="563" priority="1107" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="595" priority="1103" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="562" priority="1106" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="containsText" dxfId="594" priority="1102" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="561" priority="1105" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="593" priority="1101" operator="equal">
+    <cfRule type="cellIs" dxfId="560" priority="1104" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="592" priority="1100" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="559" priority="1103" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="591" priority="1099" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="558" priority="1102" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="590" priority="1098" operator="equal">
+    <cfRule type="cellIs" dxfId="557" priority="1101" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="589" priority="1097" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="556" priority="1100" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="588" priority="1096" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="555" priority="1099" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="587" priority="1095" operator="equal">
+    <cfRule type="cellIs" dxfId="554" priority="1098" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="586" priority="1094" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="553" priority="1097" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="585" priority="1093" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="552" priority="1096" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="584" priority="1092" operator="equal">
+    <cfRule type="cellIs" dxfId="551" priority="1095" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="583" priority="1091" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="550" priority="1094" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="582" priority="1090" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="549" priority="1093" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="581" priority="1089" operator="equal">
+    <cfRule type="cellIs" dxfId="548" priority="1092" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="580" priority="1088" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="547" priority="1091" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="579" priority="1087" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="546" priority="1090" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="578" priority="1086" operator="equal">
+    <cfRule type="cellIs" dxfId="545" priority="1089" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="577" priority="1085" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="544" priority="1088" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="containsText" dxfId="576" priority="1084" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="543" priority="1087" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="575" priority="1083" operator="equal">
+    <cfRule type="cellIs" dxfId="542" priority="1086" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="574" priority="1082" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="541" priority="1085" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="573" priority="1081" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="540" priority="1084" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="572" priority="1080" operator="equal">
+    <cfRule type="cellIs" dxfId="539" priority="1083" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="571" priority="1079" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="538" priority="1082" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="570" priority="1078" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="537" priority="1081" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="569" priority="1077" operator="equal">
+    <cfRule type="cellIs" dxfId="536" priority="1080" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="568" priority="1076" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="535" priority="1079" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="567" priority="1075" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="534" priority="1078" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="566" priority="1074" operator="equal">
+    <cfRule type="cellIs" dxfId="533" priority="1077" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="565" priority="1073" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="532" priority="1076" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="564" priority="1072" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="531" priority="1075" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="563" priority="1071" operator="equal">
+    <cfRule type="cellIs" dxfId="530" priority="1074" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="562" priority="1070" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="529" priority="1073" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="561" priority="1069" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="528" priority="1072" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="560" priority="1068" operator="equal">
+    <cfRule type="cellIs" dxfId="527" priority="1071" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="559" priority="1067" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="526" priority="1070" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="558" priority="1066" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="525" priority="1069" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="557" priority="1065" operator="equal">
+    <cfRule type="cellIs" dxfId="524" priority="1068" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="556" priority="1064" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="523" priority="1067" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="containsText" dxfId="555" priority="1063" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="522" priority="1066" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C36)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="554" priority="1062" operator="equal">
+    <cfRule type="cellIs" dxfId="521" priority="1065" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="553" priority="1061" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="520" priority="1064" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="552" priority="1060" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="519" priority="1063" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="551" priority="1059" operator="equal">
+    <cfRule type="cellIs" dxfId="518" priority="1062" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="550" priority="1058" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="517" priority="1061" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="549" priority="1057" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="516" priority="1060" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="548" priority="1056" operator="equal">
+    <cfRule type="cellIs" dxfId="515" priority="1059" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="547" priority="1055" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="514" priority="1058" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="546" priority="1054" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="513" priority="1057" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="545" priority="1053" operator="equal">
+    <cfRule type="cellIs" dxfId="512" priority="1056" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="544" priority="1052" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="511" priority="1055" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="543" priority="1051" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="510" priority="1054" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="542" priority="1050" operator="equal">
+    <cfRule type="cellIs" dxfId="509" priority="1053" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="541" priority="1049" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="508" priority="1052" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="540" priority="1048" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="507" priority="1051" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="539" priority="1047" operator="equal">
+    <cfRule type="cellIs" dxfId="506" priority="1050" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="538" priority="1046" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="505" priority="1049" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="537" priority="1045" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="504" priority="1048" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="536" priority="1044" operator="equal">
+    <cfRule type="cellIs" dxfId="503" priority="1047" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="535" priority="1043" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="502" priority="1046" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="534" priority="1042" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="501" priority="1045" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="533" priority="1041" operator="equal">
+    <cfRule type="cellIs" dxfId="500" priority="1044" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="532" priority="1040" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="499" priority="1043" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="531" priority="1039" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="498" priority="1042" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="530" priority="1038" operator="equal">
+    <cfRule type="cellIs" dxfId="497" priority="1041" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="529" priority="1037" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="496" priority="1040" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="containsText" dxfId="528" priority="1036" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="495" priority="1039" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="527" priority="1002" operator="equal">
+    <cfRule type="cellIs" dxfId="494" priority="1005" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="526" priority="1001" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="493" priority="1004" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="525" priority="1000" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="492" priority="1003" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="524" priority="1032" operator="equal">
+    <cfRule type="cellIs" dxfId="491" priority="1035" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="523" priority="1031" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="490" priority="1034" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="522" priority="1030" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="489" priority="1033" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="521" priority="1029" operator="equal">
+    <cfRule type="cellIs" dxfId="488" priority="1032" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="520" priority="1028" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="487" priority="1031" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="519" priority="1027" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="486" priority="1030" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="518" priority="1026" operator="equal">
+    <cfRule type="cellIs" dxfId="485" priority="1029" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="517" priority="1025" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="484" priority="1028" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="516" priority="1024" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="483" priority="1027" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="515" priority="1023" operator="equal">
+    <cfRule type="cellIs" dxfId="482" priority="1026" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="514" priority="1022" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="481" priority="1025" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="513" priority="1021" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="480" priority="1024" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="512" priority="1020" operator="equal">
+    <cfRule type="cellIs" dxfId="479" priority="1023" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="511" priority="1019" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="478" priority="1022" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="510" priority="1018" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="477" priority="1021" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="509" priority="1017" operator="equal">
+    <cfRule type="cellIs" dxfId="476" priority="1020" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="508" priority="1016" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="475" priority="1019" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="507" priority="1015" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="474" priority="1018" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="506" priority="1014" operator="equal">
+    <cfRule type="cellIs" dxfId="473" priority="1017" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="505" priority="1013" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="472" priority="1016" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="504" priority="1012" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="471" priority="1015" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="503" priority="1011" operator="equal">
+    <cfRule type="cellIs" dxfId="470" priority="1014" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="502" priority="1010" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="469" priority="1013" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="501" priority="1009" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="468" priority="1012" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="500" priority="1008" operator="equal">
+    <cfRule type="cellIs" dxfId="467" priority="1011" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="499" priority="1007" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="466" priority="1010" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="498" priority="1006" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="465" priority="1009" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="cellIs" dxfId="497" priority="1005" operator="equal">
+    <cfRule type="cellIs" dxfId="464" priority="1008" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="496" priority="1004" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="463" priority="1007" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="495" priority="1003" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="462" priority="1006" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="494" priority="999" operator="equal">
+    <cfRule type="cellIs" dxfId="461" priority="1002" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="493" priority="998" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="460" priority="1001" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43">
-    <cfRule type="containsText" dxfId="492" priority="997" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="459" priority="1000" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="cellIs" dxfId="491" priority="996" operator="equal">
+    <cfRule type="cellIs" dxfId="458" priority="999" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="490" priority="995" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="457" priority="998" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44">
-    <cfRule type="containsText" dxfId="489" priority="994" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="456" priority="997" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C44)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="488" priority="930" operator="equal">
+    <cfRule type="cellIs" dxfId="455" priority="933" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="487" priority="929" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="454" priority="932" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="486" priority="928" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="453" priority="931" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="485" priority="960" operator="equal">
+    <cfRule type="cellIs" dxfId="452" priority="963" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="484" priority="959" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="451" priority="962" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="483" priority="958" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="450" priority="961" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="482" priority="957" operator="equal">
+    <cfRule type="cellIs" dxfId="449" priority="960" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="481" priority="956" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="448" priority="959" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="480" priority="955" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="447" priority="958" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="479" priority="954" operator="equal">
+    <cfRule type="cellIs" dxfId="446" priority="957" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="478" priority="953" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="445" priority="956" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="477" priority="952" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="444" priority="955" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="476" priority="951" operator="equal">
+    <cfRule type="cellIs" dxfId="443" priority="954" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="475" priority="950" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="442" priority="953" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="474" priority="949" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="441" priority="952" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="473" priority="948" operator="equal">
+    <cfRule type="cellIs" dxfId="440" priority="951" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="472" priority="947" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="439" priority="950" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="471" priority="946" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="438" priority="949" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="470" priority="945" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="948" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="469" priority="944" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="436" priority="947" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="468" priority="943" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="435" priority="946" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="467" priority="942" operator="equal">
+    <cfRule type="cellIs" dxfId="434" priority="945" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="466" priority="941" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="433" priority="944" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="465" priority="940" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="432" priority="943" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="464" priority="939" operator="equal">
+    <cfRule type="cellIs" dxfId="431" priority="942" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="463" priority="938" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="430" priority="941" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="462" priority="937" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="429" priority="940" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="461" priority="936" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="939" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="460" priority="935" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="427" priority="938" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="459" priority="934" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="426" priority="937" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="cellIs" dxfId="458" priority="933" operator="equal">
+    <cfRule type="cellIs" dxfId="425" priority="936" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="457" priority="932" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="424" priority="935" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C41">
-    <cfRule type="containsText" dxfId="456" priority="931" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="423" priority="934" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C41)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="455" priority="825" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="454" priority="824" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="422" priority="828" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="421" priority="827" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="453" priority="823" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="420" priority="826" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="452" priority="855" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="451" priority="854" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="419" priority="858" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="418" priority="857" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="450" priority="853" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="417" priority="856" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="449" priority="852" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="448" priority="851" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="416" priority="855" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="415" priority="854" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="447" priority="850" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="414" priority="853" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="446" priority="849" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="445" priority="848" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="413" priority="852" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="412" priority="851" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="444" priority="847" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="411" priority="850" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="443" priority="846" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="442" priority="845" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="410" priority="849" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="409" priority="848" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="441" priority="844" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="408" priority="847" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="440" priority="843" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="439" priority="842" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="407" priority="846" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="406" priority="845" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="438" priority="841" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="405" priority="844" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="437" priority="840" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="436" priority="839" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="404" priority="843" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="403" priority="842" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="435" priority="838" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="402" priority="841" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="434" priority="837" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="433" priority="836" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="401" priority="840" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="400" priority="839" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="432" priority="835" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="399" priority="838" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="431" priority="834" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="430" priority="833" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="398" priority="837" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="397" priority="836" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="429" priority="832" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="396" priority="835" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="428" priority="831" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="427" priority="830" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="395" priority="834" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="394" priority="833" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="426" priority="829" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="393" priority="832" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="cellIs" dxfId="425" priority="828" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="424" priority="827" operator="containsText" text="En cours">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="cellIs" dxfId="392" priority="831" operator="equal">
+      <formula>"Terminé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="391" priority="830" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="423" priority="826" operator="containsText" text="à faire">
+  <conditionalFormatting sqref="C47:C48">
+    <cfRule type="containsText" dxfId="390" priority="829" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="422" priority="822" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="421" priority="821" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="420" priority="820" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="419" priority="789" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="418" priority="788" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="417" priority="787" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="416" priority="819" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="415" priority="818" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="414" priority="817" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="413" priority="816" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="412" priority="815" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="411" priority="814" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="410" priority="813" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="409" priority="812" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="408" priority="811" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="407" priority="810" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="406" priority="809" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="405" priority="808" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="404" priority="807" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="403" priority="806" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="402" priority="805" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="401" priority="804" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="400" priority="803" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="399" priority="802" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="398" priority="801" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="397" priority="800" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="396" priority="799" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="395" priority="798" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="394" priority="797" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="393" priority="796" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="392" priority="795" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="391" priority="794" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="390" priority="793" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="cellIs" dxfId="389" priority="792" operator="equal">
-      <formula>"Terminé"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="388" priority="791" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
-    <cfRule type="containsText" dxfId="387" priority="790" operator="containsText" text="à faire">
-      <formula>NOT(ISERROR(SEARCH("à faire",C48)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="cellIs" dxfId="386" priority="720" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="723" operator="equal">
       <formula>"Terminé"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45:C46">
-    <cfRule type="containsText" dxfId="385" priority="71